<commit_message>
Remove redundant file and change validation rule as discussed in the review
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
+++ b/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92582\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dataland\datalandClean\dataland-framework-toolbox\inputs\sfdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41B18B2C-A98B-405D-915B-1F27DEAABC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D41511E-883E-424F-973C-B8361E4D5317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
+    <workbookView xWindow="57490" yWindow="-10800" windowWidth="38620" windowHeight="21220" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
     <definedName name="IQ_YTD">3000</definedName>
     <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="295">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -578,9 +578,6 @@
   </si>
   <si>
     <t>Average unadjusted gender pay gap (female to male ratio, only considering gender)</t>
-  </si>
-  <si>
-    <t>Allowed Range: [-100, 100]</t>
   </si>
   <si>
     <t>Female Board Members</t>
@@ -1376,8 +1373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}">
   <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,10 +1382,10 @@
     <col min="1" max="1" width="14.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="34.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="61.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="115.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="87.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="39.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.42578125" style="4" bestFit="1" customWidth="1"/>
@@ -1398,7 +1395,7 @@
     <col min="14" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3092,9 +3089,7 @@
       <c r="G54" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H54" s="5" t="s">
-        <v>170</v>
-      </c>
+      <c r="H54" s="5"/>
       <c r="I54" s="5" t="s">
         <v>80</v>
       </c>
@@ -3113,16 +3108,16 @@
         <v>111</v>
       </c>
       <c r="D55" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E55" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="E55" s="5" t="s">
+      <c r="F55" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55" s="5" t="s">
         <v>172</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G55" s="5" t="s">
-        <v>173</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>72</v>
@@ -3145,16 +3140,16 @@
         <v>111</v>
       </c>
       <c r="D56" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E56" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="E56" s="5" t="s">
-        <v>175</v>
-      </c>
       <c r="F56" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H56" s="5" t="s">
         <v>72</v>
@@ -3177,10 +3172,10 @@
         <v>111</v>
       </c>
       <c r="D57" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="E57" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>177</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>16</v>
@@ -3189,7 +3184,7 @@
         <v>36</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>80</v>
@@ -3209,10 +3204,10 @@
         <v>111</v>
       </c>
       <c r="D58" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="E58" s="5" t="s">
         <v>179</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>180</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>16</v>
@@ -3238,13 +3233,13 @@
         <v>32</v>
       </c>
       <c r="C59" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D59" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="E59" s="5" t="s">
         <v>182</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>183</v>
       </c>
       <c r="F59" s="5"/>
       <c r="G59" s="5" t="s">
@@ -3268,13 +3263,13 @@
         <v>32</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D60" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E60" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>185</v>
       </c>
       <c r="F60" s="5"/>
       <c r="G60" s="5" t="s">
@@ -3298,13 +3293,13 @@
         <v>32</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D61" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>186</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>187</v>
       </c>
       <c r="F61" s="5"/>
       <c r="G61" s="5" t="s">
@@ -3328,16 +3323,16 @@
         <v>32</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D62" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E62" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="E62" s="5" t="s">
+      <c r="F62" s="5" t="s">
         <v>189</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>190</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>68</v>
@@ -3363,10 +3358,10 @@
         <v>69</v>
       </c>
       <c r="D63" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E63" s="5" t="s">
         <v>191</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>192</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>16</v>
@@ -3395,10 +3390,10 @@
         <v>69</v>
       </c>
       <c r="D64" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="E64" s="5" t="s">
         <v>193</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>194</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>16</v>
@@ -3427,10 +3422,10 @@
         <v>69</v>
       </c>
       <c r="D65" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E65" s="5" t="s">
         <v>195</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>196</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>16</v>
@@ -3459,10 +3454,10 @@
         <v>69</v>
       </c>
       <c r="D66" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="E66" s="5" t="s">
         <v>197</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>198</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>16</v>
@@ -3491,10 +3486,10 @@
         <v>69</v>
       </c>
       <c r="D67" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E67" s="5" t="s">
         <v>199</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>200</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>16</v>
@@ -3523,10 +3518,10 @@
         <v>69</v>
       </c>
       <c r="D68" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E68" s="5" t="s">
         <v>201</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>202</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>16</v>
@@ -3555,10 +3550,10 @@
         <v>69</v>
       </c>
       <c r="D69" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="E69" s="5" t="s">
         <v>203</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>204</v>
       </c>
       <c r="F69" s="5" t="s">
         <v>16</v>
@@ -3587,10 +3582,10 @@
         <v>104</v>
       </c>
       <c r="D70" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E70" s="5" t="s">
         <v>205</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>206</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>16</v>
@@ -3602,7 +3597,7 @@
         <v>72</v>
       </c>
       <c r="I70" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J70" s="5" t="s">
         <v>38</v>
@@ -3619,10 +3614,10 @@
         <v>104</v>
       </c>
       <c r="D71" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="E71" s="5" t="s">
         <v>208</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>209</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>16</v>
@@ -3634,7 +3629,7 @@
         <v>72</v>
       </c>
       <c r="I71" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J71" s="5" t="s">
         <v>38</v>
@@ -3651,10 +3646,10 @@
         <v>104</v>
       </c>
       <c r="D72" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E72" s="5" t="s">
         <v>210</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>211</v>
       </c>
       <c r="F72" s="5" t="s">
         <v>16</v>
@@ -3666,7 +3661,7 @@
         <v>72</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J72" s="5" t="s">
         <v>38</v>
@@ -3683,13 +3678,13 @@
         <v>104</v>
       </c>
       <c r="D73" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E73" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="E73" s="5" t="s">
+      <c r="F73" s="5" t="s">
         <v>214</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>215</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>68</v>
@@ -3715,13 +3710,13 @@
         <v>104</v>
       </c>
       <c r="D74" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="E74" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E74" s="5" t="s">
+      <c r="F74" s="5" t="s">
         <v>217</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>218</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>68</v>
@@ -3747,13 +3742,13 @@
         <v>107</v>
       </c>
       <c r="D75" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E75" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E75" s="5" t="s">
+      <c r="F75" s="5" t="s">
         <v>220</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>221</v>
       </c>
       <c r="G75" s="5" t="s">
         <v>68</v>
@@ -3779,13 +3774,13 @@
         <v>107</v>
       </c>
       <c r="D76" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="E76" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="E76" s="5" t="s">
+      <c r="F76" s="5" t="s">
         <v>223</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="G76" s="5" t="s">
         <v>68</v>
@@ -3811,13 +3806,13 @@
         <v>107</v>
       </c>
       <c r="D77" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E77" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="E77" s="5" t="s">
+      <c r="F77" s="5" t="s">
         <v>226</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>227</v>
       </c>
       <c r="G77" s="5" t="s">
         <v>68</v>
@@ -3843,13 +3838,13 @@
         <v>107</v>
       </c>
       <c r="D78" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="E78" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="E78" s="5" t="s">
+      <c r="F78" s="5" t="s">
         <v>229</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>230</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>68</v>
@@ -3875,10 +3870,10 @@
         <v>107</v>
       </c>
       <c r="D79" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E79" s="5" t="s">
         <v>231</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>232</v>
       </c>
       <c r="F79" s="5" t="s">
         <v>16</v>
@@ -3907,13 +3902,13 @@
         <v>107</v>
       </c>
       <c r="D80" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="E80" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="E80" s="5" t="s">
+      <c r="F80" s="5" t="s">
         <v>234</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>235</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>68</v>
@@ -3939,13 +3934,13 @@
         <v>107</v>
       </c>
       <c r="D81" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="E81" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="E81" s="5" t="s">
+      <c r="F81" s="5" t="s">
         <v>237</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>238</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>68</v>
@@ -3971,13 +3966,13 @@
         <v>107</v>
       </c>
       <c r="D82" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="E82" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="E82" s="5" t="s">
+      <c r="F82" s="5" t="s">
         <v>240</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>241</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>68</v>
@@ -4000,16 +3995,16 @@
         <v>110</v>
       </c>
       <c r="C83" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D83" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="E83" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="E83" s="5" t="s">
+      <c r="F83" s="5" t="s">
         <v>244</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>245</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>68</v>
@@ -4035,13 +4030,13 @@
         <v>111</v>
       </c>
       <c r="D84" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E84" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="E84" s="5" t="s">
+      <c r="F84" s="5" t="s">
         <v>247</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>248</v>
       </c>
       <c r="G84" s="5" t="s">
         <v>68</v>
@@ -4067,10 +4062,10 @@
         <v>111</v>
       </c>
       <c r="D85" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="E85" s="5" t="s">
         <v>249</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>250</v>
       </c>
       <c r="F85" s="5" t="s">
         <v>16</v>
@@ -4079,7 +4074,7 @@
         <v>36</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I85" s="5" t="s">
         <v>80</v>
@@ -4099,10 +4094,10 @@
         <v>111</v>
       </c>
       <c r="D86" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="E86" s="5" t="s">
         <v>251</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>252</v>
       </c>
       <c r="F86" s="5" t="s">
         <v>16</v>
@@ -4114,7 +4109,7 @@
         <v>72</v>
       </c>
       <c r="I86" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J86" s="5" t="s">
         <v>38</v>
@@ -4131,13 +4126,13 @@
         <v>111</v>
       </c>
       <c r="D87" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E87" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="E87" s="5" t="s">
+      <c r="F87" s="5" t="s">
         <v>255</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>256</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>68</v>
@@ -4163,13 +4158,13 @@
         <v>111</v>
       </c>
       <c r="D88" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="E88" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="E88" s="5" t="s">
+      <c r="F88" s="5" t="s">
         <v>258</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>259</v>
       </c>
       <c r="G88" s="5" t="s">
         <v>68</v>
@@ -4195,13 +4190,13 @@
         <v>111</v>
       </c>
       <c r="D89" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="E89" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="E89" s="5" t="s">
+      <c r="F89" s="5" t="s">
         <v>261</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>262</v>
       </c>
       <c r="G89" s="5" t="s">
         <v>68</v>
@@ -4227,16 +4222,16 @@
         <v>111</v>
       </c>
       <c r="D90" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E90" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="E90" s="5" t="s">
-        <v>264</v>
-      </c>
       <c r="F90" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H90" s="5" t="s">
         <v>72</v>
@@ -4259,16 +4254,16 @@
         <v>111</v>
       </c>
       <c r="D91" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="E91" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="E91" s="5" t="s">
-        <v>266</v>
-      </c>
       <c r="F91" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H91" s="5" t="s">
         <v>72</v>
@@ -4291,10 +4286,10 @@
         <v>111</v>
       </c>
       <c r="D92" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="E92" s="5" t="s">
         <v>267</v>
-      </c>
-      <c r="E92" s="5" t="s">
-        <v>268</v>
       </c>
       <c r="F92" s="5" t="s">
         <v>16</v>
@@ -4323,10 +4318,10 @@
         <v>111</v>
       </c>
       <c r="D93" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="E93" s="5" t="s">
         <v>269</v>
-      </c>
-      <c r="E93" s="5" t="s">
-        <v>270</v>
       </c>
       <c r="F93" s="5" t="s">
         <v>16</v>
@@ -4352,16 +4347,16 @@
         <v>110</v>
       </c>
       <c r="C94" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D94" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="D94" s="5" t="s">
+      <c r="E94" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="E94" s="5" t="s">
+      <c r="F94" s="5" t="s">
         <v>273</v>
-      </c>
-      <c r="F94" s="5" t="s">
-        <v>274</v>
       </c>
       <c r="G94" s="5" t="s">
         <v>68</v>
@@ -4384,16 +4379,16 @@
         <v>110</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D95" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="E95" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="E95" s="5" t="s">
+      <c r="F95" s="5" t="s">
         <v>276</v>
-      </c>
-      <c r="F95" s="5" t="s">
-        <v>277</v>
       </c>
       <c r="G95" s="5" t="s">
         <v>68</v>
@@ -4416,16 +4411,16 @@
         <v>110</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D96" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="E96" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="E96" s="5" t="s">
+      <c r="F96" s="5" t="s">
         <v>279</v>
-      </c>
-      <c r="F96" s="5" t="s">
-        <v>280</v>
       </c>
       <c r="G96" s="5" t="s">
         <v>68</v>
@@ -4448,16 +4443,16 @@
         <v>110</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D97" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="E97" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="E97" s="5" t="s">
+      <c r="F97" s="5" t="s">
         <v>282</v>
-      </c>
-      <c r="F97" s="5" t="s">
-        <v>283</v>
       </c>
       <c r="G97" s="5" t="s">
         <v>68</v>
@@ -4480,16 +4475,16 @@
         <v>110</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D98" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="E98" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="E98" s="5" t="s">
+      <c r="F98" s="5" t="s">
         <v>285</v>
-      </c>
-      <c r="F98" s="5" t="s">
-        <v>286</v>
       </c>
       <c r="G98" s="5" t="s">
         <v>68</v>
@@ -4512,19 +4507,19 @@
         <v>110</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D99" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="E99" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="E99" s="5" t="s">
-        <v>288</v>
-      </c>
       <c r="F99" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H99" s="5" t="s">
         <v>72</v>
@@ -4544,19 +4539,19 @@
         <v>110</v>
       </c>
       <c r="C100" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D100" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="D100" s="5" t="s">
+      <c r="E100" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="E100" s="5" t="s">
-        <v>291</v>
-      </c>
       <c r="F100" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G100" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H100" s="5" t="s">
         <v>72</v>
@@ -4576,19 +4571,19 @@
         <v>110</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D101" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="E101" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="E101" s="5" t="s">
-        <v>293</v>
-      </c>
       <c r="F101" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H101" s="5" t="s">
         <v>72</v>
@@ -4608,13 +4603,13 @@
         <v>110</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D102" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="E102" s="5" t="s">
         <v>294</v>
-      </c>
-      <c r="E102" s="5" t="s">
-        <v>295</v>
       </c>
       <c r="F102" s="5" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
change fields and extend quality buckets
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
+++ b/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93283\GitRepo\Dataland\dataland-framework-toolbox\inputs\sfdr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dataland\dataland_alternative\dataland-framework-toolbox\inputs\sfdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F68B414-C3FA-4869-A55C-B139C0FA8D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B27F29-E971-4D73-855C-F76120D8A682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
+    <workbookView xWindow="19090" yWindow="-10800" windowWidth="38620" windowHeight="21220" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="2" r:id="rId1"/>
@@ -941,9 +941,6 @@
     <t>Are you involved in violations of OECD Guidelines for Multinational Enterprises for Taxation: In the field of taxation, multinational enterprises should make their contribution to public finances within the framework of applicable law and regulations, in accordance with the tax rules and regulations of the host countries, and should cooperate with the tax authorities.</t>
   </si>
   <si>
-    <t>Yes/No/No Evidence Found</t>
-  </si>
-  <si>
     <t>Do you have policies in place to support/respect human rights and carry out due diligence to ensure that the business activities do not have a negative human rights impact? If yes, please share the relevant documents with us.</t>
   </si>
   <si>
@@ -954,6 +951,9 @@
   </si>
   <si>
     <t>Data Date</t>
+  </si>
+  <si>
+    <t>Yes/No</t>
   </si>
 </sst>
 </file>
@@ -1382,28 +1382,28 @@
   <dimension ref="A1:M103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.90625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="70.54296875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="70.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="79" style="3" customWidth="1"/>
-    <col min="7" max="7" width="39.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1796875" style="3"/>
+    <col min="14" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>288</v>
@@ -1479,7 +1479,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>55</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>14</v>
@@ -1989,7 +1989,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>60</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>14</v>
@@ -2051,7 +2051,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>86</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>14</v>
@@ -2333,7 +2333,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>89</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>14</v>
@@ -2365,7 +2365,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>92</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>14</v>
@@ -2397,7 +2397,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>95</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>14</v>
@@ -2429,7 +2429,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>106</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>14</v>
@@ -2523,7 +2523,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>109</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>14</v>
@@ -2555,7 +2555,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>112</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>14</v>
@@ -2587,7 +2587,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>115</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>14</v>
@@ -2619,7 +2619,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>118</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>14</v>
@@ -2651,7 +2651,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2665,13 +2665,13 @@
         <v>119</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>14</v>
@@ -2683,7 +2683,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>123</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>14</v>
@@ -2715,7 +2715,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>126</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>14</v>
@@ -2747,7 +2747,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>129</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>14</v>
@@ -2779,7 +2779,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>280</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>14</v>
@@ -2811,7 +2811,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>134</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>14</v>
@@ -2843,7 +2843,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>137</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>14</v>
@@ -2875,7 +2875,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>140</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>14</v>
@@ -2907,7 +2907,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>143</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>14</v>
@@ -2939,7 +2939,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>145</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>14</v>
@@ -2971,7 +2971,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>148</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>14</v>
@@ -3003,7 +3003,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>151</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>14</v>
@@ -3035,7 +3035,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>14</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>14</v>
@@ -3257,7 +3257,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>175</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>14</v>
@@ -3379,7 +3379,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -3475,7 +3475,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -3507,7 +3507,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -3571,7 +3571,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -3635,7 +3635,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -3699,7 +3699,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -3719,7 +3719,7 @@
         <v>200</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>14</v>
@@ -3731,7 +3731,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>203</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>14</v>
@@ -3763,7 +3763,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>206</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>14</v>
@@ -3795,7 +3795,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>209</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>14</v>
@@ -3827,7 +3827,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>212</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>14</v>
@@ -3859,7 +3859,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>215</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>14</v>
@@ -3891,7 +3891,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -3943,7 +3943,7 @@
         <v>220</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>14</v>
@@ -3955,7 +3955,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>223</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H82" s="1" t="s">
         <v>14</v>
@@ -3987,7 +3987,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>226</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>14</v>
@@ -4019,7 +4019,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>230</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>14</v>
@@ -4051,7 +4051,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -4071,7 +4071,7 @@
         <v>233</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>14</v>
@@ -4083,7 +4083,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -4097,7 +4097,7 @@
         <v>234</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>14</v>
@@ -4115,7 +4115,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -4147,7 +4147,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -4167,7 +4167,7 @@
         <v>240</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>14</v>
@@ -4179,7 +4179,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>243</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>14</v>
@@ -4211,7 +4211,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>246</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>14</v>
@@ -4243,7 +4243,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -4307,7 +4307,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -4391,7 +4391,7 @@
         <v>257</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>14</v>
@@ -4403,7 +4403,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>260</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>14</v>
@@ -4435,7 +4435,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -4455,7 +4455,7 @@
         <v>263</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>14</v>
@@ -4467,7 +4467,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -4487,7 +4487,7 @@
         <v>266</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H98" s="1" t="s">
         <v>14</v>
@@ -4499,7 +4499,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -4519,7 +4519,7 @@
         <v>269</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>14</v>
@@ -4531,7 +4531,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -4563,7 +4563,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>102</v>
       </c>

</xml_diff>

<commit_message>
Dala 4606 adapt quality buckets (#639)
- quality bucket "Incomplete" has been replaced by "NoDataFound"
- "NoEvidenceFound" has been removed as value for Yes-No-questions
- migrations for existing data
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
+++ b/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93283\GitRepo\Dataland\dataland-framework-toolbox\inputs\sfdr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dataland\dataland_alternative\dataland-framework-toolbox\inputs\sfdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F68B414-C3FA-4869-A55C-B139C0FA8D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B27F29-E971-4D73-855C-F76120D8A682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
+    <workbookView xWindow="19090" yWindow="-10800" windowWidth="38620" windowHeight="21220" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="2" r:id="rId1"/>
@@ -941,9 +941,6 @@
     <t>Are you involved in violations of OECD Guidelines for Multinational Enterprises for Taxation: In the field of taxation, multinational enterprises should make their contribution to public finances within the framework of applicable law and regulations, in accordance with the tax rules and regulations of the host countries, and should cooperate with the tax authorities.</t>
   </si>
   <si>
-    <t>Yes/No/No Evidence Found</t>
-  </si>
-  <si>
     <t>Do you have policies in place to support/respect human rights and carry out due diligence to ensure that the business activities do not have a negative human rights impact? If yes, please share the relevant documents with us.</t>
   </si>
   <si>
@@ -954,6 +951,9 @@
   </si>
   <si>
     <t>Data Date</t>
+  </si>
+  <si>
+    <t>Yes/No</t>
   </si>
 </sst>
 </file>
@@ -1382,28 +1382,28 @@
   <dimension ref="A1:M103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.90625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="70.54296875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="70.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="79" style="3" customWidth="1"/>
-    <col min="7" max="7" width="39.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1796875" style="3"/>
+    <col min="14" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>288</v>
@@ -1479,7 +1479,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>55</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>14</v>
@@ -1989,7 +1989,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>60</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>14</v>
@@ -2051,7 +2051,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>86</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>14</v>
@@ -2333,7 +2333,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>89</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>14</v>
@@ -2365,7 +2365,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>92</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>14</v>
@@ -2397,7 +2397,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>95</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>14</v>
@@ -2429,7 +2429,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>106</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>14</v>
@@ -2523,7 +2523,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>109</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>14</v>
@@ -2555,7 +2555,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>112</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>14</v>
@@ -2587,7 +2587,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>115</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>14</v>
@@ -2619,7 +2619,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>118</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>14</v>
@@ -2651,7 +2651,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2665,13 +2665,13 @@
         <v>119</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>14</v>
@@ -2683,7 +2683,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>123</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>14</v>
@@ -2715,7 +2715,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>126</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>14</v>
@@ -2747,7 +2747,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>129</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>14</v>
@@ -2779,7 +2779,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>280</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>14</v>
@@ -2811,7 +2811,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>134</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>14</v>
@@ -2843,7 +2843,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>137</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>14</v>
@@ -2875,7 +2875,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>140</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>14</v>
@@ -2907,7 +2907,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>143</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>14</v>
@@ -2939,7 +2939,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>145</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>14</v>
@@ -2971,7 +2971,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>148</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>14</v>
@@ -3003,7 +3003,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>151</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>14</v>
@@ -3035,7 +3035,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>14</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>14</v>
@@ -3257,7 +3257,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>175</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>14</v>
@@ -3379,7 +3379,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -3475,7 +3475,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -3507,7 +3507,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -3571,7 +3571,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -3635,7 +3635,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -3699,7 +3699,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -3719,7 +3719,7 @@
         <v>200</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>14</v>
@@ -3731,7 +3731,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>203</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>14</v>
@@ -3763,7 +3763,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>206</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>14</v>
@@ -3795,7 +3795,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>209</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>14</v>
@@ -3827,7 +3827,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>212</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>14</v>
@@ -3859,7 +3859,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>215</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>14</v>
@@ -3891,7 +3891,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -3943,7 +3943,7 @@
         <v>220</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>14</v>
@@ -3955,7 +3955,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>223</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H82" s="1" t="s">
         <v>14</v>
@@ -3987,7 +3987,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>226</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>14</v>
@@ -4019,7 +4019,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>230</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>14</v>
@@ -4051,7 +4051,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -4071,7 +4071,7 @@
         <v>233</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>14</v>
@@ -4083,7 +4083,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -4097,7 +4097,7 @@
         <v>234</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>14</v>
@@ -4115,7 +4115,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -4147,7 +4147,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -4167,7 +4167,7 @@
         <v>240</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>14</v>
@@ -4179,7 +4179,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>243</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>14</v>
@@ -4211,7 +4211,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>246</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>14</v>
@@ -4243,7 +4243,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -4307,7 +4307,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -4391,7 +4391,7 @@
         <v>257</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>14</v>
@@ -4403,7 +4403,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>260</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>14</v>
@@ -4435,7 +4435,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -4455,7 +4455,7 @@
         <v>263</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>14</v>
@@ -4467,7 +4467,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -4487,7 +4487,7 @@
         <v>266</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H98" s="1" t="s">
         <v>14</v>
@@ -4499,7 +4499,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -4519,7 +4519,7 @@
         <v>269</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>14</v>
@@ -4531,7 +4531,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -4563,7 +4563,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>102</v>
       </c>

</xml_diff>

<commit_message>
update sfdr excel with new fields and run toolbox
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
+++ b/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dataland\dataland_alternative\dataland-framework-toolbox\inputs\sfdr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93447\Documents\Dataland\dataland-framework-toolbox\inputs\sfdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B27F29-E971-4D73-855C-F76120D8A682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1735BEFA-D3C6-4FB5-9F3A-A832C2752945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-10800" windowWidth="38620" windowHeight="21220" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
+    <workbookView xWindow="1665" yWindow="1590" windowWidth="26040" windowHeight="13582" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$M$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$M$112</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
     <definedName name="IQ_CY">10000</definedName>
@@ -48,7 +48,7 @@
     <definedName name="IQ_YTD">3000</definedName>
     <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="313">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -545,24 +545,9 @@
     <t>Average unadjusted gender pay gap (female to male ratio, only considering gender)</t>
   </si>
   <si>
-    <t>Female Board Members</t>
-  </si>
-  <si>
-    <t>Number of females on the board, i.e. means the administrative, management or supervisory body of a company</t>
-  </si>
-  <si>
     <t>Integer</t>
   </si>
   <si>
-    <t>Male Board Members</t>
-  </si>
-  <si>
-    <t>Number of males on the board, i.e. means the administrative, management or supervisory body of a company.</t>
-  </si>
-  <si>
-    <t>Board gender diversity</t>
-  </si>
-  <si>
     <t>Allowed Range: [0, 100]</t>
   </si>
   <si>
@@ -908,9 +893,6 @@
     <t>Amount of fines for violations of anti-corruption and anti-bribery laws</t>
   </si>
   <si>
-    <t>Percentage of female board members among all board members</t>
-  </si>
-  <si>
     <t>The company is ISO 14001 certified</t>
   </si>
   <si>
@@ -954,6 +936,78 @@
   </si>
   <si>
     <t>Yes/No</t>
+  </si>
+  <si>
+    <t>Female Board Members - Supervisory Board</t>
+  </si>
+  <si>
+    <t>Number of females on the supervisory board, i.e. means the administrative, management or supervisory body of a company</t>
+  </si>
+  <si>
+    <t>Female Board Members - Board of Directors</t>
+  </si>
+  <si>
+    <t>Number of females on the board of directors of the company</t>
+  </si>
+  <si>
+    <t>Male Board Members - Supervisory Board</t>
+  </si>
+  <si>
+    <t>Number of males on the supervisory board, i.e. means the administrative, management or supervisory body of a company</t>
+  </si>
+  <si>
+    <t>Male Board Members - Board of Directors</t>
+  </si>
+  <si>
+    <t>Number of males on the board of directors of the company</t>
+  </si>
+  <si>
+    <t>Board gender diversity - Supervisory Board</t>
+  </si>
+  <si>
+    <t>Percentage of female board members among all supervisory board members</t>
+  </si>
+  <si>
+    <t>Board gender diversity - Board of Directors</t>
+  </si>
+  <si>
+    <t>Percentage of female board members among all board of directors members</t>
+  </si>
+  <si>
+    <t>Scope 3 upstream GHG emissions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scope 3 downstream GHG emissions </t>
+  </si>
+  <si>
+    <t>GHG intensity - scope 1</t>
+  </si>
+  <si>
+    <t>GHG intensity - scope 2</t>
+  </si>
+  <si>
+    <t>GHG intensity - scope 3</t>
+  </si>
+  <si>
+    <t>GHG intensity - scope 4</t>
+  </si>
+  <si>
+    <t>Tonnes of Scope 1 GHG emissions / million of the revenue (in the same currency as the total revenue)</t>
+  </si>
+  <si>
+    <t>Tonnes of Scope 2 GHG emissions / million of the revenue (in the same currency as the total revenue)</t>
+  </si>
+  <si>
+    <t>Tonnes of Scope 3 GHG emissions / million of the revenue (in the same currency as the total revenue)</t>
+  </si>
+  <si>
+    <t>Tonnes of Scope 4 GHG emissions / million of the revenue (in the same currency as the total revenue)</t>
+  </si>
+  <si>
+    <t>Indirect (gross) carbon emissions from activities related to the production and distribution of goods and services purchased by the reporting company.</t>
+  </si>
+  <si>
+    <t>Indirect (gross) carbon emissions that occur as a result of the use or disposal of the reporting company’s sold products and services.</t>
   </si>
 </sst>
 </file>
@@ -1379,31 +1433,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}">
-  <dimension ref="A1:M103"/>
+  <dimension ref="A1:M112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.265625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="70.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="29.86328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.86328125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="61.6640625" style="3" customWidth="1"/>
     <col min="6" max="6" width="79" style="3" customWidth="1"/>
-    <col min="7" max="7" width="39.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.86328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.265625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="3"/>
+    <col min="14" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1444,7 +1498,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1455,10 +1509,10 @@
         <v>13</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>14</v>
@@ -1479,7 +1533,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1514,7 +1568,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1549,7 +1603,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1579,7 +1633,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1609,7 +1663,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1637,7 +1691,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1667,7 +1721,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1697,7 +1751,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1727,7 +1781,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1757,7 +1811,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1787,7 +1841,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1817,7 +1871,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1828,14 +1882,12 @@
         <v>28</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
         <v>31</v>
       </c>
@@ -1847,7 +1899,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1857,11 +1909,11 @@
       <c r="C15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>286</v>
+      <c r="D15" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>312</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
@@ -1875,7 +1927,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1885,13 +1937,15 @@
       <c r="C16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>285</v>
+      <c r="D16" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="F16" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G16" s="1" t="s">
         <v>31</v>
       </c>
@@ -1903,7 +1957,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1913,25 +1967,25 @@
       <c r="C17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>51</v>
+      <c r="D17" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>280</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1941,25 +1995,25 @@
       <c r="C18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>54</v>
+      <c r="D18" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1970,26 +2024,24 @@
         <v>28</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2000,26 +2052,24 @@
         <v>28</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2030,28 +2080,26 @@
         <v>28</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>285</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2059,29 +2107,29 @@
         <v>27</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2089,29 +2137,27 @@
         <v>27</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>67</v>
+        <v>303</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>307</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="H23" s="1"/>
       <c r="I23" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2119,31 +2165,27 @@
         <v>27</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="H24" s="1"/>
       <c r="I24" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2151,31 +2193,27 @@
         <v>27</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="H25" s="1"/>
       <c r="I25" s="1" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2183,31 +2221,27 @@
         <v>27</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="H26" s="1"/>
       <c r="I26" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2215,31 +2249,29 @@
         <v>27</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="I27" s="1"/>
       <c r="J27" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2250,28 +2282,26 @@
         <v>61</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>79</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2282,10 +2312,10 @@
         <v>61</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
@@ -2301,7 +2331,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2309,31 +2339,31 @@
         <v>27</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>86</v>
+        <v>14</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2341,31 +2371,31 @@
         <v>27</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2373,31 +2403,31 @@
         <v>27</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2405,31 +2435,31 @@
         <v>27</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>95</v>
+        <v>14</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2437,31 +2467,31 @@
         <v>27</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2469,13 +2499,13 @@
         <v>27</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1" t="s">
@@ -2485,33 +2515,33 @@
         <v>64</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>14</v>
@@ -2523,27 +2553,27 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>14</v>
@@ -2555,27 +2585,27 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>14</v>
@@ -2587,27 +2617,27 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>14</v>
@@ -2619,71 +2649,69 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>118</v>
+        <v>14</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>120</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="F41" s="1"/>
       <c r="G41" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2694,16 +2722,16 @@
         <v>103</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>14</v>
@@ -2715,7 +2743,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2726,16 +2754,16 @@
         <v>103</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>14</v>
@@ -2747,7 +2775,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2758,16 +2786,16 @@
         <v>103</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>14</v>
@@ -2779,7 +2807,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2790,16 +2818,16 @@
         <v>103</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>280</v>
+        <v>115</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>14</v>
@@ -2811,7 +2839,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2822,16 +2850,16 @@
         <v>103</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>14</v>
@@ -2843,7 +2871,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2854,16 +2882,16 @@
         <v>103</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>136</v>
+        <v>284</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>14</v>
@@ -2875,7 +2903,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2886,16 +2914,16 @@
         <v>103</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>14</v>
@@ -2907,7 +2935,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2918,16 +2946,16 @@
         <v>103</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>14</v>
@@ -2939,7 +2967,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2950,16 +2978,16 @@
         <v>103</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>289</v>
+        <v>127</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>14</v>
@@ -2971,7 +2999,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2982,16 +3010,16 @@
         <v>103</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>148</v>
+        <v>274</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>14</v>
@@ -3003,7 +3031,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3014,16 +3042,16 @@
         <v>103</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>14</v>
@@ -3035,7 +3063,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3046,19 +3074,19 @@
         <v>103</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>14</v>
+        <v>137</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>52</v>
+        <v>288</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>14</v>
@@ -3067,7 +3095,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3078,19 +3106,19 @@
         <v>103</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>52</v>
+        <v>288</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>14</v>
@@ -3099,7 +3127,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3110,26 +3138,28 @@
         <v>103</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H55" s="1"/>
+        <v>288</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="I55" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3140,19 +3170,19 @@
         <v>103</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>159</v>
+        <v>144</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>283</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>14</v>
+        <v>145</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>160</v>
+        <v>288</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>14</v>
@@ -3161,7 +3191,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3172,19 +3202,19 @@
         <v>103</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>14</v>
+        <v>148</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>160</v>
+        <v>288</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>14</v>
@@ -3193,7 +3223,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3204,28 +3234,28 @@
         <v>103</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>279</v>
+        <v>150</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>14</v>
+        <v>151</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>164</v>
+        <v>14</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3236,19 +3266,19 @@
         <v>103</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>294</v>
+        <v>52</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>14</v>
@@ -3257,289 +3287,273 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>167</v>
+        <v>103</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="F60" s="1"/>
+        <v>155</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G60" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>64</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J60" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>167</v>
+        <v>103</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="F61" s="1"/>
+        <v>157</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G61" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H61" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="H61" s="1"/>
       <c r="I61" s="1" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>167</v>
+        <v>103</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>171</v>
+        <v>289</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>172</v>
+        <v>290</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1" t="s">
-        <v>31</v>
+        <v>158</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I62" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="I62" s="1"/>
       <c r="J62" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63" s="1">
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>167</v>
+        <v>103</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>173</v>
+        <v>291</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>175</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="F63" s="1"/>
       <c r="G63" s="1" t="s">
-        <v>294</v>
+        <v>158</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="I63" s="1"/>
       <c r="J63" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64" s="1">
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>61</v>
+        <v>103</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>176</v>
+        <v>293</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>294</v>
+      </c>
+      <c r="F64" s="1"/>
       <c r="G64" s="1" t="s">
-        <v>31</v>
+        <v>158</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I64" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="I64" s="1"/>
       <c r="J64" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65" s="1">
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>61</v>
+        <v>103</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>178</v>
+        <v>295</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
-        <v>31</v>
+        <v>158</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I65" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="I65" s="1"/>
       <c r="J65" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66" s="1">
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>61</v>
+        <v>103</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>180</v>
+        <v>297</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="J66" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A67" s="1">
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>61</v>
+        <v>103</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>182</v>
+        <v>299</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="J67" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A68" s="1">
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>61</v>
+        <v>103</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="J68" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -3547,17 +3561,15 @@
         <v>27</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>186</v>
+        <v>163</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
         <v>31</v>
       </c>
@@ -3565,13 +3577,13 @@
         <v>64</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="J69" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -3579,17 +3591,15 @@
         <v>27</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
         <v>31</v>
       </c>
@@ -3597,13 +3607,13 @@
         <v>64</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -3611,17 +3621,15 @@
         <v>27</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>96</v>
+        <v>162</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="F71" s="1"/>
       <c r="G71" s="1" t="s">
         <v>31</v>
       </c>
@@ -3629,13 +3637,13 @@
         <v>64</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>192</v>
+        <v>32</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -3643,31 +3651,31 @@
         <v>27</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>96</v>
+        <v>162</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>193</v>
+        <v>168</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>194</v>
+        <v>169</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>14</v>
+        <v>170</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>192</v>
+        <v>14</v>
       </c>
       <c r="J72" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -3675,13 +3683,13 @@
         <v>27</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>14</v>
@@ -3693,13 +3701,13 @@
         <v>64</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>197</v>
+        <v>65</v>
       </c>
       <c r="J73" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -3707,31 +3715,31 @@
         <v>27</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>198</v>
+        <v>173</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>199</v>
+        <v>174</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>200</v>
+        <v>14</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J74" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -3739,31 +3747,31 @@
         <v>27</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>202</v>
+        <v>176</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>203</v>
+        <v>14</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J75" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -3771,31 +3779,31 @@
         <v>27</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>204</v>
+        <v>177</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>205</v>
+        <v>178</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>206</v>
+        <v>14</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J76" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -3803,31 +3811,31 @@
         <v>27</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>207</v>
+        <v>179</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>208</v>
+        <v>180</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>209</v>
+        <v>14</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J77" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -3835,31 +3843,31 @@
         <v>27</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>210</v>
+        <v>181</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>212</v>
+        <v>14</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J78" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -3867,31 +3875,31 @@
         <v>27</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>215</v>
+        <v>14</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J79" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -3899,13 +3907,13 @@
         <v>27</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>216</v>
+        <v>185</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>217</v>
+        <v>186</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>14</v>
@@ -3917,13 +3925,13 @@
         <v>64</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>32</v>
+        <v>187</v>
       </c>
       <c r="J80" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -3931,31 +3939,31 @@
         <v>27</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>220</v>
+        <v>14</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>14</v>
+        <v>187</v>
       </c>
       <c r="J81" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -3963,31 +3971,31 @@
         <v>27</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>221</v>
+        <v>190</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>222</v>
+        <v>191</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>223</v>
+        <v>14</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>14</v>
+        <v>192</v>
       </c>
       <c r="J82" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -3995,19 +4003,19 @@
         <v>27</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>224</v>
+        <v>193</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>14</v>
@@ -4019,27 +4027,27 @@
         <v>33</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A84" s="1">
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>227</v>
+        <v>96</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>14</v>
@@ -4051,27 +4059,27 @@
         <v>33</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A85" s="1">
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>14</v>
@@ -4083,91 +4091,91 @@
         <v>33</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A86" s="1">
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>292</v>
+        <v>203</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>14</v>
+        <v>204</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>164</v>
+        <v>14</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="J86" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A87" s="1">
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>236</v>
+        <v>206</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>237</v>
+        <v>14</v>
       </c>
       <c r="J87" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A88" s="1">
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>238</v>
+        <v>208</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>239</v>
+        <v>209</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>240</v>
+        <v>210</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>14</v>
@@ -4179,59 +4187,59 @@
         <v>33</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A89" s="1">
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>241</v>
+        <v>211</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>242</v>
+        <v>212</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>243</v>
+        <v>14</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J89" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A90" s="1">
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>244</v>
+        <v>213</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>245</v>
+        <v>214</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>14</v>
@@ -4243,30 +4251,30 @@
         <v>33</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A91" s="1">
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>14</v>
+        <v>218</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>160</v>
+        <v>288</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I91" s="1" t="s">
         <v>14</v>
@@ -4275,30 +4283,30 @@
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A92" s="1">
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>249</v>
+        <v>219</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>14</v>
+        <v>221</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>160</v>
+        <v>288</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I92" s="1" t="s">
         <v>14</v>
@@ -4307,7 +4315,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -4315,22 +4323,22 @@
         <v>102</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>103</v>
+        <v>222</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>252</v>
+        <v>224</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>14</v>
+        <v>225</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I93" s="1" t="s">
         <v>14</v>
@@ -4339,7 +4347,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -4350,28 +4358,28 @@
         <v>103</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>253</v>
+        <v>226</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>254</v>
+        <v>227</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>14</v>
+        <v>228</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="J94" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -4379,31 +4387,31 @@
         <v>102</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>256</v>
+        <v>103</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>229</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>257</v>
+        <v>14</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>14</v>
+        <v>159</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="J95" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -4411,31 +4419,31 @@
         <v>102</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>258</v>
+        <v>103</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>260</v>
+        <v>14</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>14</v>
+        <v>232</v>
       </c>
       <c r="J96" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -4443,19 +4451,19 @@
         <v>102</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>255</v>
+        <v>103</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>261</v>
+        <v>233</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>262</v>
+        <v>234</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>14</v>
@@ -4467,7 +4475,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -4475,19 +4483,19 @@
         <v>102</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>255</v>
+        <v>103</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>265</v>
+        <v>237</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>266</v>
+        <v>238</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H98" s="1" t="s">
         <v>14</v>
@@ -4499,7 +4507,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -4507,19 +4515,19 @@
         <v>102</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>255</v>
+        <v>103</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>267</v>
+        <v>239</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>268</v>
+        <v>240</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>269</v>
+        <v>241</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>14</v>
@@ -4531,7 +4539,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -4539,19 +4547,19 @@
         <v>102</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>255</v>
+        <v>103</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>270</v>
+        <v>242</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>271</v>
+        <v>243</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>64</v>
@@ -4563,7 +4571,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -4571,19 +4579,19 @@
         <v>102</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>272</v>
+        <v>103</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>273</v>
+        <v>244</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>274</v>
+        <v>245</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>64</v>
@@ -4595,7 +4603,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -4603,19 +4611,19 @@
         <v>102</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>272</v>
+        <v>103</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>275</v>
+        <v>246</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>276</v>
+        <v>247</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>160</v>
+        <v>31</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>64</v>
@@ -4627,7 +4635,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -4635,32 +4643,320 @@
         <v>102</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>272</v>
+        <v>103</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>277</v>
+        <v>248</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>278</v>
+        <v>249</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>64</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="J103" s="1" t="s">
         <v>33</v>
       </c>
     </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A104" s="1">
+        <v>103</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I104" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J104" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A105" s="1">
+        <v>104</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I105" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J105" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A106" s="1">
+        <v>105</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I106" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J106" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A107" s="1">
+        <v>106</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I107" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J107" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A108" s="1">
+        <v>107</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I108" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A109" s="1">
+        <v>108</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J109" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A110" s="1">
+        <v>109</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I110" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J110" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A111" s="1">
+        <v>110</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I111" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J111" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A112" s="1">
+        <v>111</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I112" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J112" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M103" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}"/>
+  <autoFilter ref="A1:M112" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
DALA 4684: Add 7 simple fields to SfDR data set - Deka RfP (#645)
Update SFDR framework

---------

Co-authored-by: SiegfriedSobkowiak <siegfried.sobkowiak@d-fine.de>
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
+++ b/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dataland\dataland_alternative\dataland-framework-toolbox\inputs\sfdr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93447\Documents\Dataland\dataland-framework-toolbox\inputs\sfdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B27F29-E971-4D73-855C-F76120D8A682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1735BEFA-D3C6-4FB5-9F3A-A832C2752945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-10800" windowWidth="38620" windowHeight="21220" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
+    <workbookView xWindow="1665" yWindow="1590" windowWidth="26040" windowHeight="13582" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$M$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$M$112</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
     <definedName name="IQ_CY">10000</definedName>
@@ -48,7 +48,7 @@
     <definedName name="IQ_YTD">3000</definedName>
     <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="313">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -545,24 +545,9 @@
     <t>Average unadjusted gender pay gap (female to male ratio, only considering gender)</t>
   </si>
   <si>
-    <t>Female Board Members</t>
-  </si>
-  <si>
-    <t>Number of females on the board, i.e. means the administrative, management or supervisory body of a company</t>
-  </si>
-  <si>
     <t>Integer</t>
   </si>
   <si>
-    <t>Male Board Members</t>
-  </si>
-  <si>
-    <t>Number of males on the board, i.e. means the administrative, management or supervisory body of a company.</t>
-  </si>
-  <si>
-    <t>Board gender diversity</t>
-  </si>
-  <si>
     <t>Allowed Range: [0, 100]</t>
   </si>
   <si>
@@ -908,9 +893,6 @@
     <t>Amount of fines for violations of anti-corruption and anti-bribery laws</t>
   </si>
   <si>
-    <t>Percentage of female board members among all board members</t>
-  </si>
-  <si>
     <t>The company is ISO 14001 certified</t>
   </si>
   <si>
@@ -954,6 +936,78 @@
   </si>
   <si>
     <t>Yes/No</t>
+  </si>
+  <si>
+    <t>Female Board Members - Supervisory Board</t>
+  </si>
+  <si>
+    <t>Number of females on the supervisory board, i.e. means the administrative, management or supervisory body of a company</t>
+  </si>
+  <si>
+    <t>Female Board Members - Board of Directors</t>
+  </si>
+  <si>
+    <t>Number of females on the board of directors of the company</t>
+  </si>
+  <si>
+    <t>Male Board Members - Supervisory Board</t>
+  </si>
+  <si>
+    <t>Number of males on the supervisory board, i.e. means the administrative, management or supervisory body of a company</t>
+  </si>
+  <si>
+    <t>Male Board Members - Board of Directors</t>
+  </si>
+  <si>
+    <t>Number of males on the board of directors of the company</t>
+  </si>
+  <si>
+    <t>Board gender diversity - Supervisory Board</t>
+  </si>
+  <si>
+    <t>Percentage of female board members among all supervisory board members</t>
+  </si>
+  <si>
+    <t>Board gender diversity - Board of Directors</t>
+  </si>
+  <si>
+    <t>Percentage of female board members among all board of directors members</t>
+  </si>
+  <si>
+    <t>Scope 3 upstream GHG emissions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scope 3 downstream GHG emissions </t>
+  </si>
+  <si>
+    <t>GHG intensity - scope 1</t>
+  </si>
+  <si>
+    <t>GHG intensity - scope 2</t>
+  </si>
+  <si>
+    <t>GHG intensity - scope 3</t>
+  </si>
+  <si>
+    <t>GHG intensity - scope 4</t>
+  </si>
+  <si>
+    <t>Tonnes of Scope 1 GHG emissions / million of the revenue (in the same currency as the total revenue)</t>
+  </si>
+  <si>
+    <t>Tonnes of Scope 2 GHG emissions / million of the revenue (in the same currency as the total revenue)</t>
+  </si>
+  <si>
+    <t>Tonnes of Scope 3 GHG emissions / million of the revenue (in the same currency as the total revenue)</t>
+  </si>
+  <si>
+    <t>Tonnes of Scope 4 GHG emissions / million of the revenue (in the same currency as the total revenue)</t>
+  </si>
+  <si>
+    <t>Indirect (gross) carbon emissions from activities related to the production and distribution of goods and services purchased by the reporting company.</t>
+  </si>
+  <si>
+    <t>Indirect (gross) carbon emissions that occur as a result of the use or disposal of the reporting company’s sold products and services.</t>
   </si>
 </sst>
 </file>
@@ -1379,31 +1433,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}">
-  <dimension ref="A1:M103"/>
+  <dimension ref="A1:M112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.265625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="70.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="29.86328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.86328125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="61.6640625" style="3" customWidth="1"/>
     <col min="6" max="6" width="79" style="3" customWidth="1"/>
-    <col min="7" max="7" width="39.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.86328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.265625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="3"/>
+    <col min="14" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1444,7 +1498,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1455,10 +1509,10 @@
         <v>13</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>14</v>
@@ -1479,7 +1533,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1514,7 +1568,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1549,7 +1603,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1579,7 +1633,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1609,7 +1663,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1637,7 +1691,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1667,7 +1721,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1697,7 +1751,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1727,7 +1781,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1757,7 +1811,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1787,7 +1841,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1817,7 +1871,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1828,14 +1882,12 @@
         <v>28</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
         <v>31</v>
       </c>
@@ -1847,7 +1899,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1857,11 +1909,11 @@
       <c r="C15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>286</v>
+      <c r="D15" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>312</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
@@ -1875,7 +1927,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1885,13 +1937,15 @@
       <c r="C16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>285</v>
+      <c r="D16" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="F16" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G16" s="1" t="s">
         <v>31</v>
       </c>
@@ -1903,7 +1957,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1913,25 +1967,25 @@
       <c r="C17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>51</v>
+      <c r="D17" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>280</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1941,25 +1995,25 @@
       <c r="C18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>54</v>
+      <c r="D18" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1970,26 +2024,24 @@
         <v>28</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2000,26 +2052,24 @@
         <v>28</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2030,28 +2080,26 @@
         <v>28</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>285</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2059,29 +2107,29 @@
         <v>27</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2089,29 +2137,27 @@
         <v>27</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>67</v>
+        <v>303</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>307</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="H23" s="1"/>
       <c r="I23" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2119,31 +2165,27 @@
         <v>27</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="H24" s="1"/>
       <c r="I24" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2151,31 +2193,27 @@
         <v>27</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="H25" s="1"/>
       <c r="I25" s="1" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2183,31 +2221,27 @@
         <v>27</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="H26" s="1"/>
       <c r="I26" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2215,31 +2249,29 @@
         <v>27</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="I27" s="1"/>
       <c r="J27" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2250,28 +2282,26 @@
         <v>61</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>79</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2282,10 +2312,10 @@
         <v>61</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
@@ -2301,7 +2331,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2309,31 +2339,31 @@
         <v>27</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>86</v>
+        <v>14</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2341,31 +2371,31 @@
         <v>27</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2373,31 +2403,31 @@
         <v>27</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2405,31 +2435,31 @@
         <v>27</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>95</v>
+        <v>14</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2437,31 +2467,31 @@
         <v>27</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2469,13 +2499,13 @@
         <v>27</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1" t="s">
@@ -2485,33 +2515,33 @@
         <v>64</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>14</v>
@@ -2523,27 +2553,27 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>14</v>
@@ -2555,27 +2585,27 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>14</v>
@@ -2587,27 +2617,27 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>14</v>
@@ -2619,71 +2649,69 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>118</v>
+        <v>14</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>120</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="F41" s="1"/>
       <c r="G41" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2694,16 +2722,16 @@
         <v>103</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>14</v>
@@ -2715,7 +2743,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2726,16 +2754,16 @@
         <v>103</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>14</v>
@@ -2747,7 +2775,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2758,16 +2786,16 @@
         <v>103</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>14</v>
@@ -2779,7 +2807,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2790,16 +2818,16 @@
         <v>103</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>280</v>
+        <v>115</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>14</v>
@@ -2811,7 +2839,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2822,16 +2850,16 @@
         <v>103</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>14</v>
@@ -2843,7 +2871,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2854,16 +2882,16 @@
         <v>103</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>136</v>
+        <v>284</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>14</v>
@@ -2875,7 +2903,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2886,16 +2914,16 @@
         <v>103</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>14</v>
@@ -2907,7 +2935,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2918,16 +2946,16 @@
         <v>103</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>14</v>
@@ -2939,7 +2967,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2950,16 +2978,16 @@
         <v>103</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>289</v>
+        <v>127</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>14</v>
@@ -2971,7 +2999,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2982,16 +3010,16 @@
         <v>103</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>148</v>
+        <v>274</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>14</v>
@@ -3003,7 +3031,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3014,16 +3042,16 @@
         <v>103</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>14</v>
@@ -3035,7 +3063,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3046,19 +3074,19 @@
         <v>103</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>14</v>
+        <v>137</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>52</v>
+        <v>288</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>14</v>
@@ -3067,7 +3095,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3078,19 +3106,19 @@
         <v>103</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>52</v>
+        <v>288</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>14</v>
@@ -3099,7 +3127,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3110,26 +3138,28 @@
         <v>103</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H55" s="1"/>
+        <v>288</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="I55" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3140,19 +3170,19 @@
         <v>103</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>159</v>
+        <v>144</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>283</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>14</v>
+        <v>145</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>160</v>
+        <v>288</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>14</v>
@@ -3161,7 +3191,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3172,19 +3202,19 @@
         <v>103</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>14</v>
+        <v>148</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>160</v>
+        <v>288</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>14</v>
@@ -3193,7 +3223,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3204,28 +3234,28 @@
         <v>103</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>279</v>
+        <v>150</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>14</v>
+        <v>151</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>164</v>
+        <v>14</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3236,19 +3266,19 @@
         <v>103</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>294</v>
+        <v>52</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>14</v>
@@ -3257,289 +3287,273 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>167</v>
+        <v>103</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="F60" s="1"/>
+        <v>155</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G60" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>64</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J60" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>167</v>
+        <v>103</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="F61" s="1"/>
+        <v>157</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G61" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H61" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="H61" s="1"/>
       <c r="I61" s="1" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>167</v>
+        <v>103</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>171</v>
+        <v>289</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>172</v>
+        <v>290</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1" t="s">
-        <v>31</v>
+        <v>158</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I62" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="I62" s="1"/>
       <c r="J62" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63" s="1">
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>167</v>
+        <v>103</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>173</v>
+        <v>291</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>175</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="F63" s="1"/>
       <c r="G63" s="1" t="s">
-        <v>294</v>
+        <v>158</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="I63" s="1"/>
       <c r="J63" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64" s="1">
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>61</v>
+        <v>103</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>176</v>
+        <v>293</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>294</v>
+      </c>
+      <c r="F64" s="1"/>
       <c r="G64" s="1" t="s">
-        <v>31</v>
+        <v>158</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I64" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="I64" s="1"/>
       <c r="J64" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65" s="1">
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>61</v>
+        <v>103</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>178</v>
+        <v>295</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
-        <v>31</v>
+        <v>158</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I65" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="I65" s="1"/>
       <c r="J65" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66" s="1">
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>61</v>
+        <v>103</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>180</v>
+        <v>297</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="J66" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A67" s="1">
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>61</v>
+        <v>103</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>182</v>
+        <v>299</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="J67" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A68" s="1">
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>61</v>
+        <v>103</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="J68" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -3547,17 +3561,15 @@
         <v>27</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>186</v>
+        <v>163</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
         <v>31</v>
       </c>
@@ -3565,13 +3577,13 @@
         <v>64</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="J69" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -3579,17 +3591,15 @@
         <v>27</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
         <v>31</v>
       </c>
@@ -3597,13 +3607,13 @@
         <v>64</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -3611,17 +3621,15 @@
         <v>27</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>96</v>
+        <v>162</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="F71" s="1"/>
       <c r="G71" s="1" t="s">
         <v>31</v>
       </c>
@@ -3629,13 +3637,13 @@
         <v>64</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>192</v>
+        <v>32</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -3643,31 +3651,31 @@
         <v>27</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>96</v>
+        <v>162</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>193</v>
+        <v>168</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>194</v>
+        <v>169</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>14</v>
+        <v>170</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>192</v>
+        <v>14</v>
       </c>
       <c r="J72" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -3675,13 +3683,13 @@
         <v>27</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>14</v>
@@ -3693,13 +3701,13 @@
         <v>64</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>197</v>
+        <v>65</v>
       </c>
       <c r="J73" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -3707,31 +3715,31 @@
         <v>27</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>198</v>
+        <v>173</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>199</v>
+        <v>174</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>200</v>
+        <v>14</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J74" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -3739,31 +3747,31 @@
         <v>27</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>202</v>
+        <v>176</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>203</v>
+        <v>14</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J75" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -3771,31 +3779,31 @@
         <v>27</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>204</v>
+        <v>177</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>205</v>
+        <v>178</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>206</v>
+        <v>14</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J76" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -3803,31 +3811,31 @@
         <v>27</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>207</v>
+        <v>179</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>208</v>
+        <v>180</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>209</v>
+        <v>14</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J77" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -3835,31 +3843,31 @@
         <v>27</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>210</v>
+        <v>181</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>212</v>
+        <v>14</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J78" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -3867,31 +3875,31 @@
         <v>27</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>215</v>
+        <v>14</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J79" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -3899,13 +3907,13 @@
         <v>27</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>216</v>
+        <v>185</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>217</v>
+        <v>186</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>14</v>
@@ -3917,13 +3925,13 @@
         <v>64</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>32</v>
+        <v>187</v>
       </c>
       <c r="J80" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -3931,31 +3939,31 @@
         <v>27</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>220</v>
+        <v>14</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>14</v>
+        <v>187</v>
       </c>
       <c r="J81" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -3963,31 +3971,31 @@
         <v>27</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>221</v>
+        <v>190</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>222</v>
+        <v>191</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>223</v>
+        <v>14</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>14</v>
+        <v>192</v>
       </c>
       <c r="J82" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -3995,19 +4003,19 @@
         <v>27</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>224</v>
+        <v>193</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>14</v>
@@ -4019,27 +4027,27 @@
         <v>33</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A84" s="1">
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>227</v>
+        <v>96</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>14</v>
@@ -4051,27 +4059,27 @@
         <v>33</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A85" s="1">
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>14</v>
@@ -4083,91 +4091,91 @@
         <v>33</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A86" s="1">
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>292</v>
+        <v>203</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>14</v>
+        <v>204</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>164</v>
+        <v>14</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="J86" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A87" s="1">
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>236</v>
+        <v>206</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>237</v>
+        <v>14</v>
       </c>
       <c r="J87" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A88" s="1">
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>238</v>
+        <v>208</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>239</v>
+        <v>209</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>240</v>
+        <v>210</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>14</v>
@@ -4179,59 +4187,59 @@
         <v>33</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A89" s="1">
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>241</v>
+        <v>211</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>242</v>
+        <v>212</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>243</v>
+        <v>14</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J89" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A90" s="1">
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>244</v>
+        <v>213</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>245</v>
+        <v>214</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>14</v>
@@ -4243,30 +4251,30 @@
         <v>33</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A91" s="1">
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>14</v>
+        <v>218</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>160</v>
+        <v>288</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I91" s="1" t="s">
         <v>14</v>
@@ -4275,30 +4283,30 @@
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A92" s="1">
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>249</v>
+        <v>219</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>14</v>
+        <v>221</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>160</v>
+        <v>288</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I92" s="1" t="s">
         <v>14</v>
@@ -4307,7 +4315,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -4315,22 +4323,22 @@
         <v>102</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>103</v>
+        <v>222</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>252</v>
+        <v>224</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>14</v>
+        <v>225</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I93" s="1" t="s">
         <v>14</v>
@@ -4339,7 +4347,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -4350,28 +4358,28 @@
         <v>103</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>253</v>
+        <v>226</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>254</v>
+        <v>227</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>14</v>
+        <v>228</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="J94" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -4379,31 +4387,31 @@
         <v>102</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>256</v>
+        <v>103</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>229</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>257</v>
+        <v>14</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>14</v>
+        <v>159</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="J95" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -4411,31 +4419,31 @@
         <v>102</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>258</v>
+        <v>103</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>260</v>
+        <v>14</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>14</v>
+        <v>232</v>
       </c>
       <c r="J96" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -4443,19 +4451,19 @@
         <v>102</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>255</v>
+        <v>103</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>261</v>
+        <v>233</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>262</v>
+        <v>234</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>14</v>
@@ -4467,7 +4475,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -4475,19 +4483,19 @@
         <v>102</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>255</v>
+        <v>103</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>265</v>
+        <v>237</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>266</v>
+        <v>238</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H98" s="1" t="s">
         <v>14</v>
@@ -4499,7 +4507,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -4507,19 +4515,19 @@
         <v>102</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>255</v>
+        <v>103</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>267</v>
+        <v>239</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>268</v>
+        <v>240</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>269</v>
+        <v>241</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>14</v>
@@ -4531,7 +4539,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -4539,19 +4547,19 @@
         <v>102</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>255</v>
+        <v>103</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>270</v>
+        <v>242</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>271</v>
+        <v>243</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>64</v>
@@ -4563,7 +4571,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -4571,19 +4579,19 @@
         <v>102</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>272</v>
+        <v>103</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>273</v>
+        <v>244</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>274</v>
+        <v>245</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>64</v>
@@ -4595,7 +4603,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -4603,19 +4611,19 @@
         <v>102</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>272</v>
+        <v>103</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>275</v>
+        <v>246</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>276</v>
+        <v>247</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>160</v>
+        <v>31</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>64</v>
@@ -4627,7 +4635,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -4635,32 +4643,320 @@
         <v>102</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>272</v>
+        <v>103</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>277</v>
+        <v>248</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>278</v>
+        <v>249</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>64</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="J103" s="1" t="s">
         <v>33</v>
       </c>
     </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A104" s="1">
+        <v>103</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I104" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J104" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A105" s="1">
+        <v>104</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I105" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J105" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A106" s="1">
+        <v>105</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I106" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J106" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A107" s="1">
+        <v>106</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I107" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J107" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A108" s="1">
+        <v>107</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I108" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A109" s="1">
+        <v>108</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J109" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A110" s="1">
+        <v>109</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I110" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J110" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A111" s="1">
+        <v>110</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I111" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J111" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A112" s="1">
+        <v>111</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I112" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J112" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M103" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}"/>
+  <autoFilter ref="A1:M112" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added scope 4 ghg.
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
+++ b/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dataland\Dataland\dataland-framework-toolbox\inputs\sfdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85354912-A1C6-401E-BDDF-A8AEC0A38E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8F43B6-68A1-4599-B37E-74769BB6EC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Framework Data Model" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$M$115</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$M$116</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
     <definedName name="IQ_CY">10000</definedName>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="322">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -1025,10 +1025,16 @@
     <t>The sum of scope 1 and scope 2 emissions of financed companies</t>
   </si>
   <si>
-    <t>Financed scope 4 emissions</t>
-  </si>
-  <si>
-    <t>The scope 4 emissions of financed companies</t>
+    <t>Scope 4 GHG emissions</t>
+  </si>
+  <si>
+    <t>Scope 4 carbon emissions refer to emissions avoided when a product is used as a substitute for other goods or services that fulfill the same functions but have a lower carbon intensity.</t>
+  </si>
+  <si>
+    <t>Scope 1 and 2 and 3 and 4 GHG emissions</t>
+  </si>
+  <si>
+    <t>Sum of scope 1, 2, 3 and 4 carbon emissions</t>
   </si>
 </sst>
 </file>
@@ -1462,10 +1468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}">
-  <dimension ref="A1:M115"/>
+  <dimension ref="A1:M116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
@@ -2053,18 +2059,20 @@
         <v>28</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>50</v>
+        <v>318</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" s="1"/>
+        <v>319</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G19" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>33</v>
@@ -2081,18 +2089,20 @@
         <v>28</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" s="1"/>
+        <v>320</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G20" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>33</v>
@@ -2109,20 +2119,18 @@
         <v>28</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>33</v>
@@ -2139,20 +2147,18 @@
         <v>28</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>33</v>
@@ -2169,12 +2175,14 @@
         <v>28</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>303</v>
+        <v>55</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="F23" s="1"/>
+        <v>285</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G23" s="1" t="s">
         <v>31</v>
       </c>
@@ -2197,12 +2205,14 @@
         <v>28</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>304</v>
+        <v>57</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="F24" s="1"/>
+        <v>277</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G24" s="1" t="s">
         <v>31</v>
       </c>
@@ -2225,10 +2235,10 @@
         <v>28</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
@@ -2253,10 +2263,10 @@
         <v>28</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
@@ -2274,27 +2284,27 @@
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>313</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>317</v>
+      <c r="D27" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>309</v>
       </c>
       <c r="F27" s="1"/>
-      <c r="G27" s="7" t="s">
+      <c r="G27" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H27" s="1"/>
-      <c r="I27" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="J27" s="7" t="s">
+      <c r="I27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J27" s="1" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2302,27 +2312,27 @@
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>315</v>
+      <c r="D28" s="1" t="s">
+        <v>306</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="F28" s="1"/>
-      <c r="G28" s="7" t="s">
+      <c r="G28" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H28" s="1"/>
-      <c r="I28" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="J28" s="7" t="s">
+      <c r="I28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J28" s="1" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2330,27 +2340,29 @@
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H29" s="1"/>
-      <c r="I29" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="J29" s="7" t="s">
+      <c r="D29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2358,29 +2370,27 @@
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1" t="s">
+      <c r="D30" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="J30" s="7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2388,29 +2398,27 @@
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>63</v>
+        <v>28</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>316</v>
       </c>
       <c r="F31" s="1"/>
-      <c r="G31" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J31" s="1" t="s">
+      <c r="G31" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="J31" s="7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2425,10 +2433,10 @@
         <v>61</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1" t="s">
@@ -2455,14 +2463,12 @@
         <v>61</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="F33" s="1"/>
       <c r="G33" s="1" t="s">
         <v>31</v>
       </c>
@@ -2487,10 +2493,10 @@
         <v>61</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>14</v>
@@ -2502,7 +2508,7 @@
         <v>64</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>33</v>
@@ -2519,10 +2525,10 @@
         <v>61</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>14</v>
@@ -2534,7 +2540,7 @@
         <v>64</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>33</v>
@@ -2551,10 +2557,10 @@
         <v>61</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>14</v>
@@ -2566,7 +2572,7 @@
         <v>64</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>33</v>
@@ -2583,25 +2589,25 @@
         <v>61</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2615,23 +2621,25 @@
         <v>61</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F38" s="1"/>
+        <v>78</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="G38" s="1" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2642,25 +2650,23 @@
         <v>27</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>86</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>33</v>
@@ -2677,13 +2683,13 @@
         <v>83</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>288</v>
@@ -2709,13 +2715,13 @@
         <v>83</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>288</v>
@@ -2741,13 +2747,13 @@
         <v>83</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>288</v>
@@ -2770,25 +2776,25 @@
         <v>27</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>33</v>
@@ -2802,15 +2808,17 @@
         <v>27</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F44" s="1"/>
+        <v>98</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G44" s="1" t="s">
         <v>31</v>
       </c>
@@ -2829,28 +2837,26 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="F45" s="1"/>
       <c r="G45" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>33</v>
@@ -2867,13 +2873,13 @@
         <v>103</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>288</v>
@@ -2899,13 +2905,13 @@
         <v>103</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>288</v>
@@ -2931,13 +2937,13 @@
         <v>103</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>288</v>
@@ -2963,13 +2969,13 @@
         <v>103</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>288</v>
@@ -2995,13 +3001,13 @@
         <v>103</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>284</v>
+        <v>117</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>288</v>
@@ -3027,13 +3033,13 @@
         <v>103</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>122</v>
+        <v>284</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>288</v>
@@ -3059,13 +3065,13 @@
         <v>103</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>288</v>
@@ -3091,13 +3097,13 @@
         <v>103</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>288</v>
@@ -3123,13 +3129,13 @@
         <v>103</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>274</v>
+        <v>129</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>288</v>
@@ -3155,13 +3161,13 @@
         <v>103</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>134</v>
+        <v>274</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>288</v>
@@ -3187,13 +3193,13 @@
         <v>103</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>288</v>
@@ -3219,13 +3225,13 @@
         <v>103</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>288</v>
@@ -3251,13 +3257,13 @@
         <v>103</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>288</v>
@@ -3283,13 +3289,13 @@
         <v>103</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E59" s="7" t="s">
-        <v>283</v>
+        <v>141</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>288</v>
@@ -3315,13 +3321,13 @@
         <v>103</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>283</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>288</v>
@@ -3347,13 +3353,13 @@
         <v>103</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>288</v>
@@ -3379,19 +3385,19 @@
         <v>103</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>14</v>
+        <v>151</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>52</v>
+        <v>288</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>14</v>
@@ -3411,10 +3417,10 @@
         <v>103</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>14</v>
@@ -3443,20 +3449,22 @@
         <v>103</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H64" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="I64" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="J64" s="1" t="s">
         <v>33</v>
@@ -3473,19 +3481,21 @@
         <v>103</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>289</v>
+        <v>156</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="F65" s="1"/>
+        <v>157</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G65" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I65" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="J65" s="1" t="s">
         <v>33</v>
       </c>
@@ -3501,10 +3511,10 @@
         <v>103</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
@@ -3529,10 +3539,10 @@
         <v>103</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
@@ -3557,10 +3567,10 @@
         <v>103</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
@@ -3585,21 +3595,19 @@
         <v>103</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
-        <v>31</v>
+        <v>158</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="I69" s="1"/>
       <c r="J69" s="1" t="s">
         <v>33</v>
       </c>
@@ -3615,10 +3623,10 @@
         <v>103</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
@@ -3645,22 +3653,20 @@
         <v>103</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>160</v>
+        <v>299</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="F71" s="1"/>
       <c r="G71" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>14</v>
+        <v>159</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>33</v>
@@ -3671,26 +3677,28 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>162</v>
+        <v>103</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="F72" s="1"/>
+        <v>161</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G72" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J72" s="1" t="s">
         <v>33</v>
@@ -3707,10 +3715,10 @@
         <v>162</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>165</v>
+        <v>275</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
@@ -3737,10 +3745,10 @@
         <v>162</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
@@ -3767,22 +3775,20 @@
         <v>162</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>170</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="F75" s="1"/>
       <c r="G75" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J75" s="1" t="s">
         <v>33</v>
@@ -3796,25 +3802,25 @@
         <v>27</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>14</v>
+        <v>170</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="J76" s="1" t="s">
         <v>33</v>
@@ -3831,10 +3837,10 @@
         <v>61</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>14</v>
@@ -3863,10 +3869,10 @@
         <v>61</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>14</v>
@@ -3895,10 +3901,10 @@
         <v>61</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>14</v>
@@ -3927,10 +3933,10 @@
         <v>61</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>14</v>
@@ -3959,10 +3965,10 @@
         <v>61</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>14</v>
@@ -3991,10 +3997,10 @@
         <v>61</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>14</v>
@@ -4020,13 +4026,13 @@
         <v>27</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>14</v>
@@ -4038,7 +4044,7 @@
         <v>64</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>187</v>
+        <v>65</v>
       </c>
       <c r="J83" s="1" t="s">
         <v>33</v>
@@ -4055,10 +4061,10 @@
         <v>96</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>14</v>
@@ -4087,10 +4093,10 @@
         <v>96</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>14</v>
@@ -4102,7 +4108,7 @@
         <v>64</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="J85" s="1" t="s">
         <v>33</v>
@@ -4119,22 +4125,22 @@
         <v>96</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>195</v>
+        <v>14</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>14</v>
+        <v>192</v>
       </c>
       <c r="J86" s="1" t="s">
         <v>33</v>
@@ -4151,13 +4157,13 @@
         <v>96</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>288</v>
@@ -4180,16 +4186,16 @@
         <v>27</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>288</v>
@@ -4215,13 +4221,13 @@
         <v>83</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>288</v>
@@ -4247,13 +4253,13 @@
         <v>83</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>288</v>
@@ -4279,13 +4285,13 @@
         <v>83</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>288</v>
@@ -4308,25 +4314,25 @@
         <v>27</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>14</v>
+        <v>210</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J92" s="1" t="s">
         <v>33</v>
@@ -4340,25 +4346,25 @@
         <v>27</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>215</v>
+        <v>14</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J93" s="1" t="s">
         <v>33</v>
@@ -4375,13 +4381,13 @@
         <v>83</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>288</v>
@@ -4407,13 +4413,13 @@
         <v>83</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>288</v>
@@ -4433,19 +4439,19 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>222</v>
+        <v>83</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>288</v>
@@ -4468,16 +4474,16 @@
         <v>102</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>103</v>
+        <v>222</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G97" s="1" t="s">
         <v>288</v>
@@ -4503,22 +4509,22 @@
         <v>103</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>286</v>
+        <v>227</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>14</v>
+        <v>228</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>159</v>
+        <v>14</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="J98" s="1" t="s">
         <v>33</v>
@@ -4535,10 +4541,10 @@
         <v>103</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>231</v>
+        <v>286</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>14</v>
@@ -4547,10 +4553,10 @@
         <v>31</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>232</v>
+        <v>72</v>
       </c>
       <c r="J99" s="1" t="s">
         <v>33</v>
@@ -4567,22 +4573,22 @@
         <v>103</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>235</v>
+        <v>14</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>14</v>
+        <v>232</v>
       </c>
       <c r="J100" s="1" t="s">
         <v>33</v>
@@ -4599,13 +4605,13 @@
         <v>103</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>288</v>
@@ -4631,13 +4637,13 @@
         <v>103</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>288</v>
@@ -4663,19 +4669,19 @@
         <v>103</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>14</v>
+        <v>241</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>158</v>
+        <v>288</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I103" s="1" t="s">
         <v>14</v>
@@ -4695,10 +4701,10 @@
         <v>103</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>14</v>
@@ -4727,16 +4733,16 @@
         <v>103</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>31</v>
+        <v>158</v>
       </c>
       <c r="H105" s="1" t="s">
         <v>64</v>
@@ -4759,10 +4765,10 @@
         <v>103</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>14</v>
@@ -4774,7 +4780,7 @@
         <v>64</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="J106" s="1" t="s">
         <v>33</v>
@@ -4788,25 +4794,25 @@
         <v>102</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>251</v>
+        <v>103</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>248</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>252</v>
+        <v>14</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="J107" s="1" t="s">
         <v>33</v>
@@ -4823,13 +4829,13 @@
         <v>250</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>254</v>
+        <v>276</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>288</v>
@@ -4854,14 +4860,14 @@
       <c r="C109" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D109" s="1" t="s">
-        <v>256</v>
+      <c r="D109" s="2" t="s">
+        <v>253</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>288</v>
@@ -4887,13 +4893,13 @@
         <v>250</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G110" s="1" t="s">
         <v>288</v>
@@ -4919,13 +4925,13 @@
         <v>250</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G111" s="1" t="s">
         <v>288</v>
@@ -4951,19 +4957,19 @@
         <v>250</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>14</v>
+        <v>264</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>158</v>
+        <v>288</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I112" s="1" t="s">
         <v>14</v>
@@ -4980,13 +4986,13 @@
         <v>102</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>14</v>
@@ -5015,10 +5021,10 @@
         <v>267</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>14</v>
@@ -5047,16 +5053,16 @@
         <v>267</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="H115" s="1" t="s">
         <v>64</v>
@@ -5068,8 +5074,40 @@
         <v>33</v>
       </c>
     </row>
+    <row r="116" spans="1:10">
+      <c r="A116" s="1">
+        <v>115</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I116" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J116" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M115" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}"/>
+  <autoFilter ref="A1:M116" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
deleted one field in framework.
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
+++ b/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dataland\Dataland\dataland-framework-toolbox\inputs\sfdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8F43B6-68A1-4599-B37E-74769BB6EC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A480180-3EA1-4D55-A340-D4E81C5EA998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
+    <workbookView xWindow="1480" yWindow="1480" windowWidth="14400" windowHeight="7360" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$M$116</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$M$115</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
     <definedName name="IQ_CY">10000</definedName>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="320">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -1029,12 +1029,6 @@
   </si>
   <si>
     <t>Scope 4 carbon emissions refer to emissions avoided when a product is used as a substitute for other goods or services that fulfill the same functions but have a lower carbon intensity.</t>
-  </si>
-  <si>
-    <t>Scope 1 and 2 and 3 and 4 GHG emissions</t>
-  </si>
-  <si>
-    <t>Sum of scope 1, 2, 3 and 4 carbon emissions</t>
   </si>
 </sst>
 </file>
@@ -1468,10 +1462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}">
-  <dimension ref="A1:M116"/>
+  <dimension ref="A1:M115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
@@ -2089,20 +2083,18 @@
         <v>28</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>321</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>33</v>
@@ -2119,10 +2111,10 @@
         <v>28</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
@@ -2147,18 +2139,20 @@
         <v>28</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F22" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G22" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>33</v>
@@ -2175,10 +2169,10 @@
         <v>28</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>14</v>
@@ -2205,14 +2199,12 @@
         <v>28</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>57</v>
+        <v>303</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
         <v>31</v>
       </c>
@@ -2235,10 +2227,10 @@
         <v>28</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
@@ -2263,10 +2255,10 @@
         <v>28</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
@@ -2291,10 +2283,10 @@
         <v>28</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
@@ -2319,19 +2311,21 @@
         <v>28</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="F28" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="G28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" s="1"/>
       <c r="J28" s="1" t="s">
         <v>33</v>
       </c>
@@ -2340,29 +2334,27 @@
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1" t="s">
+      <c r="D29" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H29" s="1"/>
+      <c r="I29" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="J29" s="7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2376,11 +2368,11 @@
       <c r="C30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>313</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>317</v>
+      <c r="D30" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>316</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="7" t="s">
@@ -2398,27 +2390,29 @@
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>316</v>
+        <v>61</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="F31" s="1"/>
-      <c r="G31" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H31" s="1"/>
-      <c r="I31" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="J31" s="7" t="s">
+      <c r="G31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2433,10 +2427,10 @@
         <v>61</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1" t="s">
@@ -2463,12 +2457,14 @@
         <v>61</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F33" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G33" s="1" t="s">
         <v>31</v>
       </c>
@@ -2493,10 +2489,10 @@
         <v>61</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>14</v>
@@ -2508,7 +2504,7 @@
         <v>64</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>33</v>
@@ -2525,10 +2521,10 @@
         <v>61</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>14</v>
@@ -2540,7 +2536,7 @@
         <v>64</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>33</v>
@@ -2557,10 +2553,10 @@
         <v>61</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>14</v>
@@ -2572,7 +2568,7 @@
         <v>64</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>33</v>
@@ -2589,25 +2585,25 @@
         <v>61</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2621,25 +2617,23 @@
         <v>61</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>79</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2650,23 +2644,25 @@
         <v>27</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F39" s="1"/>
+        <v>85</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="G39" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>33</v>
@@ -2683,13 +2679,13 @@
         <v>83</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>288</v>
@@ -2715,13 +2711,13 @@
         <v>83</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>288</v>
@@ -2747,13 +2743,13 @@
         <v>83</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>288</v>
@@ -2776,25 +2772,25 @@
         <v>27</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>95</v>
+        <v>14</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>33</v>
@@ -2808,17 +2804,15 @@
         <v>27</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="F44" s="1"/>
       <c r="G44" s="1" t="s">
         <v>31</v>
       </c>
@@ -2837,26 +2831,28 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F45" s="1"/>
+        <v>105</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="G45" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>33</v>
@@ -2873,13 +2869,13 @@
         <v>103</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>288</v>
@@ -2905,13 +2901,13 @@
         <v>103</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>288</v>
@@ -2937,13 +2933,13 @@
         <v>103</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>288</v>
@@ -2969,13 +2965,13 @@
         <v>103</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>288</v>
@@ -3001,13 +2997,13 @@
         <v>103</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>117</v>
+        <v>284</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>288</v>
@@ -3033,13 +3029,13 @@
         <v>103</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>284</v>
+        <v>122</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>288</v>
@@ -3065,13 +3061,13 @@
         <v>103</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>288</v>
@@ -3097,13 +3093,13 @@
         <v>103</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>288</v>
@@ -3129,13 +3125,13 @@
         <v>103</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>129</v>
+        <v>274</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>288</v>
@@ -3161,13 +3157,13 @@
         <v>103</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>274</v>
+        <v>134</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>288</v>
@@ -3193,13 +3189,13 @@
         <v>103</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>288</v>
@@ -3225,13 +3221,13 @@
         <v>103</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>288</v>
@@ -3257,13 +3253,13 @@
         <v>103</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>288</v>
@@ -3289,13 +3285,13 @@
         <v>103</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>283</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>288</v>
@@ -3321,13 +3317,13 @@
         <v>103</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>283</v>
+        <v>146</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>288</v>
@@ -3353,13 +3349,13 @@
         <v>103</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>288</v>
@@ -3385,19 +3381,19 @@
         <v>103</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>151</v>
+        <v>14</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>288</v>
+        <v>52</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>14</v>
@@ -3417,10 +3413,10 @@
         <v>103</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>14</v>
@@ -3449,22 +3445,20 @@
         <v>103</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>64</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="H64" s="1"/>
       <c r="I64" s="1" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="J64" s="1" t="s">
         <v>33</v>
@@ -3481,21 +3475,19 @@
         <v>103</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>156</v>
+        <v>289</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I65" s="1"/>
       <c r="J65" s="1" t="s">
         <v>33</v>
       </c>
@@ -3511,10 +3503,10 @@
         <v>103</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
@@ -3539,10 +3531,10 @@
         <v>103</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
@@ -3567,10 +3559,10 @@
         <v>103</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
@@ -3595,19 +3587,21 @@
         <v>103</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
-        <v>158</v>
+        <v>31</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I69" s="1"/>
+        <v>159</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="J69" s="1" t="s">
         <v>33</v>
       </c>
@@ -3623,10 +3617,10 @@
         <v>103</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
@@ -3653,20 +3647,22 @@
         <v>103</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>299</v>
+        <v>160</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F71" s="1"/>
+        <v>161</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G71" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>159</v>
+        <v>14</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>33</v>
@@ -3677,28 +3673,26 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>103</v>
+        <v>162</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="F72" s="1"/>
       <c r="G72" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J72" s="1" t="s">
         <v>33</v>
@@ -3715,10 +3709,10 @@
         <v>162</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>275</v>
+        <v>165</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
@@ -3745,10 +3739,10 @@
         <v>162</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
@@ -3775,20 +3769,22 @@
         <v>162</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F75" s="1"/>
+        <v>169</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>170</v>
+      </c>
       <c r="G75" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J75" s="1" t="s">
         <v>33</v>
@@ -3802,25 +3798,25 @@
         <v>27</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>162</v>
+        <v>61</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>170</v>
+        <v>14</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J76" s="1" t="s">
         <v>33</v>
@@ -3837,10 +3833,10 @@
         <v>61</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>14</v>
@@ -3869,10 +3865,10 @@
         <v>61</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>14</v>
@@ -3901,10 +3897,10 @@
         <v>61</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>14</v>
@@ -3933,10 +3929,10 @@
         <v>61</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>14</v>
@@ -3965,10 +3961,10 @@
         <v>61</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>14</v>
@@ -3997,10 +3993,10 @@
         <v>61</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>14</v>
@@ -4026,13 +4022,13 @@
         <v>27</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>14</v>
@@ -4044,7 +4040,7 @@
         <v>64</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>65</v>
+        <v>187</v>
       </c>
       <c r="J83" s="1" t="s">
         <v>33</v>
@@ -4061,10 +4057,10 @@
         <v>96</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>14</v>
@@ -4093,10 +4089,10 @@
         <v>96</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>14</v>
@@ -4108,7 +4104,7 @@
         <v>64</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="J85" s="1" t="s">
         <v>33</v>
@@ -4125,22 +4121,22 @@
         <v>96</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>14</v>
+        <v>195</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>192</v>
+        <v>14</v>
       </c>
       <c r="J86" s="1" t="s">
         <v>33</v>
@@ -4157,13 +4153,13 @@
         <v>96</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>288</v>
@@ -4186,16 +4182,16 @@
         <v>27</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>288</v>
@@ -4221,13 +4217,13 @@
         <v>83</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>288</v>
@@ -4253,13 +4249,13 @@
         <v>83</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>288</v>
@@ -4285,13 +4281,13 @@
         <v>83</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>288</v>
@@ -4314,25 +4310,25 @@
         <v>27</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>210</v>
+        <v>14</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J92" s="1" t="s">
         <v>33</v>
@@ -4346,25 +4342,25 @@
         <v>27</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>14</v>
+        <v>215</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J93" s="1" t="s">
         <v>33</v>
@@ -4381,13 +4377,13 @@
         <v>83</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>288</v>
@@ -4413,13 +4409,13 @@
         <v>83</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>288</v>
@@ -4439,19 +4435,19 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>83</v>
+        <v>222</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>288</v>
@@ -4474,16 +4470,16 @@
         <v>102</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>222</v>
+        <v>103</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="G97" s="1" t="s">
         <v>288</v>
@@ -4509,22 +4505,22 @@
         <v>103</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>227</v>
+        <v>286</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>228</v>
+        <v>14</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>14</v>
+        <v>159</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="J98" s="1" t="s">
         <v>33</v>
@@ -4541,10 +4537,10 @@
         <v>103</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>286</v>
+        <v>231</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>14</v>
@@ -4553,10 +4549,10 @@
         <v>31</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>159</v>
+        <v>64</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>72</v>
+        <v>232</v>
       </c>
       <c r="J99" s="1" t="s">
         <v>33</v>
@@ -4573,22 +4569,22 @@
         <v>103</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>14</v>
+        <v>235</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>232</v>
+        <v>14</v>
       </c>
       <c r="J100" s="1" t="s">
         <v>33</v>
@@ -4605,13 +4601,13 @@
         <v>103</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>288</v>
@@ -4637,13 +4633,13 @@
         <v>103</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>288</v>
@@ -4669,19 +4665,19 @@
         <v>103</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>241</v>
+        <v>14</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>288</v>
+        <v>158</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I103" s="1" t="s">
         <v>14</v>
@@ -4701,10 +4697,10 @@
         <v>103</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>14</v>
@@ -4733,16 +4729,16 @@
         <v>103</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>158</v>
+        <v>31</v>
       </c>
       <c r="H105" s="1" t="s">
         <v>64</v>
@@ -4765,10 +4761,10 @@
         <v>103</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>14</v>
@@ -4780,7 +4776,7 @@
         <v>64</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="J106" s="1" t="s">
         <v>33</v>
@@ -4794,25 +4790,25 @@
         <v>102</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>251</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>249</v>
+        <v>276</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>14</v>
+        <v>252</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="J107" s="1" t="s">
         <v>33</v>
@@ -4829,13 +4825,13 @@
         <v>250</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>276</v>
+        <v>254</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>288</v>
@@ -4860,14 +4856,14 @@
       <c r="C109" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D109" s="2" t="s">
-        <v>253</v>
+      <c r="D109" s="1" t="s">
+        <v>256</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>288</v>
@@ -4893,13 +4889,13 @@
         <v>250</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="G110" s="1" t="s">
         <v>288</v>
@@ -4925,13 +4921,13 @@
         <v>250</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="G111" s="1" t="s">
         <v>288</v>
@@ -4957,19 +4953,19 @@
         <v>250</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>264</v>
+        <v>14</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>288</v>
+        <v>158</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I112" s="1" t="s">
         <v>14</v>
@@ -4986,13 +4982,13 @@
         <v>102</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>14</v>
@@ -5021,10 +5017,10 @@
         <v>267</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>14</v>
@@ -5053,16 +5049,16 @@
         <v>267</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>158</v>
+        <v>52</v>
       </c>
       <c r="H115" s="1" t="s">
         <v>64</v>
@@ -5074,40 +5070,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
-      <c r="A116" s="1">
-        <v>115</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G116" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H116" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I116" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J116" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:M116" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}"/>
+  <autoFilter ref="A1:M115" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Dala 5047 Update SFDR questionnaire (#797)
Introduce three new fields for scope 4, financed scope 1 and scope 2 emissions, financed scope 3 greenhouse gas emissions.
Update tooltips.
---------

Co-authored-by: Jenny <178264328+jenniferlechner@users.noreply.github.com>
Co-authored-by: Dennis Groh <173401487+dennis-dfine@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
+++ b/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93447\Documents\Dataland\dataland-framework-toolbox\inputs\sfdr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dataland\Dataland\dataland-framework-toolbox\inputs\sfdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1735BEFA-D3C6-4FB5-9F3A-A832C2752945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF609C33-5D67-4DBB-AB43-1A7E0F61F9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="1590" windowWidth="26040" windowHeight="13582" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$M$112</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$M$115</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
     <definedName name="IQ_CY">10000</definedName>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="320">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -992,29 +992,50 @@
     <t>GHG intensity - scope 4</t>
   </si>
   <si>
-    <t>Tonnes of Scope 1 GHG emissions / million of the revenue (in the same currency as the total revenue)</t>
-  </si>
-  <si>
-    <t>Tonnes of Scope 2 GHG emissions / million of the revenue (in the same currency as the total revenue)</t>
-  </si>
-  <si>
-    <t>Tonnes of Scope 3 GHG emissions / million of the revenue (in the same currency as the total revenue)</t>
-  </si>
-  <si>
-    <t>Tonnes of Scope 4 GHG emissions / million of the revenue (in the same currency as the total revenue)</t>
-  </si>
-  <si>
     <t>Indirect (gross) carbon emissions from activities related to the production and distribution of goods and services purchased by the reporting company.</t>
   </si>
   <si>
     <t>Indirect (gross) carbon emissions that occur as a result of the use or disposal of the reporting company’s sold products and services.</t>
+  </si>
+  <si>
+    <t>Financed scope 1 and scope 2 emissions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tonnes </t>
+  </si>
+  <si>
+    <t>Financed scope 3 emissions</t>
+  </si>
+  <si>
+    <t>The scope 3 emissions of financed companies</t>
+  </si>
+  <si>
+    <t>The sum of scope 1 and scope 2 emissions of financed companies</t>
+  </si>
+  <si>
+    <t>Scope 4 GHG emissions</t>
+  </si>
+  <si>
+    <t>Tonnes of Scope 1 GHG emissions / million of the revenue (in the same currency as the total revenue). Scope 1 carbon emissions, namely emissions generated from sources that are controlled by the company that issues the underlying assets</t>
+  </si>
+  <si>
+    <t>Tonnes of Scope 2 GHG emissions / million of the revenue (in the same currency as the total revenue). Scope 2 carbon emissions, namely emissions from the consumption of purchased electricity, steam, or other sources of energy generated upstream from the company that issues the underlying assets</t>
+  </si>
+  <si>
+    <t>Scope 4, as defined by the GHG Protocol, covers emissions avoided when a product is used as a substitute for other goods or services, fulfilling the same functions but with a lower carbon intensity.</t>
+  </si>
+  <si>
+    <t>Tonnes of Scope 4 GHG emissions / million of the revenue (in the same currency as the total revenue). Scope 4, as defined by the GHG Protocol, covers emissions avoided when a product is used as a substitute for other goods or services, fulfilling the same functions but with a lower carbon intensity.</t>
+  </si>
+  <si>
+    <t>Tonnes of Scope 3 GHG emissions / million of the revenue (in the same currency as the total revenue). Scope 3 carbon emissions, i.e. all indirect upstream and downstream emissions that are not included in scope 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1050,6 +1071,11 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1103,7 +1129,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -1118,6 +1144,9 @@
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1433,31 +1462,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}">
-  <dimension ref="A1:M112"/>
+  <dimension ref="A1:M115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.86328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.86328125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="61.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="29.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.81640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="61.6328125" style="3" customWidth="1"/>
     <col min="6" max="6" width="79" style="3" customWidth="1"/>
-    <col min="7" max="7" width="39.73046875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.1328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.86328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.3984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1328125" style="3"/>
+    <col min="14" max="16384" width="9.08984375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1498,7 +1527,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1533,7 +1562,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1568,7 +1597,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1603,7 +1632,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1633,7 +1662,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1663,7 +1692,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1691,7 +1720,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1721,7 +1750,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1751,7 +1780,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1781,7 +1810,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1811,7 +1840,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1841,7 +1870,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1871,7 +1900,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1885,7 +1914,7 @@
         <v>301</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
@@ -1899,7 +1928,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1913,7 +1942,7 @@
         <v>302</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
@@ -1927,7 +1956,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1957,7 +1986,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1985,7 +2014,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2013,7 +2042,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2024,24 +2053,26 @@
         <v>28</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>50</v>
+        <v>314</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" s="1"/>
+        <v>317</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G19" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2052,10 +2083,10 @@
         <v>28</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
@@ -2069,7 +2100,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2080,26 +2111,24 @@
         <v>28</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2110,10 +2139,10 @@
         <v>28</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>14</v>
@@ -2129,7 +2158,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2140,12 +2169,14 @@
         <v>28</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>303</v>
+        <v>57</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="F23" s="1"/>
+        <v>277</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G23" s="1" t="s">
         <v>31</v>
       </c>
@@ -2157,7 +2188,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2168,10 +2199,10 @@
         <v>28</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
@@ -2185,7 +2216,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2196,10 +2227,10 @@
         <v>28</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
@@ -2213,7 +2244,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2224,10 +2255,10 @@
         <v>28</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
@@ -2241,7 +2272,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2252,118 +2283,110 @@
         <v>28</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="H28" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>65</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="I28" s="1"/>
       <c r="J28" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>67</v>
+        <v>28</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>313</v>
       </c>
       <c r="F29" s="1"/>
-      <c r="G29" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="G29" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H29" s="1"/>
+      <c r="I29" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2374,14 +2397,12 @@
         <v>61</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
         <v>31</v>
       </c>
@@ -2389,13 +2410,13 @@
         <v>64</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2406,14 +2427,12 @@
         <v>61</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="F32" s="1"/>
       <c r="G32" s="1" t="s">
         <v>31</v>
       </c>
@@ -2427,7 +2446,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2438,10 +2457,10 @@
         <v>61</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>14</v>
@@ -2453,13 +2472,13 @@
         <v>64</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2470,28 +2489,28 @@
         <v>61</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2502,12 +2521,14 @@
         <v>61</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F35" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G35" s="1" t="s">
         <v>31</v>
       </c>
@@ -2521,7 +2542,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2529,31 +2550,31 @@
         <v>27</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>86</v>
+        <v>14</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2561,19 +2582,19 @@
         <v>27</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>288</v>
+        <v>80</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>14</v>
@@ -2582,10 +2603,10 @@
         <v>14</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2593,31 +2614,29 @@
         <v>27</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>92</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2628,13 +2647,13 @@
         <v>83</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>288</v>
@@ -2649,7 +2668,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2657,31 +2676,31 @@
         <v>27</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2689,46 +2708,48 @@
         <v>27</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F41" s="1"/>
+        <v>91</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="G41" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>288</v>
@@ -2743,71 +2764,69 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:10">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>109</v>
+        <v>14</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>112</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="F44" s="1"/>
       <c r="G44" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2818,13 +2837,13 @@
         <v>103</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>288</v>
@@ -2839,7 +2858,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2850,13 +2869,13 @@
         <v>103</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>288</v>
@@ -2871,7 +2890,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2882,13 +2901,13 @@
         <v>103</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>284</v>
+        <v>111</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>288</v>
@@ -2903,7 +2922,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:10">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2914,13 +2933,13 @@
         <v>103</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>288</v>
@@ -2935,7 +2954,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2946,13 +2965,13 @@
         <v>103</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>288</v>
@@ -2967,7 +2986,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:10">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2978,13 +2997,13 @@
         <v>103</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>128</v>
+        <v>284</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>288</v>
@@ -2999,7 +3018,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:10">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -3010,13 +3029,13 @@
         <v>103</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>274</v>
+        <v>123</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>288</v>
@@ -3031,7 +3050,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:10">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3042,13 +3061,13 @@
         <v>103</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>288</v>
@@ -3063,7 +3082,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:10">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3074,13 +3093,13 @@
         <v>103</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>288</v>
@@ -3095,7 +3114,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:10">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3106,13 +3125,13 @@
         <v>103</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>140</v>
+        <v>274</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>288</v>
@@ -3127,7 +3146,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:10">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3138,13 +3157,13 @@
         <v>103</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>288</v>
@@ -3159,7 +3178,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:10">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3170,13 +3189,13 @@
         <v>103</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>283</v>
+        <v>135</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>288</v>
@@ -3191,7 +3210,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:10">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3202,13 +3221,13 @@
         <v>103</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>288</v>
@@ -3223,7 +3242,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:10">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3234,13 +3253,13 @@
         <v>103</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>288</v>
@@ -3255,7 +3274,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:10">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3266,19 +3285,19 @@
         <v>103</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>153</v>
+        <v>144</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>283</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>14</v>
+        <v>145</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>52</v>
+        <v>288</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>14</v>
@@ -3287,7 +3306,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:10">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -3298,19 +3317,19 @@
         <v>103</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>14</v>
+        <v>148</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>52</v>
+        <v>288</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>14</v>
@@ -3319,7 +3338,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:10">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -3330,26 +3349,28 @@
         <v>103</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>14</v>
+        <v>151</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H61" s="1"/>
+        <v>288</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="I61" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:10">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -3360,24 +3381,28 @@
         <v>103</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>289</v>
+        <v>152</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="F62" s="1"/>
+        <v>153</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G62" s="1" t="s">
-        <v>158</v>
+        <v>52</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I62" s="1"/>
+      <c r="I62" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="J62" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:10">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -3388,24 +3413,28 @@
         <v>103</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>291</v>
+        <v>154</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="F63" s="1"/>
+        <v>155</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G63" s="1" t="s">
-        <v>158</v>
+        <v>52</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I63" s="1"/>
+      <c r="I63" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="J63" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:10">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -3416,24 +3445,26 @@
         <v>103</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>293</v>
+        <v>156</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="F64" s="1"/>
+        <v>157</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G64" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I64" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="J64" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:10">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -3444,10 +3475,10 @@
         <v>103</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
@@ -3461,7 +3492,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:10">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -3472,26 +3503,24 @@
         <v>103</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
-        <v>31</v>
+        <v>158</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="I66" s="1"/>
       <c r="J66" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:10">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -3502,26 +3531,24 @@
         <v>103</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
-        <v>31</v>
+        <v>158</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I67" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="I67" s="1"/>
       <c r="J67" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:10">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -3532,118 +3559,116 @@
         <v>103</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>160</v>
+        <v>295</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
-        <v>288</v>
+        <v>158</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="I68" s="1"/>
       <c r="J68" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:10">
       <c r="A69" s="1">
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>162</v>
+        <v>103</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>163</v>
+        <v>297</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>275</v>
+        <v>298</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="J69" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:10">
       <c r="A70" s="1">
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>162</v>
+        <v>103</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>164</v>
+        <v>299</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>165</v>
+        <v>300</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:10">
       <c r="A71" s="1">
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>162</v>
+        <v>103</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F71" s="1"/>
+        <v>161</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G71" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:10">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -3654,28 +3679,26 @@
         <v>162</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>170</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="F72" s="1"/>
       <c r="G72" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J72" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:10">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -3683,17 +3706,15 @@
         <v>27</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
         <v>31</v>
       </c>
@@ -3701,13 +3722,13 @@
         <v>64</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="J73" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:10">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -3715,17 +3736,15 @@
         <v>27</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
         <v>31</v>
       </c>
@@ -3733,13 +3752,13 @@
         <v>64</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="J74" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:10">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -3747,31 +3766,31 @@
         <v>27</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>14</v>
+        <v>170</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="J75" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:10">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -3782,10 +3801,10 @@
         <v>61</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>14</v>
@@ -3803,7 +3822,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:10">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -3814,10 +3833,10 @@
         <v>61</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>14</v>
@@ -3835,7 +3854,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:10">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -3846,10 +3865,10 @@
         <v>61</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>14</v>
@@ -3867,7 +3886,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:10">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -3878,10 +3897,10 @@
         <v>61</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>14</v>
@@ -3899,7 +3918,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:10">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -3907,13 +3926,13 @@
         <v>27</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>14</v>
@@ -3925,13 +3944,13 @@
         <v>64</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>187</v>
+        <v>65</v>
       </c>
       <c r="J80" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:10">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -3939,13 +3958,13 @@
         <v>27</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>14</v>
@@ -3957,13 +3976,13 @@
         <v>64</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>187</v>
+        <v>65</v>
       </c>
       <c r="J81" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:10">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -3971,13 +3990,13 @@
         <v>27</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>14</v>
@@ -3989,13 +4008,13 @@
         <v>64</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>192</v>
+        <v>65</v>
       </c>
       <c r="J82" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:10">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -4006,28 +4025,28 @@
         <v>96</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>195</v>
+        <v>14</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>14</v>
+        <v>187</v>
       </c>
       <c r="J83" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:10">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -4038,28 +4057,28 @@
         <v>96</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>198</v>
+        <v>14</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>14</v>
+        <v>187</v>
       </c>
       <c r="J84" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:10">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -4067,31 +4086,31 @@
         <v>27</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>201</v>
+        <v>14</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>14</v>
+        <v>192</v>
       </c>
       <c r="J85" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:10">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -4099,16 +4118,16 @@
         <v>27</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="G86" s="1" t="s">
         <v>288</v>
@@ -4123,7 +4142,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:10">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -4131,16 +4150,16 @@
         <v>27</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>288</v>
@@ -4155,7 +4174,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:10">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -4166,13 +4185,13 @@
         <v>83</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>288</v>
@@ -4187,7 +4206,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:10">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -4195,31 +4214,31 @@
         <v>27</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>14</v>
+        <v>204</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J89" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:10">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -4230,13 +4249,13 @@
         <v>83</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>288</v>
@@ -4251,7 +4270,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:10">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -4262,13 +4281,13 @@
         <v>83</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>288</v>
@@ -4283,7 +4302,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:10">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -4291,48 +4310,48 @@
         <v>27</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>221</v>
+        <v>14</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J92" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:10">
       <c r="A93" s="1">
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>222</v>
+        <v>83</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>288</v>
@@ -4347,24 +4366,24 @@
         <v>33</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:10">
       <c r="A94" s="1">
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>288</v>
@@ -4379,39 +4398,39 @@
         <v>33</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:10">
       <c r="A95" s="1">
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>286</v>
+        <v>220</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>14</v>
+        <v>221</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>159</v>
+        <v>14</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="J95" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:10">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -4419,31 +4438,31 @@
         <v>102</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>103</v>
+        <v>222</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>14</v>
+        <v>225</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>232</v>
+        <v>14</v>
       </c>
       <c r="J96" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:10">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -4454,13 +4473,13 @@
         <v>103</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="G97" s="1" t="s">
         <v>288</v>
@@ -4475,7 +4494,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:10">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -4486,28 +4505,28 @@
         <v>103</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>237</v>
+        <v>286</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>238</v>
+        <v>14</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>14</v>
+        <v>159</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="J98" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:10">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -4518,28 +4537,28 @@
         <v>103</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>241</v>
+        <v>14</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>14</v>
+        <v>232</v>
       </c>
       <c r="J99" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:10">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -4550,19 +4569,19 @@
         <v>103</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>14</v>
+        <v>235</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>158</v>
+        <v>288</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I100" s="1" t="s">
         <v>14</v>
@@ -4571,7 +4590,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:10">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -4582,19 +4601,19 @@
         <v>103</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>14</v>
+        <v>238</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>158</v>
+        <v>288</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I101" s="1" t="s">
         <v>14</v>
@@ -4603,7 +4622,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:10">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -4614,19 +4633,19 @@
         <v>103</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>14</v>
+        <v>241</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>31</v>
+        <v>288</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I102" s="1" t="s">
         <v>14</v>
@@ -4635,7 +4654,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:10">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -4646,28 +4665,28 @@
         <v>103</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>31</v>
+        <v>158</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>64</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="J103" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:10">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -4675,22 +4694,22 @@
         <v>102</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>251</v>
+        <v>103</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>244</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>276</v>
+        <v>245</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>252</v>
+        <v>14</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>288</v>
+        <v>158</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I104" s="1" t="s">
         <v>14</v>
@@ -4699,7 +4718,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:10">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -4707,22 +4726,22 @@
         <v>102</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>253</v>
+        <v>103</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>246</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>255</v>
+        <v>14</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I105" s="1" t="s">
         <v>14</v>
@@ -4731,7 +4750,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:10">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -4739,31 +4758,31 @@
         <v>102</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>250</v>
+        <v>103</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>258</v>
+        <v>14</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>288</v>
+        <v>31</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="J106" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:10">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -4773,14 +4792,14 @@
       <c r="C107" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D107" s="1" t="s">
-        <v>259</v>
+      <c r="D107" s="2" t="s">
+        <v>251</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="G107" s="1" t="s">
         <v>288</v>
@@ -4795,7 +4814,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:10">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -4805,14 +4824,14 @@
       <c r="C108" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D108" s="1" t="s">
-        <v>262</v>
+      <c r="D108" s="2" t="s">
+        <v>253</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>288</v>
@@ -4827,7 +4846,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:10">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -4838,19 +4857,19 @@
         <v>250</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>14</v>
+        <v>258</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>158</v>
+        <v>288</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I109" s="1" t="s">
         <v>14</v>
@@ -4859,7 +4878,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:10">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -4867,22 +4886,22 @@
         <v>102</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>14</v>
+        <v>261</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>158</v>
+        <v>288</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I110" s="1" t="s">
         <v>14</v>
@@ -4891,7 +4910,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:10">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -4899,22 +4918,22 @@
         <v>102</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>14</v>
+        <v>264</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>158</v>
+        <v>288</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I111" s="1" t="s">
         <v>14</v>
@@ -4923,7 +4942,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:10">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -4931,19 +4950,19 @@
         <v>102</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="H112" s="1" t="s">
         <v>64</v>
@@ -4955,8 +4974,104 @@
         <v>33</v>
       </c>
     </row>
+    <row r="113" spans="1:10">
+      <c r="A113" s="1">
+        <v>112</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J113" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10">
+      <c r="A114" s="1">
+        <v>113</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I114" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J114" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10">
+      <c r="A115" s="1">
+        <v>114</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I115" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J115" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M112" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}"/>
+  <autoFilter ref="A1:M115" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated tooltips for workdays lost and non renewable energy consumption crude oil
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
+++ b/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dataland\Dataland\dataland-framework-toolbox\inputs\sfdr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d60171\GitHub\Dataland\dataland-framework-toolbox\inputs\sfdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF609C33-5D67-4DBB-AB43-1A7E0F61F9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF925873-EA1A-47E2-9BFD-9454B5B5F7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="2" r:id="rId1"/>
@@ -593,9 +593,6 @@
     <t>Non-Renewable Energy Consumption Crude Oil</t>
   </si>
   <si>
-    <t>Energy consumption from crude oil (non-renewable energy source)</t>
-  </si>
-  <si>
     <t>Non-Renewable Energy Consumption Natural Gas</t>
   </si>
   <si>
@@ -764,9 +761,6 @@
     <t>Workdays Lost</t>
   </si>
   <si>
-    <t>Number of workdays lost to injuries, accidents, fatalities or illness</t>
-  </si>
-  <si>
     <t>Days</t>
   </si>
   <si>
@@ -1029,6 +1023,12 @@
   </si>
   <si>
     <t>Tonnes of Scope 3 GHG emissions / million of the revenue (in the same currency as the total revenue). Scope 3 carbon emissions, i.e. all indirect upstream and downstream emissions that are not included in scope 2</t>
+  </si>
+  <si>
+    <t>Energy consumption from crude oil (including petrol, diesel, fuel oil and others) (non-renewable energy source)</t>
+  </si>
+  <si>
+    <t>Number of workdays lost to injuries, accidents, fatalities or illness in total</t>
   </si>
 </sst>
 </file>
@@ -1464,26 +1464,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}">
   <dimension ref="A1:M115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.81640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="61.6328125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="29.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.77734375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="61.6640625" style="3" customWidth="1"/>
     <col min="6" max="6" width="79" style="3" customWidth="1"/>
-    <col min="7" max="7" width="39.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.36328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.08984375" style="3"/>
+    <col min="14" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -1538,10 +1538,10 @@
         <v>13</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>14</v>
@@ -1911,10 +1911,10 @@
         <v>28</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
@@ -1939,10 +1939,10 @@
         <v>28</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
@@ -1997,10 +1997,10 @@
         <v>28</v>
       </c>
       <c r="D17" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>278</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>280</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
@@ -2025,10 +2025,10 @@
         <v>28</v>
       </c>
       <c r="D18" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>279</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>281</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
@@ -2053,10 +2053,10 @@
         <v>28</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>14</v>
@@ -2142,7 +2142,7 @@
         <v>55</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>14</v>
@@ -2172,7 +2172,7 @@
         <v>57</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>14</v>
@@ -2199,10 +2199,10 @@
         <v>28</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
@@ -2227,10 +2227,10 @@
         <v>28</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
@@ -2255,10 +2255,10 @@
         <v>28</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
@@ -2283,10 +2283,10 @@
         <v>28</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
@@ -2320,7 +2320,7 @@
         <v>60</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>14</v>
@@ -2341,10 +2341,10 @@
         <v>28</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="7" t="s">
@@ -2352,7 +2352,7 @@
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J29" s="7" t="s">
         <v>33</v>
@@ -2369,10 +2369,10 @@
         <v>28</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="7" t="s">
@@ -2380,7 +2380,7 @@
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J30" s="7" t="s">
         <v>33</v>
@@ -2656,7 +2656,7 @@
         <v>86</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>14</v>
@@ -2688,7 +2688,7 @@
         <v>89</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>14</v>
@@ -2720,7 +2720,7 @@
         <v>92</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>14</v>
@@ -2752,7 +2752,7 @@
         <v>95</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>14</v>
@@ -2846,7 +2846,7 @@
         <v>106</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>14</v>
@@ -2878,7 +2878,7 @@
         <v>109</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>14</v>
@@ -2910,7 +2910,7 @@
         <v>112</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>14</v>
@@ -2942,7 +2942,7 @@
         <v>115</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>14</v>
@@ -2974,7 +2974,7 @@
         <v>118</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>14</v>
@@ -3000,13 +3000,13 @@
         <v>119</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>14</v>
@@ -3038,7 +3038,7 @@
         <v>123</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>14</v>
@@ -3070,7 +3070,7 @@
         <v>126</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>14</v>
@@ -3102,7 +3102,7 @@
         <v>129</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>14</v>
@@ -3131,10 +3131,10 @@
         <v>131</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>14</v>
@@ -3166,7 +3166,7 @@
         <v>134</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>14</v>
@@ -3198,7 +3198,7 @@
         <v>137</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>14</v>
@@ -3230,7 +3230,7 @@
         <v>140</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>14</v>
@@ -3262,7 +3262,7 @@
         <v>143</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>14</v>
@@ -3288,13 +3288,13 @@
         <v>144</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>145</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>14</v>
@@ -3326,7 +3326,7 @@
         <v>148</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>14</v>
@@ -3358,7 +3358,7 @@
         <v>151</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>14</v>
@@ -3475,10 +3475,10 @@
         <v>103</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
@@ -3503,10 +3503,10 @@
         <v>103</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
@@ -3531,10 +3531,10 @@
         <v>103</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
@@ -3559,10 +3559,10 @@
         <v>103</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
@@ -3587,10 +3587,10 @@
         <v>103</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
@@ -3617,10 +3617,10 @@
         <v>103</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
@@ -3656,7 +3656,7 @@
         <v>14</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>14</v>
@@ -3682,7 +3682,7 @@
         <v>163</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1" t="s">
@@ -3778,7 +3778,7 @@
         <v>170</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>14</v>
@@ -3836,7 +3836,7 @@
         <v>173</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>174</v>
+        <v>318</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>14</v>
@@ -3865,10 +3865,10 @@
         <v>61</v>
       </c>
       <c r="D78" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>14</v>
@@ -3897,10 +3897,10 @@
         <v>61</v>
       </c>
       <c r="D79" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E79" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>14</v>
@@ -3929,10 +3929,10 @@
         <v>61</v>
       </c>
       <c r="D80" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E80" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>14</v>
@@ -3961,10 +3961,10 @@
         <v>61</v>
       </c>
       <c r="D81" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E81" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>14</v>
@@ -3993,10 +3993,10 @@
         <v>61</v>
       </c>
       <c r="D82" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E82" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>14</v>
@@ -4025,10 +4025,10 @@
         <v>96</v>
       </c>
       <c r="D83" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>14</v>
@@ -4040,7 +4040,7 @@
         <v>64</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J83" s="1" t="s">
         <v>33</v>
@@ -4057,10 +4057,10 @@
         <v>96</v>
       </c>
       <c r="D84" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E84" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>14</v>
@@ -4072,7 +4072,7 @@
         <v>64</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J84" s="1" t="s">
         <v>33</v>
@@ -4089,10 +4089,10 @@
         <v>96</v>
       </c>
       <c r="D85" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E85" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>14</v>
@@ -4104,7 +4104,7 @@
         <v>64</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J85" s="1" t="s">
         <v>33</v>
@@ -4121,16 +4121,16 @@
         <v>96</v>
       </c>
       <c r="D86" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E86" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E86" s="1" t="s">
+      <c r="F86" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="F86" s="1" t="s">
-        <v>195</v>
-      </c>
       <c r="G86" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>14</v>
@@ -4153,16 +4153,16 @@
         <v>96</v>
       </c>
       <c r="D87" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E87" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E87" s="1" t="s">
+      <c r="F87" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="F87" s="1" t="s">
-        <v>198</v>
-      </c>
       <c r="G87" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>14</v>
@@ -4185,16 +4185,16 @@
         <v>83</v>
       </c>
       <c r="D88" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E88" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="F88" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="F88" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="G88" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>14</v>
@@ -4217,16 +4217,16 @@
         <v>83</v>
       </c>
       <c r="D89" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E89" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E89" s="1" t="s">
+      <c r="F89" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="F89" s="1" t="s">
-        <v>204</v>
-      </c>
       <c r="G89" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>14</v>
@@ -4249,16 +4249,16 @@
         <v>83</v>
       </c>
       <c r="D90" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E90" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E90" s="1" t="s">
+      <c r="F90" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="F90" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="G90" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>14</v>
@@ -4281,16 +4281,16 @@
         <v>83</v>
       </c>
       <c r="D91" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E91" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="F91" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="F91" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="G91" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>14</v>
@@ -4313,10 +4313,10 @@
         <v>99</v>
       </c>
       <c r="D92" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E92" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>14</v>
@@ -4345,16 +4345,16 @@
         <v>83</v>
       </c>
       <c r="D93" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E93" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E93" s="1" t="s">
+      <c r="F93" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="F93" s="1" t="s">
-        <v>215</v>
-      </c>
       <c r="G93" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>14</v>
@@ -4377,16 +4377,16 @@
         <v>83</v>
       </c>
       <c r="D94" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E94" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E94" s="1" t="s">
+      <c r="F94" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F94" s="1" t="s">
-        <v>218</v>
-      </c>
       <c r="G94" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>14</v>
@@ -4409,16 +4409,16 @@
         <v>83</v>
       </c>
       <c r="D95" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E95" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E95" s="1" t="s">
+      <c r="F95" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F95" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="G95" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>14</v>
@@ -4438,19 +4438,19 @@
         <v>102</v>
       </c>
       <c r="C96" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="E96" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="E96" s="1" t="s">
+      <c r="F96" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="F96" s="1" t="s">
-        <v>225</v>
-      </c>
       <c r="G96" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>14</v>
@@ -4473,16 +4473,16 @@
         <v>103</v>
       </c>
       <c r="D97" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E97" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="E97" s="1" t="s">
+      <c r="F97" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="F97" s="1" t="s">
-        <v>228</v>
-      </c>
       <c r="G97" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>14</v>
@@ -4505,10 +4505,10 @@
         <v>103</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>14</v>
@@ -4537,10 +4537,10 @@
         <v>103</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>231</v>
+        <v>319</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>14</v>
@@ -4552,7 +4552,7 @@
         <v>64</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J99" s="1" t="s">
         <v>33</v>
@@ -4569,16 +4569,16 @@
         <v>103</v>
       </c>
       <c r="D100" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F100" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="E100" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>235</v>
-      </c>
       <c r="G100" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>14</v>
@@ -4601,16 +4601,16 @@
         <v>103</v>
       </c>
       <c r="D101" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F101" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E101" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>238</v>
-      </c>
       <c r="G101" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>14</v>
@@ -4633,16 +4633,16 @@
         <v>103</v>
       </c>
       <c r="D102" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F102" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E102" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>241</v>
-      </c>
       <c r="G102" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>14</v>
@@ -4665,10 +4665,10 @@
         <v>103</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>14</v>
@@ -4697,10 +4697,10 @@
         <v>103</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>14</v>
@@ -4729,10 +4729,10 @@
         <v>103</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>14</v>
@@ -4761,10 +4761,10 @@
         <v>103</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>14</v>
@@ -4790,19 +4790,19 @@
         <v>102</v>
       </c>
       <c r="C107" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F107" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D107" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>252</v>
-      </c>
       <c r="G107" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H107" s="1" t="s">
         <v>14</v>
@@ -4822,19 +4822,19 @@
         <v>102</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D108" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F108" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="E108" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>255</v>
-      </c>
       <c r="G108" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H108" s="1" t="s">
         <v>14</v>
@@ -4854,19 +4854,19 @@
         <v>102</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D109" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F109" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="E109" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="G109" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H109" s="1" t="s">
         <v>14</v>
@@ -4886,19 +4886,19 @@
         <v>102</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D110" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F110" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="E110" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>261</v>
-      </c>
       <c r="G110" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H110" s="1" t="s">
         <v>14</v>
@@ -4918,19 +4918,19 @@
         <v>102</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D111" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F111" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="E111" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="F111" s="1" t="s">
-        <v>264</v>
-      </c>
       <c r="G111" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H111" s="1" t="s">
         <v>14</v>
@@ -4950,13 +4950,13 @@
         <v>102</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>14</v>
@@ -4982,13 +4982,13 @@
         <v>102</v>
       </c>
       <c r="C113" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E113" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>14</v>
@@ -5014,13 +5014,13 @@
         <v>102</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>14</v>
@@ -5046,13 +5046,13 @@
         <v>102</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
changed rate of accidents to without percentage and added migration script
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
+++ b/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d60171\GitHub\Dataland\dataland-framework-toolbox\inputs\sfdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF925873-EA1A-47E2-9BFD-9454B5B5F7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34575512-9EE1-4F2A-937A-D8562FB1FDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="320">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -1464,8 +1464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}">
   <dimension ref="A1:M115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+    <sheetView tabSelected="1" topLeftCell="E84" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I97" sqref="I97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -4517,11 +4517,9 @@
         <v>31</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I98" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="I98" s="1"/>
       <c r="J98" s="1" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
tests for migration and started ceo pay ratio
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
+++ b/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d60171\GitHub\Dataland\dataland-framework-toolbox\inputs\sfdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34575512-9EE1-4F2A-937A-D8562FB1FDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C4837B-C32D-4186-8700-4B854BB5CB17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Framework Data Model" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$M$115</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$M$114</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
     <definedName name="IQ_CY">10000</definedName>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="318">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -803,18 +803,9 @@
     <t>Number of discrimination related incidents reported that lead to any kind of penalty and/or fine</t>
   </si>
   <si>
-    <t>CEO to Employee Pay Gap Ratio</t>
-  </si>
-  <si>
-    <t>Annual total compensation for the highest compensated individual divided by the median annual total compensation for all employees (excluding the highest-compensated individual).</t>
-  </si>
-  <si>
     <t>Excessive CEO pay ratio</t>
   </si>
   <si>
-    <t>Average ratio of the annual total compensation for the highest compensated individual to the median annual total compensation for all employees (excluding the highest-compensated individual)</t>
-  </si>
-  <si>
     <t>Human rights</t>
   </si>
   <si>
@@ -1029,6 +1020,9 @@
   </si>
   <si>
     <t>Number of workdays lost to injuries, accidents, fatalities or illness in total</t>
+  </si>
+  <si>
+    <t>Annual total compensation for the highest compensated individual divided by the median annual total compensation for all employees (excluding the highest-compensated individual)</t>
   </si>
 </sst>
 </file>
@@ -1462,10 +1456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}">
-  <dimension ref="A1:M115"/>
+  <dimension ref="A1:M114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E84" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I97" sqref="I97"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H105" sqref="H105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -1538,10 +1532,10 @@
         <v>13</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>14</v>
@@ -1911,10 +1905,10 @@
         <v>28</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
@@ -1939,10 +1933,10 @@
         <v>28</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
@@ -1997,10 +1991,10 @@
         <v>28</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
@@ -2025,10 +2019,10 @@
         <v>28</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
@@ -2053,10 +2047,10 @@
         <v>28</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>312</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>315</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>14</v>
@@ -2142,7 +2136,7 @@
         <v>55</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>14</v>
@@ -2172,7 +2166,7 @@
         <v>57</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>14</v>
@@ -2199,10 +2193,10 @@
         <v>28</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
@@ -2227,10 +2221,10 @@
         <v>28</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
@@ -2255,10 +2249,10 @@
         <v>28</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
@@ -2283,10 +2277,10 @@
         <v>28</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
@@ -2320,7 +2314,7 @@
         <v>60</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>14</v>
@@ -2341,10 +2335,10 @@
         <v>28</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="7" t="s">
@@ -2352,7 +2346,7 @@
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="7" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="J29" s="7" t="s">
         <v>33</v>
@@ -2369,10 +2363,10 @@
         <v>28</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="7" t="s">
@@ -2380,7 +2374,7 @@
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="7" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="J30" s="7" t="s">
         <v>33</v>
@@ -2656,7 +2650,7 @@
         <v>86</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>14</v>
@@ -2688,7 +2682,7 @@
         <v>89</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>14</v>
@@ -2720,7 +2714,7 @@
         <v>92</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>14</v>
@@ -2752,7 +2746,7 @@
         <v>95</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>14</v>
@@ -2846,7 +2840,7 @@
         <v>106</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>14</v>
@@ -2878,7 +2872,7 @@
         <v>109</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>14</v>
@@ -2910,7 +2904,7 @@
         <v>112</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>14</v>
@@ -2942,7 +2936,7 @@
         <v>115</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>14</v>
@@ -2974,7 +2968,7 @@
         <v>118</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>14</v>
@@ -3000,13 +2994,13 @@
         <v>119</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>14</v>
@@ -3038,7 +3032,7 @@
         <v>123</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>14</v>
@@ -3070,7 +3064,7 @@
         <v>126</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>14</v>
@@ -3102,7 +3096,7 @@
         <v>129</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>14</v>
@@ -3131,10 +3125,10 @@
         <v>131</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>14</v>
@@ -3166,7 +3160,7 @@
         <v>134</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>14</v>
@@ -3198,7 +3192,7 @@
         <v>137</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>14</v>
@@ -3230,7 +3224,7 @@
         <v>140</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>14</v>
@@ -3262,7 +3256,7 @@
         <v>143</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>14</v>
@@ -3288,13 +3282,13 @@
         <v>144</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>145</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>14</v>
@@ -3326,7 +3320,7 @@
         <v>148</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>14</v>
@@ -3358,7 +3352,7 @@
         <v>151</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>14</v>
@@ -3475,10 +3469,10 @@
         <v>103</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
@@ -3503,10 +3497,10 @@
         <v>103</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
@@ -3531,10 +3525,10 @@
         <v>103</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
@@ -3559,10 +3553,10 @@
         <v>103</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
@@ -3587,10 +3581,10 @@
         <v>103</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
@@ -3617,10 +3611,10 @@
         <v>103</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
@@ -3656,7 +3650,7 @@
         <v>14</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>14</v>
@@ -3682,7 +3676,7 @@
         <v>163</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1" t="s">
@@ -3778,7 +3772,7 @@
         <v>170</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>14</v>
@@ -3836,7 +3830,7 @@
         <v>173</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>14</v>
@@ -4130,7 +4124,7 @@
         <v>194</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>14</v>
@@ -4162,7 +4156,7 @@
         <v>197</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>14</v>
@@ -4194,7 +4188,7 @@
         <v>200</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>14</v>
@@ -4226,7 +4220,7 @@
         <v>203</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>14</v>
@@ -4258,7 +4252,7 @@
         <v>206</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>14</v>
@@ -4290,7 +4284,7 @@
         <v>209</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>14</v>
@@ -4354,7 +4348,7 @@
         <v>214</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>14</v>
@@ -4386,7 +4380,7 @@
         <v>217</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>14</v>
@@ -4418,7 +4412,7 @@
         <v>220</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>14</v>
@@ -4450,7 +4444,7 @@
         <v>224</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>14</v>
@@ -4482,7 +4476,7 @@
         <v>227</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>14</v>
@@ -4508,7 +4502,7 @@
         <v>228</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>14</v>
@@ -4538,7 +4532,7 @@
         <v>229</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>14</v>
@@ -4576,7 +4570,7 @@
         <v>233</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>14</v>
@@ -4608,7 +4602,7 @@
         <v>236</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>14</v>
@@ -4640,7 +4634,7 @@
         <v>239</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>14</v>
@@ -4718,7 +4712,7 @@
     </row>
     <row r="105" spans="1:10">
       <c r="A105" s="1">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>102</v>
@@ -4730,7 +4724,7 @@
         <v>244</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>245</v>
+        <v>317</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>14</v>
@@ -4741,40 +4735,38 @@
       <c r="H105" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I105" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="I105" s="1"/>
       <c r="J105" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="106" spans="1:10">
       <c r="A106" s="1">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D106" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D106" s="2" t="s">
         <v>246</v>
       </c>
       <c r="E106" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F106" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="F106" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="G106" s="1" t="s">
-        <v>31</v>
+        <v>283</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="J106" s="1" t="s">
         <v>33</v>
@@ -4782,25 +4774,25 @@
     </row>
     <row r="107" spans="1:10">
       <c r="A107" s="1">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C107" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D107" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="D107" s="2" t="s">
+      <c r="E107" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>274</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>250</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H107" s="1" t="s">
         <v>14</v>
@@ -4814,15 +4806,15 @@
     </row>
     <row r="108" spans="1:10">
       <c r="A108" s="1">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D108" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D108" s="1" t="s">
         <v>251</v>
       </c>
       <c r="E108" s="1" t="s">
@@ -4832,7 +4824,7 @@
         <v>253</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H108" s="1" t="s">
         <v>14</v>
@@ -4846,13 +4838,13 @@
     </row>
     <row r="109" spans="1:10">
       <c r="A109" s="1">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>254</v>
@@ -4864,7 +4856,7 @@
         <v>256</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H109" s="1" t="s">
         <v>14</v>
@@ -4878,13 +4870,13 @@
     </row>
     <row r="110" spans="1:10">
       <c r="A110" s="1">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>257</v>
@@ -4896,7 +4888,7 @@
         <v>259</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H110" s="1" t="s">
         <v>14</v>
@@ -4910,13 +4902,13 @@
     </row>
     <row r="111" spans="1:10">
       <c r="A111" s="1">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>260</v>
@@ -4925,13 +4917,13 @@
         <v>261</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>262</v>
+        <v>14</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>286</v>
+        <v>158</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I111" s="1" t="s">
         <v>14</v>
@@ -4942,13 +4934,13 @@
     </row>
     <row r="112" spans="1:10">
       <c r="A112" s="1">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>263</v>
@@ -4974,19 +4966,19 @@
     </row>
     <row r="113" spans="1:10">
       <c r="A113" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C113" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D113" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D113" s="1" t="s">
+      <c r="E113" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>267</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>14</v>
@@ -5006,25 +4998,25 @@
     </row>
     <row r="114" spans="1:10">
       <c r="A114" s="1">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D114" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E114" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="E114" s="1" t="s">
-        <v>269</v>
-      </c>
       <c r="F114" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>158</v>
+        <v>52</v>
       </c>
       <c r="H114" s="1" t="s">
         <v>64</v>
@@ -5036,40 +5028,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
-      <c r="A115" s="1">
-        <v>114</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G115" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H115" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I115" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J115" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:M115" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}"/>
+  <autoFilter ref="A1:M114" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
changed to currency and tonnes / M Revenue for most fields. Regenerated sfdr framework
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
+++ b/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dataland\Dataland\dataland-framework-toolbox\inputs\sfdr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d60171\GitHub\Dataland\dataland-framework-toolbox\inputs\sfdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF609C33-5D67-4DBB-AB43-1A7E0F61F9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140BAF2A-A8FD-4384-BAA0-12636DDF344E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="2" r:id="rId1"/>
@@ -239,9 +239,6 @@
     <t>Carbon footprint</t>
   </si>
   <si>
-    <t>Tonnes / €M Revenue</t>
-  </si>
-  <si>
     <t>GHG intensity</t>
   </si>
   <si>
@@ -647,9 +644,6 @@
     <t>Average amount in cubic meters of fresh water used per million EUR revenue</t>
   </si>
   <si>
-    <t>Cubic Meters / €M Revenue</t>
-  </si>
-  <si>
     <t>Water Management Policy</t>
   </si>
   <si>
@@ -1029,6 +1023,12 @@
   </si>
   <si>
     <t>Tonnes of Scope 3 GHG emissions / million of the revenue (in the same currency as the total revenue). Scope 3 carbon emissions, i.e. all indirect upstream and downstream emissions that are not included in scope 2</t>
+  </si>
+  <si>
+    <t>Tonnes / M Revenue</t>
+  </si>
+  <si>
+    <t>Cubic Meters / M Revenue</t>
   </si>
 </sst>
 </file>
@@ -1464,26 +1464,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}">
   <dimension ref="A1:M115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.81640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="61.6328125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="61.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="79" style="3" customWidth="1"/>
-    <col min="7" max="7" width="39.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.36328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.08984375" style="3"/>
+    <col min="14" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -1538,10 +1538,10 @@
         <v>13</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>14</v>
@@ -1911,10 +1911,10 @@
         <v>28</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
@@ -1939,10 +1939,10 @@
         <v>28</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
@@ -1997,10 +1997,10 @@
         <v>28</v>
       </c>
       <c r="D17" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>278</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>280</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
@@ -2025,10 +2025,10 @@
         <v>28</v>
       </c>
       <c r="D18" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>279</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>281</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
@@ -2053,10 +2053,10 @@
         <v>28</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>14</v>
@@ -2142,17 +2142,17 @@
         <v>55</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
-        <v>56</v>
+        <v>318</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>33</v>
@@ -2169,20 +2169,20 @@
         <v>28</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1" t="s">
-        <v>56</v>
+        <v>318</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>33</v>
@@ -2199,18 +2199,18 @@
         <v>28</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1" t="s">
-        <v>56</v>
+        <v>318</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>33</v>
@@ -2227,18 +2227,18 @@
         <v>28</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1" t="s">
-        <v>56</v>
+        <v>318</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>33</v>
@@ -2255,18 +2255,18 @@
         <v>28</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1" t="s">
-        <v>56</v>
+        <v>318</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>33</v>
@@ -2283,18 +2283,18 @@
         <v>28</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1" t="s">
-        <v>56</v>
+        <v>318</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>33</v>
@@ -2311,16 +2311,16 @@
         <v>28</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="G28" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>14</v>
@@ -2341,10 +2341,10 @@
         <v>28</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="7" t="s">
@@ -2352,7 +2352,7 @@
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J29" s="7" t="s">
         <v>33</v>
@@ -2369,10 +2369,10 @@
         <v>28</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="7" t="s">
@@ -2380,7 +2380,7 @@
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J30" s="7" t="s">
         <v>33</v>
@@ -2394,23 +2394,23 @@
         <v>27</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H31" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>33</v>
@@ -2424,23 +2424,23 @@
         <v>27</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>33</v>
@@ -2454,13 +2454,13 @@
         <v>27</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>14</v>
@@ -2469,10 +2469,10 @@
         <v>31</v>
       </c>
       <c r="H33" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>33</v>
@@ -2486,13 +2486,13 @@
         <v>27</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>14</v>
@@ -2501,10 +2501,10 @@
         <v>31</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>33</v>
@@ -2518,13 +2518,13 @@
         <v>27</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>14</v>
@@ -2533,10 +2533,10 @@
         <v>31</v>
       </c>
       <c r="H35" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>33</v>
@@ -2550,13 +2550,13 @@
         <v>27</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D36" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>14</v>
@@ -2565,10 +2565,10 @@
         <v>31</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>33</v>
@@ -2582,19 +2582,19 @@
         <v>27</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D37" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>14</v>
@@ -2614,23 +2614,23 @@
         <v>27</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D38" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H38" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>33</v>
@@ -2644,19 +2644,19 @@
         <v>27</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="G39" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>14</v>
@@ -2676,19 +2676,19 @@
         <v>27</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="G40" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>14</v>
@@ -2708,19 +2708,19 @@
         <v>27</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="G41" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>14</v>
@@ -2740,19 +2740,19 @@
         <v>27</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="G42" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>14</v>
@@ -2772,13 +2772,13 @@
         <v>27</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>14</v>
@@ -2787,7 +2787,7 @@
         <v>31</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>32</v>
@@ -2804,20 +2804,20 @@
         <v>27</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>32</v>
@@ -2831,22 +2831,22 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="G45" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>14</v>
@@ -2863,22 +2863,22 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D46" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="G46" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>14</v>
@@ -2895,22 +2895,22 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D47" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="G47" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>14</v>
@@ -2927,22 +2927,22 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D48" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="G48" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>14</v>
@@ -2959,22 +2959,22 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D49" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="G49" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>14</v>
@@ -2991,22 +2991,22 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D50" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E50" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="G50" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>14</v>
@@ -3023,22 +3023,22 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D51" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="G51" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>14</v>
@@ -3055,22 +3055,22 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D52" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="F52" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="G52" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>14</v>
@@ -3087,22 +3087,22 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D53" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="G53" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>14</v>
@@ -3119,22 +3119,22 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D54" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E54" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="F54" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>14</v>
@@ -3151,22 +3151,22 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D55" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F55" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="G55" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>14</v>
@@ -3183,22 +3183,22 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D56" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="F56" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F56" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="G56" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>14</v>
@@ -3215,22 +3215,22 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D57" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F57" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="G57" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>14</v>
@@ -3247,22 +3247,22 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D58" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="F58" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F58" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="G58" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>14</v>
@@ -3279,22 +3279,22 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D59" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E59" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="G59" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>14</v>
@@ -3311,22 +3311,22 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D60" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="F60" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F60" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="G60" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>14</v>
@@ -3343,22 +3343,22 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D61" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="F61" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F61" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="G61" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>14</v>
@@ -3375,16 +3375,16 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D62" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>14</v>
@@ -3393,7 +3393,7 @@
         <v>52</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>14</v>
@@ -3407,16 +3407,16 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D63" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>14</v>
@@ -3425,7 +3425,7 @@
         <v>52</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I63" s="1" t="s">
         <v>14</v>
@@ -3439,16 +3439,16 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D64" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>14</v>
@@ -3458,7 +3458,7 @@
       </c>
       <c r="H64" s="1"/>
       <c r="I64" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J64" s="1" t="s">
         <v>33</v>
@@ -3469,23 +3469,23 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D65" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I65" s="1"/>
       <c r="J65" s="1" t="s">
@@ -3497,23 +3497,23 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D66" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I66" s="1"/>
       <c r="J66" s="1" t="s">
@@ -3525,23 +3525,23 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D67" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I67" s="1"/>
       <c r="J67" s="1" t="s">
@@ -3553,23 +3553,23 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D68" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I68" s="1"/>
       <c r="J68" s="1" t="s">
@@ -3581,26 +3581,26 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D69" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J69" s="1" t="s">
         <v>33</v>
@@ -3611,26 +3611,26 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D70" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>33</v>
@@ -3641,22 +3641,22 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D71" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E71" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E71" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="F71" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>14</v>
@@ -3676,20 +3676,20 @@
         <v>27</v>
       </c>
       <c r="C72" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D72" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="E72" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I72" s="1" t="s">
         <v>32</v>
@@ -3706,20 +3706,20 @@
         <v>27</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D73" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E73" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I73" s="1" t="s">
         <v>32</v>
@@ -3736,20 +3736,20 @@
         <v>27</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D74" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E74" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>32</v>
@@ -3766,19 +3766,19 @@
         <v>27</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D75" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E75" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="F75" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="F75" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="G75" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>14</v>
@@ -3798,13 +3798,13 @@
         <v>27</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D76" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E76" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>14</v>
@@ -3813,10 +3813,10 @@
         <v>31</v>
       </c>
       <c r="H76" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I76" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="I76" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="J76" s="1" t="s">
         <v>33</v>
@@ -3830,13 +3830,13 @@
         <v>27</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D77" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E77" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>14</v>
@@ -3845,10 +3845,10 @@
         <v>31</v>
       </c>
       <c r="H77" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I77" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="I77" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="J77" s="1" t="s">
         <v>33</v>
@@ -3862,13 +3862,13 @@
         <v>27</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D78" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>14</v>
@@ -3877,10 +3877,10 @@
         <v>31</v>
       </c>
       <c r="H78" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I78" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="I78" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="J78" s="1" t="s">
         <v>33</v>
@@ -3894,13 +3894,13 @@
         <v>27</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D79" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E79" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>14</v>
@@ -3909,10 +3909,10 @@
         <v>31</v>
       </c>
       <c r="H79" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I79" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="I79" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="J79" s="1" t="s">
         <v>33</v>
@@ -3926,13 +3926,13 @@
         <v>27</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D80" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E80" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>14</v>
@@ -3941,10 +3941,10 @@
         <v>31</v>
       </c>
       <c r="H80" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I80" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="I80" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="J80" s="1" t="s">
         <v>33</v>
@@ -3958,13 +3958,13 @@
         <v>27</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D81" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E81" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>14</v>
@@ -3973,10 +3973,10 @@
         <v>31</v>
       </c>
       <c r="H81" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I81" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="I81" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="J81" s="1" t="s">
         <v>33</v>
@@ -3990,13 +3990,13 @@
         <v>27</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D82" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E82" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>14</v>
@@ -4005,10 +4005,10 @@
         <v>31</v>
       </c>
       <c r="H82" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I82" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="I82" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="J82" s="1" t="s">
         <v>33</v>
@@ -4022,13 +4022,13 @@
         <v>27</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D83" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>14</v>
@@ -4037,10 +4037,10 @@
         <v>31</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J83" s="1" t="s">
         <v>33</v>
@@ -4054,13 +4054,13 @@
         <v>27</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D84" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E84" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>14</v>
@@ -4069,10 +4069,10 @@
         <v>31</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J84" s="1" t="s">
         <v>33</v>
@@ -4086,25 +4086,25 @@
         <v>27</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D85" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E85" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E85" s="1" t="s">
-        <v>191</v>
-      </c>
       <c r="F85" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>192</v>
+        <v>319</v>
       </c>
       <c r="J85" s="1" t="s">
         <v>33</v>
@@ -4118,19 +4118,19 @@
         <v>27</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D86" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F86" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E86" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>195</v>
-      </c>
       <c r="G86" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>14</v>
@@ -4150,19 +4150,19 @@
         <v>27</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D87" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F87" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E87" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>198</v>
-      </c>
       <c r="G87" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>14</v>
@@ -4182,19 +4182,19 @@
         <v>27</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D88" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F88" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E88" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="G88" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>14</v>
@@ -4214,19 +4214,19 @@
         <v>27</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D89" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F89" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E89" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>204</v>
-      </c>
       <c r="G89" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>14</v>
@@ -4246,19 +4246,19 @@
         <v>27</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D90" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F90" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E90" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="G90" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>14</v>
@@ -4278,19 +4278,19 @@
         <v>27</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D91" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F91" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E91" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="G91" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>14</v>
@@ -4310,13 +4310,13 @@
         <v>27</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>14</v>
@@ -4325,7 +4325,7 @@
         <v>31</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I92" s="1" t="s">
         <v>32</v>
@@ -4342,19 +4342,19 @@
         <v>27</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D93" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F93" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E93" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>215</v>
-      </c>
       <c r="G93" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>14</v>
@@ -4374,19 +4374,19 @@
         <v>27</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D94" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F94" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E94" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>218</v>
-      </c>
       <c r="G94" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>14</v>
@@ -4406,19 +4406,19 @@
         <v>27</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D95" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F95" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E95" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="G95" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>14</v>
@@ -4435,22 +4435,22 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C96" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E96" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="F96" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="E96" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>225</v>
-      </c>
       <c r="G96" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>14</v>
@@ -4467,22 +4467,22 @@
         <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D97" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F97" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="E97" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>228</v>
-      </c>
       <c r="G97" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>14</v>
@@ -4499,16 +4499,16 @@
         <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C98" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D98" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>14</v>
@@ -4517,10 +4517,10 @@
         <v>31</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J98" s="1" t="s">
         <v>33</v>
@@ -4531,16 +4531,16 @@
         <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C99" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C99" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D99" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>14</v>
@@ -4549,10 +4549,10 @@
         <v>31</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J99" s="1" t="s">
         <v>33</v>
@@ -4563,22 +4563,22 @@
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C100" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D100" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F100" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="E100" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>235</v>
-      </c>
       <c r="G100" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>14</v>
@@ -4595,22 +4595,22 @@
         <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D101" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F101" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E101" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>238</v>
-      </c>
       <c r="G101" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>14</v>
@@ -4627,22 +4627,22 @@
         <v>101</v>
       </c>
       <c r="B102" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D102" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F102" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E102" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>241</v>
-      </c>
       <c r="G102" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>14</v>
@@ -4659,25 +4659,25 @@
         <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C103" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D103" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I103" s="1" t="s">
         <v>14</v>
@@ -4691,25 +4691,25 @@
         <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C104" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D104" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I104" s="1" t="s">
         <v>14</v>
@@ -4723,16 +4723,16 @@
         <v>104</v>
       </c>
       <c r="B105" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C105" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D105" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>14</v>
@@ -4741,7 +4741,7 @@
         <v>31</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I105" s="1" t="s">
         <v>14</v>
@@ -4755,16 +4755,16 @@
         <v>105</v>
       </c>
       <c r="B106" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C106" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D106" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>14</v>
@@ -4773,10 +4773,10 @@
         <v>31</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J106" s="1" t="s">
         <v>33</v>
@@ -4787,22 +4787,22 @@
         <v>106</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C107" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F107" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D107" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>252</v>
-      </c>
       <c r="G107" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H107" s="1" t="s">
         <v>14</v>
@@ -4819,22 +4819,22 @@
         <v>107</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D108" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F108" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="E108" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>255</v>
-      </c>
       <c r="G108" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H108" s="1" t="s">
         <v>14</v>
@@ -4851,22 +4851,22 @@
         <v>108</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D109" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F109" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="E109" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="G109" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H109" s="1" t="s">
         <v>14</v>
@@ -4883,22 +4883,22 @@
         <v>109</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D110" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F110" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="E110" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>261</v>
-      </c>
       <c r="G110" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H110" s="1" t="s">
         <v>14</v>
@@ -4915,22 +4915,22 @@
         <v>110</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D111" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F111" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="E111" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="F111" s="1" t="s">
-        <v>264</v>
-      </c>
       <c r="G111" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H111" s="1" t="s">
         <v>14</v>
@@ -4947,25 +4947,25 @@
         <v>111</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I112" s="1" t="s">
         <v>14</v>
@@ -4979,25 +4979,25 @@
         <v>112</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C113" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E113" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="D113" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>269</v>
-      </c>
       <c r="F113" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I113" s="1" t="s">
         <v>14</v>
@@ -5011,25 +5011,25 @@
         <v>113</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I114" s="1" t="s">
         <v>14</v>
@@ -5043,16 +5043,16 @@
         <v>114</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>14</v>
@@ -5061,7 +5061,7 @@
         <v>52</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I115" s="1" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
DALA-5108 Update to SFDR data model Issues 2-5 (#876)
---------

Co-authored-by: SiegfriedSobkowiak <71646830+SiegfriedSobkowiak@users.noreply.github.com>
Co-authored-by: Dennis Groh <173401487+dennis-dfine@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
+++ b/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dataland\Dataland\dataland-framework-toolbox\inputs\sfdr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d60171\GitHub\Dataland\dataland-framework-toolbox\inputs\sfdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF609C33-5D67-4DBB-AB43-1A7E0F61F9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E97675-B968-4D74-A5E2-BD63B1AC6CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$M$115</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Framework Data Model'!$A$1:$M$114</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
     <definedName name="IQ_CY">10000</definedName>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="318">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -593,9 +593,6 @@
     <t>Non-Renewable Energy Consumption Crude Oil</t>
   </si>
   <si>
-    <t>Energy consumption from crude oil (non-renewable energy source)</t>
-  </si>
-  <si>
     <t>Non-Renewable Energy Consumption Natural Gas</t>
   </si>
   <si>
@@ -764,9 +761,6 @@
     <t>Workdays Lost</t>
   </si>
   <si>
-    <t>Number of workdays lost to injuries, accidents, fatalities or illness</t>
-  </si>
-  <si>
     <t>Days</t>
   </si>
   <si>
@@ -809,18 +803,9 @@
     <t>Number of discrimination related incidents reported that lead to any kind of penalty and/or fine</t>
   </si>
   <si>
-    <t>CEO to Employee Pay Gap Ratio</t>
-  </si>
-  <si>
-    <t>Annual total compensation for the highest compensated individual divided by the median annual total compensation for all employees (excluding the highest-compensated individual).</t>
-  </si>
-  <si>
     <t>Excessive CEO pay ratio</t>
   </si>
   <si>
-    <t>Average ratio of the annual total compensation for the highest compensated individual to the median annual total compensation for all employees (excluding the highest-compensated individual)</t>
-  </si>
-  <si>
     <t>Human rights</t>
   </si>
   <si>
@@ -1029,6 +1014,15 @@
   </si>
   <si>
     <t>Tonnes of Scope 3 GHG emissions / million of the revenue (in the same currency as the total revenue). Scope 3 carbon emissions, i.e. all indirect upstream and downstream emissions that are not included in scope 2</t>
+  </si>
+  <si>
+    <t>Energy consumption from crude oil (including petrol, diesel, fuel oil and others) (non-renewable energy source)</t>
+  </si>
+  <si>
+    <t>Number of workdays lost to injuries, accidents, fatalities or illness in total</t>
+  </si>
+  <si>
+    <t>Annual total compensation for the highest compensated individual divided by the median annual total compensation for all employees (excluding the highest-compensated individual)</t>
   </si>
 </sst>
 </file>
@@ -1462,28 +1456,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}">
-  <dimension ref="A1:M115"/>
+  <dimension ref="A1:M114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.81640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="61.6328125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="61.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="79" style="3" customWidth="1"/>
-    <col min="7" max="7" width="39.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.36328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.08984375" style="3"/>
+    <col min="14" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -1538,10 +1532,10 @@
         <v>13</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>14</v>
@@ -1911,10 +1905,10 @@
         <v>28</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
@@ -1939,10 +1933,10 @@
         <v>28</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
@@ -1997,10 +1991,10 @@
         <v>28</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
@@ -2025,10 +2019,10 @@
         <v>28</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
@@ -2053,10 +2047,10 @@
         <v>28</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>14</v>
@@ -2142,7 +2136,7 @@
         <v>55</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>14</v>
@@ -2172,7 +2166,7 @@
         <v>57</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>14</v>
@@ -2199,10 +2193,10 @@
         <v>28</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
@@ -2227,10 +2221,10 @@
         <v>28</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
@@ -2255,10 +2249,10 @@
         <v>28</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
@@ -2283,10 +2277,10 @@
         <v>28</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
@@ -2320,7 +2314,7 @@
         <v>60</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>14</v>
@@ -2341,10 +2335,10 @@
         <v>28</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="7" t="s">
@@ -2352,7 +2346,7 @@
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="7" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="J29" s="7" t="s">
         <v>33</v>
@@ -2369,10 +2363,10 @@
         <v>28</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="7" t="s">
@@ -2380,7 +2374,7 @@
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="7" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="J30" s="7" t="s">
         <v>33</v>
@@ -2656,7 +2650,7 @@
         <v>86</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>14</v>
@@ -2688,7 +2682,7 @@
         <v>89</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>14</v>
@@ -2720,7 +2714,7 @@
         <v>92</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>14</v>
@@ -2752,7 +2746,7 @@
         <v>95</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>14</v>
@@ -2846,7 +2840,7 @@
         <v>106</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>14</v>
@@ -2878,7 +2872,7 @@
         <v>109</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>14</v>
@@ -2910,7 +2904,7 @@
         <v>112</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>14</v>
@@ -2942,7 +2936,7 @@
         <v>115</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>14</v>
@@ -2974,7 +2968,7 @@
         <v>118</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>14</v>
@@ -3000,13 +2994,13 @@
         <v>119</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>14</v>
@@ -3038,7 +3032,7 @@
         <v>123</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>14</v>
@@ -3070,7 +3064,7 @@
         <v>126</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>14</v>
@@ -3102,7 +3096,7 @@
         <v>129</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>14</v>
@@ -3131,10 +3125,10 @@
         <v>131</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>14</v>
@@ -3166,7 +3160,7 @@
         <v>134</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>14</v>
@@ -3198,7 +3192,7 @@
         <v>137</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>14</v>
@@ -3230,7 +3224,7 @@
         <v>140</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>14</v>
@@ -3262,7 +3256,7 @@
         <v>143</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>14</v>
@@ -3288,13 +3282,13 @@
         <v>144</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>145</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>14</v>
@@ -3326,7 +3320,7 @@
         <v>148</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>14</v>
@@ -3358,7 +3352,7 @@
         <v>151</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>14</v>
@@ -3475,10 +3469,10 @@
         <v>103</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
@@ -3503,10 +3497,10 @@
         <v>103</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
@@ -3531,10 +3525,10 @@
         <v>103</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
@@ -3559,10 +3553,10 @@
         <v>103</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
@@ -3587,10 +3581,10 @@
         <v>103</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
@@ -3617,10 +3611,10 @@
         <v>103</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
@@ -3656,7 +3650,7 @@
         <v>14</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>14</v>
@@ -3682,7 +3676,7 @@
         <v>163</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1" t="s">
@@ -3778,7 +3772,7 @@
         <v>170</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>14</v>
@@ -3836,7 +3830,7 @@
         <v>173</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>174</v>
+        <v>315</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>14</v>
@@ -3865,10 +3859,10 @@
         <v>61</v>
       </c>
       <c r="D78" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>14</v>
@@ -3897,10 +3891,10 @@
         <v>61</v>
       </c>
       <c r="D79" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E79" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>14</v>
@@ -3929,10 +3923,10 @@
         <v>61</v>
       </c>
       <c r="D80" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E80" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>14</v>
@@ -3961,10 +3955,10 @@
         <v>61</v>
       </c>
       <c r="D81" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E81" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>14</v>
@@ -3993,10 +3987,10 @@
         <v>61</v>
       </c>
       <c r="D82" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E82" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>14</v>
@@ -4025,10 +4019,10 @@
         <v>96</v>
       </c>
       <c r="D83" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>14</v>
@@ -4040,7 +4034,7 @@
         <v>64</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J83" s="1" t="s">
         <v>33</v>
@@ -4057,10 +4051,10 @@
         <v>96</v>
       </c>
       <c r="D84" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E84" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>14</v>
@@ -4072,7 +4066,7 @@
         <v>64</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J84" s="1" t="s">
         <v>33</v>
@@ -4089,10 +4083,10 @@
         <v>96</v>
       </c>
       <c r="D85" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E85" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>14</v>
@@ -4104,7 +4098,7 @@
         <v>64</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J85" s="1" t="s">
         <v>33</v>
@@ -4121,16 +4115,16 @@
         <v>96</v>
       </c>
       <c r="D86" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E86" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E86" s="1" t="s">
+      <c r="F86" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="F86" s="1" t="s">
-        <v>195</v>
-      </c>
       <c r="G86" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>14</v>
@@ -4153,16 +4147,16 @@
         <v>96</v>
       </c>
       <c r="D87" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E87" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E87" s="1" t="s">
+      <c r="F87" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="F87" s="1" t="s">
-        <v>198</v>
-      </c>
       <c r="G87" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>14</v>
@@ -4185,16 +4179,16 @@
         <v>83</v>
       </c>
       <c r="D88" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E88" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="F88" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="F88" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="G88" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>14</v>
@@ -4217,16 +4211,16 @@
         <v>83</v>
       </c>
       <c r="D89" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E89" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E89" s="1" t="s">
+      <c r="F89" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="F89" s="1" t="s">
-        <v>204</v>
-      </c>
       <c r="G89" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>14</v>
@@ -4249,16 +4243,16 @@
         <v>83</v>
       </c>
       <c r="D90" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E90" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E90" s="1" t="s">
+      <c r="F90" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="F90" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="G90" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>14</v>
@@ -4281,16 +4275,16 @@
         <v>83</v>
       </c>
       <c r="D91" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E91" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="F91" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="F91" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="G91" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>14</v>
@@ -4313,10 +4307,10 @@
         <v>99</v>
       </c>
       <c r="D92" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E92" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>14</v>
@@ -4345,16 +4339,16 @@
         <v>83</v>
       </c>
       <c r="D93" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E93" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E93" s="1" t="s">
+      <c r="F93" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="F93" s="1" t="s">
-        <v>215</v>
-      </c>
       <c r="G93" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>14</v>
@@ -4377,16 +4371,16 @@
         <v>83</v>
       </c>
       <c r="D94" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E94" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E94" s="1" t="s">
+      <c r="F94" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F94" s="1" t="s">
-        <v>218</v>
-      </c>
       <c r="G94" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>14</v>
@@ -4409,16 +4403,16 @@
         <v>83</v>
       </c>
       <c r="D95" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E95" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E95" s="1" t="s">
+      <c r="F95" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F95" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="G95" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>14</v>
@@ -4438,19 +4432,19 @@
         <v>102</v>
       </c>
       <c r="C96" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="E96" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="E96" s="1" t="s">
+      <c r="F96" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="F96" s="1" t="s">
-        <v>225</v>
-      </c>
       <c r="G96" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>14</v>
@@ -4473,16 +4467,16 @@
         <v>103</v>
       </c>
       <c r="D97" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E97" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="E97" s="1" t="s">
+      <c r="F97" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="F97" s="1" t="s">
-        <v>228</v>
-      </c>
       <c r="G97" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>14</v>
@@ -4505,10 +4499,10 @@
         <v>103</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>14</v>
@@ -4517,11 +4511,9 @@
         <v>31</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I98" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="I98" s="1"/>
       <c r="J98" s="1" t="s">
         <v>33</v>
       </c>
@@ -4537,10 +4529,10 @@
         <v>103</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>231</v>
+        <v>316</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>14</v>
@@ -4552,7 +4544,7 @@
         <v>64</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J99" s="1" t="s">
         <v>33</v>
@@ -4569,16 +4561,16 @@
         <v>103</v>
       </c>
       <c r="D100" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F100" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="E100" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>235</v>
-      </c>
       <c r="G100" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>14</v>
@@ -4601,16 +4593,16 @@
         <v>103</v>
       </c>
       <c r="D101" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F101" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E101" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>238</v>
-      </c>
       <c r="G101" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>14</v>
@@ -4633,16 +4625,16 @@
         <v>103</v>
       </c>
       <c r="D102" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F102" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E102" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>241</v>
-      </c>
       <c r="G102" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>14</v>
@@ -4665,10 +4657,10 @@
         <v>103</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>14</v>
@@ -4697,10 +4689,10 @@
         <v>103</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>14</v>
@@ -4720,7 +4712,7 @@
     </row>
     <row r="105" spans="1:10">
       <c r="A105" s="1">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>102</v>
@@ -4729,10 +4721,10 @@
         <v>103</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>247</v>
+        <v>317</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>14</v>
@@ -4743,40 +4735,38 @@
       <c r="H105" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I105" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="I105" s="1"/>
       <c r="J105" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="106" spans="1:10">
       <c r="A106" s="1">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>246</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>249</v>
+        <v>271</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>14</v>
+        <v>247</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>31</v>
+        <v>283</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="J106" s="1" t="s">
         <v>33</v>
@@ -4784,25 +4774,25 @@
     </row>
     <row r="107" spans="1:10">
       <c r="A107" s="1">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C107" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F107" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D107" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>252</v>
-      </c>
       <c r="G107" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H107" s="1" t="s">
         <v>14</v>
@@ -4816,25 +4806,25 @@
     </row>
     <row r="108" spans="1:10">
       <c r="A108" s="1">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="D108" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F108" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="E108" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>255</v>
-      </c>
       <c r="G108" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H108" s="1" t="s">
         <v>14</v>
@@ -4848,25 +4838,25 @@
     </row>
     <row r="109" spans="1:10">
       <c r="A109" s="1">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D109" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F109" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="E109" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="G109" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H109" s="1" t="s">
         <v>14</v>
@@ -4880,25 +4870,25 @@
     </row>
     <row r="110" spans="1:10">
       <c r="A110" s="1">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D110" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F110" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="E110" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>261</v>
-      </c>
       <c r="G110" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H110" s="1" t="s">
         <v>14</v>
@@ -4912,28 +4902,28 @@
     </row>
     <row r="111" spans="1:10">
       <c r="A111" s="1">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>264</v>
+        <v>14</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>288</v>
+        <v>158</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="I111" s="1" t="s">
         <v>14</v>
@@ -4944,19 +4934,19 @@
     </row>
     <row r="112" spans="1:10">
       <c r="A112" s="1">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>14</v>
@@ -4976,19 +4966,19 @@
     </row>
     <row r="113" spans="1:10">
       <c r="A113" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>14</v>
@@ -5008,25 +4998,25 @@
     </row>
     <row r="114" spans="1:10">
       <c r="A114" s="1">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C114" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D114" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="D114" s="1" t="s">
-        <v>270</v>
-      </c>
       <c r="E114" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>158</v>
+        <v>52</v>
       </c>
       <c r="H114" s="1" t="s">
         <v>64</v>
@@ -5038,40 +5028,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
-      <c r="A115" s="1">
-        <v>114</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G115" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H115" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I115" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J115" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:M115" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}"/>
+  <autoFilter ref="A1:M114" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update tests using the edit functionality
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
+++ b/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dataland\Dataland\dataland-framework-toolbox\inputs\sfdr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dataland\datalandClean\dataland-framework-toolbox\inputs\sfdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95FC28A-9700-442A-B6AE-A3715804F48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9301C896-2570-46B3-BA20-F045C89CA158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
+    <workbookView xWindow="19090" yWindow="-10800" windowWidth="38620" windowHeight="21220" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="2" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="275">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -212,9 +212,6 @@
     <t>Fossil Fuel Sector Exposure</t>
   </si>
   <si>
-    <t>(Part of) revenues derived from exploration, mining, extraction, production, processing, storage, refining or distribution, including transportation, storage and trade, of fossil fuels as defined in Article 2, point (62), of Regulation (EU) 2018/1999 of the European Parliament and of the Council? See also Regulation, Annex I, top (5).</t>
-  </si>
-  <si>
     <t>Energy performance</t>
   </si>
   <si>
@@ -251,9 +248,6 @@
     <t>Applicable High Impact Climate Sectors</t>
   </si>
   <si>
-    <t>Sector applicable activities</t>
-  </si>
-  <si>
     <t>Custom - SFDR High Impact Climate Sectors</t>
   </si>
   <si>
@@ -266,27 +260,15 @@
     <t>Primary Forest And Wooded Land Of Native Species Exposure</t>
   </si>
   <si>
-    <t>Sites/operations (partly) located in or near to primary forest and other wooded areas where activities of those sites/operations negatively affect those areas? See also Regulation, Annex I, table 1, indicator nr. 7).</t>
-  </si>
-  <si>
     <t>Protected Areas Exposure</t>
   </si>
   <si>
-    <t>Sites/operations (partly) located in or near protected areas where activities of those sites/operations negatively affect those areas? See also Regulation, Annex I, table 1, indicator nr. 7).</t>
-  </si>
-  <si>
     <t>Rare Or Endangered Ecosystems Exposure</t>
   </si>
   <si>
-    <t>Sites/operations in or near areas designated for the protection of species (including flora and fauna) and where the activities of those sites/operations lead to the deterioration of natural habitats and the habitats of those species and disturb the species for which the protected area has been designated? See also Regulation, Annex I, table 1, indicator nr. 7 and Annex I, definition 18(a).</t>
-  </si>
-  <si>
     <t>Highly Biodiverse Grassland Exposure</t>
   </si>
   <si>
-    <t>Sites/operations (partly) located in highly biodiverse grassland that is: (i) natural, namely, grassland that would remain grassland in the absence of human intervention and which maintains the natural species composition and ecological characteristics and processes; or (ii) non-natural, namely, grassland that would cease to be grassland in the absence of human intervention and which is species-rich and not degraded, unless evidence is provided that the harvesting of the raw material is necessary to preserve its grassland status?</t>
-  </si>
-  <si>
     <t>Water</t>
   </si>
   <si>
@@ -308,123 +290,75 @@
     <t>Human Rights Legal Proceedings</t>
   </si>
   <si>
-    <t>Involvement in Human Rights related legal proceedings</t>
-  </si>
-  <si>
     <t>ILO Core Labour Standards</t>
   </si>
   <si>
-    <t>Abidance by the ILO Core Labour Standards</t>
-  </si>
-  <si>
     <t>Environmental Policy</t>
   </si>
   <si>
-    <t>Existence of an environmental policy</t>
-  </si>
-  <si>
     <t>Corruption Legal Proceedings</t>
   </si>
   <si>
-    <t>Involvement in corruption-related legal proceedings</t>
-  </si>
-  <si>
     <t>Transparency Disclosure Policy</t>
   </si>
   <si>
     <t>Do you have a transparency policy? If yes, please share the policy with us. According to the OECD Guidelines for Multinational Enterprises, multinational companies should inform the public not only about their financial performance, but also about all of the important aspects of their business activities, such as how they are meeting social and environmental standards and what risks they foresee linked to their business activities.</t>
   </si>
   <si>
-    <t>Existence of a transparency policy. According to the OECD Guidelines for Multinational Enterprises, multinational companies should inform the public not only about their financial performance, but also about all of the important aspects of their business activities, such as how they are meeting social and environmental standards and what risks they foresee linked to their business activities.</t>
-  </si>
-  <si>
     <t>Human Rights Due Diligence Policy</t>
   </si>
   <si>
-    <t>Policies in place to support/respect human rights and conduct due diligence to ensure that business activities do not have a negative human rights impact.</t>
-  </si>
-  <si>
     <t>Policy against Child Labour</t>
   </si>
   <si>
     <t>Do you have policies in place to abolish all forms of child labour? If yes, please share the policy with us.</t>
   </si>
   <si>
-    <t>Policies in place to abolish all forms of child labour.</t>
-  </si>
-  <si>
     <t>Policy against Forced Labour</t>
   </si>
   <si>
     <t>Do you have policies in place to abolish all forms of forced labour? If yes, please share the policy with us.</t>
   </si>
   <si>
-    <t>Policies in place to abolish all forms of forced labour.</t>
-  </si>
-  <si>
     <t>Policy against Discrimination in the Workplace</t>
   </si>
   <si>
     <t>Do you have policies in place to eliminate discrimination in the workplace? If yes, please share the policy with us.</t>
   </si>
   <si>
-    <t>Policies in place to eliminate discrimination in the workplace.</t>
-  </si>
-  <si>
     <t>ISO 14001 Certificate</t>
   </si>
   <si>
     <t>Policy against Bribery and Corruption</t>
   </si>
   <si>
-    <t>Existence of a policy on anti-corruption and anti-bribery consistent with the United Nations Convention against Corruption.</t>
-  </si>
-  <si>
     <t>Fair Business Marketing Advertising Policy</t>
   </si>
   <si>
     <t>Do you have policies and procedures in place to apply fair business, marketing and advertising practices and to guarantee the safety and quality of the goods and services? If yes, please share the relevant documents with us.</t>
   </si>
   <si>
-    <t>Policies and procedures in place to apply fair business, marketing, and advertising practices and ensure the safety and quality of goods and services.</t>
-  </si>
-  <si>
     <t>Technologies Expertise Transfer Policy</t>
   </si>
   <si>
     <t>Do you have policies and procedures in place to permit the transfer and rapid dissemination of technologies and expertise? If yes, please share the relevant documents with us.</t>
   </si>
   <si>
-    <t>Policies and procedures in place to permit the transfer and rapid dissemination of technologies and expertise</t>
-  </si>
-  <si>
     <t>Fair Competition Policy</t>
   </si>
   <si>
     <t>Do you have policies and procedures in place related to fair competition and anti-competitive cartels? If yes, please share the relevant documents with us.</t>
   </si>
   <si>
-    <t>Policies and procedures in place related to fair competition and anti-competitive cartels</t>
-  </si>
-  <si>
     <t>Violation Of Tax Rules And Regulation</t>
   </si>
   <si>
-    <t>Involvement in a violation of OECD Guidelines for Multinational Enterprises for Taxation: In the field of taxation, multinational enterprises should make their contribution to public finances within the framework of applicable law and regulations, in accordance with the tax rules and regulations of the host countries, and should cooperate with the tax authorities.</t>
-  </si>
-  <si>
     <t>UN Global Compact Principles Compliance Policy</t>
   </si>
   <si>
-    <t>Existence of a policy to monitor compliance with the UNGC principles or OECD Guidelines for Multinational Enterprises</t>
-  </si>
-  <si>
     <t>OECD Guidelines For Multinational Enterprises Grievance Handling</t>
   </si>
   <si>
-    <t>Existence of grievance/complaints handling mechanisms to address violations of the UNGC principles or OECD Guidelines for Multinational Enterprises</t>
-  </si>
-  <si>
     <t>Average Gross Hourly Earnings Male Employees</t>
   </si>
   <si>
@@ -464,9 +398,6 @@
     <t>Carbon Reduction Initiatives</t>
   </si>
   <si>
-    <t>Existence of policies or procedures for carbon emission reduction aimed at aligning with the Paris Agreement</t>
-  </si>
-  <si>
     <t>Non-Renewable Energy Consumption Fossil Fuels</t>
   </si>
   <si>
@@ -506,60 +437,33 @@
     <t>Water Management Policy</t>
   </si>
   <si>
-    <t>Existence of policies and procedures for water management</t>
-  </si>
-  <si>
     <t>High Water Stress Area Exposure</t>
   </si>
   <si>
-    <t>Sites (partly) located in "areas of high water stress", i.e. regions where the percentage of total water withdrawn is high (60%) or extremely high (80%), without a water management policy</t>
-  </si>
-  <si>
     <t>Manufacture Of Agrochemical Pesticides Products</t>
   </si>
   <si>
-    <t>Involvement in manufacture of pesticides and other agrochemical products</t>
-  </si>
-  <si>
     <t>Land Degradation Desertification Soil Sealing Exposure</t>
   </si>
   <si>
-    <t>Involvement in activities, which cause land degradation, desertification or soil sealing</t>
-  </si>
-  <si>
     <t>Sustainable Agriculture Policy</t>
   </si>
   <si>
-    <t>Sustainable land/agriculture practices or policies</t>
-  </si>
-  <si>
     <t>Sustainable Oceans And Seas Policy</t>
   </si>
   <si>
-    <t>Sustainable oceans/seas practices or policies</t>
-  </si>
-  <si>
     <t>Non-Recycled Waste</t>
   </si>
   <si>
     <t>Threatened Species Exposure</t>
   </si>
   <si>
-    <t>Operations, which affect threatened species</t>
-  </si>
-  <si>
     <t>Biodiversity Protection Policy</t>
   </si>
   <si>
-    <t>Existence of a biodiversity protection policy that encompasses operational sites owned, leased, managed in, or adjacent to, a protected area or an area of high biodiversity value outside protected areas</t>
-  </si>
-  <si>
     <t>Deforestation Policy</t>
   </si>
   <si>
-    <t>Existence of a policy to address deforestation. "Deforestation" means the human-induced conversion of forested land to non-forested land, which can be permanent, when this change is definitive, or temporary when this change is part of a cycle that includes natural or assisted regeneration, according to the Intergovernmental Science-Policy Platform on Biodiversity and Ecosystem Services (IPBES) as referred to in paragraph 100 of Decision No 1386/2013/EU of the European Parliament and of the Council.</t>
-  </si>
-  <si>
     <t>Green securities</t>
   </si>
   <si>
@@ -569,15 +473,9 @@
     <t>Do you have securities in investments not certified as green under a future EU legal act setting up an EU Green Bond Standard?</t>
   </si>
   <si>
-    <t>Possession of securities in investments that are not certified as green under a future EU legal act establishing an EU Green Bond Standard</t>
-  </si>
-  <si>
     <t>Workplace Accident Prevention Policy</t>
   </si>
   <si>
-    <t>Existence of a workplace accident prevention policy</t>
-  </si>
-  <si>
     <t>Rate Of Accidents</t>
   </si>
   <si>
@@ -590,21 +488,12 @@
     <t>Supplier Code Of Conduct</t>
   </si>
   <si>
-    <t>Supplier code of conduct addressing unsafe working conditions, precarious work, child labor, and forced labor.</t>
-  </si>
-  <si>
     <t>Grievance Handling Mechanism</t>
   </si>
   <si>
-    <t>Existence of a grievance/complaints handling mechanism related to employee matters</t>
-  </si>
-  <si>
     <t>Whistleblower Protection Policy</t>
   </si>
   <si>
-    <t>Existence of a policy on the protection of whistleblowers</t>
-  </si>
-  <si>
     <t>Reported Incidents Of Discrimination</t>
   </si>
   <si>
@@ -620,33 +509,18 @@
     <t>Human Rights Policy</t>
   </si>
   <si>
-    <t>Existence of a human rights policy</t>
-  </si>
-  <si>
     <t>Human Rights Due Diligence</t>
   </si>
   <si>
-    <t>Existence of due diligence processes to identify, prevent, mitigate and address adverse human rights impacts</t>
-  </si>
-  <si>
     <t>Trafficking In Human Beings Policy</t>
   </si>
   <si>
-    <t>Existence of a policy against trafficking in human beings</t>
-  </si>
-  <si>
     <t>Reported Child Labour Incidents</t>
   </si>
   <si>
-    <t>Reported incidents of child labor within own operations or supply chain</t>
-  </si>
-  <si>
     <t>Reported Forced Or Compulsory Labour Incidents</t>
   </si>
   <si>
-    <t>Reported incidents of forced or compulsory labor within own operations or supply chain.</t>
-  </si>
-  <si>
     <t>Number Of Reported Incidents Of Human Rights Violations</t>
   </si>
   <si>
@@ -660,9 +534,6 @@
   </si>
   <si>
     <t>Total Amount Of Reported Fines Of Bribery and Corruption</t>
-  </si>
-  <si>
-    <t>The company is ISO 14001 certified</t>
   </si>
   <si>
     <t>Scope 1 and 2 and 3 GHG emissions (location-based)</t>
@@ -1521,26 +1392,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}">
   <dimension ref="A1:M114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E100" sqref="E100:E114"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.7265625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="61.7265625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="79" style="3" customWidth="1"/>
-    <col min="7" max="7" width="39.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="61.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="255.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1796875" style="3"/>
+    <col min="14" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -1595,10 +1466,10 @@
         <v>13</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>202</v>
+        <v>159</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>226</v>
+        <v>183</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>14</v>
@@ -1668,7 +1539,7 @@
         <v>21</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>227</v>
+        <v>184</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>14</v>
@@ -1719,7 +1590,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="43.5">
+    <row r="6" spans="1:13" ht="45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1733,7 +1604,7 @@
         <v>28</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>228</v>
+        <v>185</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>14</v>
@@ -1749,7 +1620,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="72.5">
+    <row r="7" spans="1:13" ht="75">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1763,7 +1634,7 @@
         <v>32</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>229</v>
+        <v>186</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
@@ -1777,7 +1648,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="29">
+    <row r="8" spans="1:13" ht="30">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1791,7 +1662,7 @@
         <v>33</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>230</v>
+        <v>187</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>14</v>
@@ -1807,7 +1678,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="29">
+    <row r="9" spans="1:13" ht="30">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1821,7 +1692,7 @@
         <v>34</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>14</v>
@@ -1837,7 +1708,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="29">
+    <row r="10" spans="1:13" ht="45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1851,7 +1722,7 @@
         <v>35</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>232</v>
+        <v>189</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>14</v>
@@ -1867,7 +1738,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="43.5">
+    <row r="11" spans="1:13" ht="45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1881,7 +1752,7 @@
         <v>36</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>233</v>
+        <v>190</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>14</v>
@@ -1897,7 +1768,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="43.5">
+    <row r="12" spans="1:13" ht="45">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1911,7 +1782,7 @@
         <v>37</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>234</v>
+        <v>191</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>14</v>
@@ -1927,7 +1798,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="43.5">
+    <row r="13" spans="1:13" ht="45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1941,7 +1812,7 @@
         <v>38</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>235</v>
+        <v>192</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>14</v>
@@ -1957,7 +1828,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="43.5">
+    <row r="14" spans="1:13" ht="60">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1968,10 +1839,10 @@
         <v>27</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>214</v>
+        <v>171</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>236</v>
+        <v>193</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
@@ -1985,7 +1856,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="43.5">
+    <row r="15" spans="1:13" ht="45">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1996,10 +1867,10 @@
         <v>27</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>215</v>
+        <v>172</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>237</v>
+        <v>194</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
@@ -2013,7 +1884,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="29">
+    <row r="16" spans="1:13" ht="30">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2027,7 +1898,7 @@
         <v>39</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>238</v>
+        <v>195</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>14</v>
@@ -2043,7 +1914,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="43.5">
+    <row r="17" spans="1:10" ht="45">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2054,10 +1925,10 @@
         <v>27</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>198</v>
+        <v>155</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>239</v>
+        <v>196</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
@@ -2071,7 +1942,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="43.5">
+    <row r="18" spans="1:10" ht="45">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2082,10 +1953,10 @@
         <v>27</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>199</v>
+        <v>156</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>240</v>
+        <v>197</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
@@ -2110,10 +1981,10 @@
         <v>27</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>224</v>
+        <v>181</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>14</v>
@@ -2129,7 +2000,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="72.5">
+    <row r="20" spans="1:10" ht="75">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2143,7 +2014,7 @@
         <v>40</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>241</v>
+        <v>198</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
@@ -2157,7 +2028,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="87">
+    <row r="21" spans="1:10" ht="90">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2171,7 +2042,7 @@
         <v>42</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>242</v>
+        <v>199</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
@@ -2185,7 +2056,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="29">
+    <row r="22" spans="1:10" ht="30">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2199,7 +2070,7 @@
         <v>43</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>243</v>
+        <v>200</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>14</v>
@@ -2215,7 +2086,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="43.5">
+    <row r="23" spans="1:10" ht="45">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2229,7 +2100,7 @@
         <v>45</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>244</v>
+        <v>201</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>14</v>
@@ -2245,7 +2116,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="72.5">
+    <row r="24" spans="1:10" ht="75">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2256,10 +2127,10 @@
         <v>27</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>216</v>
+        <v>173</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>245</v>
+        <v>202</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
@@ -2273,7 +2144,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="87">
+    <row r="25" spans="1:10" ht="105">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2284,10 +2155,10 @@
         <v>27</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>217</v>
+        <v>174</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>246</v>
+        <v>203</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
@@ -2301,7 +2172,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="72.5">
+    <row r="26" spans="1:10" ht="75">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2312,10 +2183,10 @@
         <v>27</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>247</v>
+        <v>204</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
@@ -2329,7 +2200,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="72.5">
+    <row r="27" spans="1:10" ht="75">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2340,10 +2211,10 @@
         <v>27</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>219</v>
+        <v>176</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>248</v>
+        <v>205</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
@@ -2357,7 +2228,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="72.5">
+    <row r="28" spans="1:10" ht="90">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2371,13 +2242,11 @@
         <v>46</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>249</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>47</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>14</v>
@@ -2398,10 +2267,10 @@
         <v>27</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>220</v>
+        <v>177</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="7" t="s">
@@ -2409,7 +2278,7 @@
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="7" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="J29" s="7" t="s">
         <v>31</v>
@@ -2426,10 +2295,10 @@
         <v>27</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>222</v>
+        <v>179</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>251</v>
+        <v>208</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="7" t="s">
@@ -2437,13 +2306,13 @@
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="7" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="J30" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="72.5">
+    <row r="31" spans="1:10" ht="90">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2451,59 +2320,59 @@
         <v>26</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="E31" s="15" t="s">
-        <v>252</v>
+        <v>209</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H31" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="J31" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="90">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J31" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="72.5">
-      <c r="A32" s="1">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="E32" s="15" t="s">
-        <v>253</v>
+        <v>210</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I32" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="J32" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="43.5">
+    <row r="33" spans="1:10" ht="45">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2511,13 +2380,13 @@
         <v>26</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>254</v>
+        <v>211</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>14</v>
@@ -2526,10 +2395,10 @@
         <v>29</v>
       </c>
       <c r="H33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>31</v>
@@ -2543,31 +2412,31 @@
         <v>26</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D34" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="J34" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="43.5">
+    <row r="35" spans="1:10" ht="45">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2575,13 +2444,13 @@
         <v>26</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>255</v>
+        <v>212</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>14</v>
@@ -2590,16 +2459,16 @@
         <v>29</v>
       </c>
       <c r="H35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I35" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="J35" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="29">
+    <row r="36" spans="1:10" ht="30">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2607,13 +2476,13 @@
         <v>26</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>256</v>
+        <v>213</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>14</v>
@@ -2622,10 +2491,10 @@
         <v>29</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>31</v>
@@ -2639,20 +2508,18 @@
         <v>26</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E37" s="16" t="s">
-        <v>257</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="H37" s="1" t="s">
         <v>14</v>
       </c>
@@ -2663,7 +2530,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="101.5">
+    <row r="38" spans="1:10" ht="120">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2671,29 +2538,29 @@
         <v>26</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>258</v>
+        <v>215</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H38" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I38" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="J38" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="58">
+    <row r="39" spans="1:10" ht="75">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2701,19 +2568,17 @@
         <v>26</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>259</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>65</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>14</v>
@@ -2725,7 +2590,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="58">
+    <row r="40" spans="1:10" ht="60">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2733,19 +2598,17 @@
         <v>26</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="E40" s="17" t="s">
-        <v>260</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>67</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>14</v>
@@ -2757,7 +2620,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="87">
+    <row r="41" spans="1:10" ht="90">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2765,19 +2628,17 @@
         <v>26</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>69</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="F41" s="1"/>
       <c r="G41" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>14</v>
@@ -2789,7 +2650,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="116">
+    <row r="42" spans="1:10" ht="135">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2797,19 +2658,17 @@
         <v>26</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>262</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>71</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>14</v>
@@ -2821,7 +2680,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="72.5">
+    <row r="43" spans="1:10" ht="75">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2829,13 +2688,13 @@
         <v>26</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>263</v>
+        <v>220</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>14</v>
@@ -2844,7 +2703,7 @@
         <v>29</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>30</v>
@@ -2853,7 +2712,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="159.5">
+    <row r="44" spans="1:10" ht="180">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2861,20 +2720,20 @@
         <v>26</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>264</v>
+        <v>221</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>30</v>
@@ -2888,22 +2747,20 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>265</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>79</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="F45" s="1"/>
       <c r="G45" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>14</v>
@@ -2920,22 +2777,20 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>266</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>81</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="F46" s="1"/>
       <c r="G46" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>14</v>
@@ -2952,22 +2807,20 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>267</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>83</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="F47" s="1"/>
       <c r="G47" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>14</v>
@@ -2984,22 +2837,20 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>268</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>85</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="F48" s="1"/>
       <c r="G48" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>14</v>
@@ -3016,22 +2867,20 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>88</v>
-      </c>
+      <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>14</v>
@@ -3048,22 +2897,20 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>90</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>14</v>
@@ -3080,22 +2927,20 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>93</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>14</v>
@@ -3112,22 +2957,20 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>96</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F52" s="1"/>
       <c r="G52" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>14</v>
@@ -3144,22 +2987,20 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>99</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="F53" s="1"/>
       <c r="G53" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>14</v>
@@ -3176,22 +3017,20 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>269</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>197</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="F54" s="1"/>
       <c r="G54" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>14</v>
@@ -3203,27 +3042,25 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="43.5">
+    <row r="55" spans="1:10" ht="45">
       <c r="A55" s="1">
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>102</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="F55" s="1"/>
       <c r="G55" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>14</v>
@@ -3240,22 +3077,20 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>105</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="F56" s="1"/>
       <c r="G56" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>14</v>
@@ -3272,22 +3107,20 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>108</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="F57" s="1"/>
       <c r="G57" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>14</v>
@@ -3304,22 +3137,20 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>111</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="F58" s="1"/>
       <c r="G58" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>14</v>
@@ -3336,22 +3167,20 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>113</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="F59" s="1"/>
       <c r="G59" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>14</v>
@@ -3363,27 +3192,25 @@
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="43.5">
+    <row r="60" spans="1:10" ht="60">
       <c r="A60" s="1">
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>115</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="F60" s="1"/>
       <c r="G60" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>14</v>
@@ -3395,27 +3222,25 @@
         <v>31</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="58">
+    <row r="61" spans="1:10" ht="60">
       <c r="A61" s="1">
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>272</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>117</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="F61" s="1"/>
       <c r="G61" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>14</v>
@@ -3432,16 +3257,16 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>14</v>
@@ -3450,7 +3275,7 @@
         <v>41</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>14</v>
@@ -3464,16 +3289,16 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>14</v>
@@ -3482,7 +3307,7 @@
         <v>41</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I63" s="1" t="s">
         <v>14</v>
@@ -3491,21 +3316,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="58">
+    <row r="64" spans="1:10" ht="60">
       <c r="A64" s="1">
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>273</v>
+        <v>230</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>14</v>
@@ -3515,7 +3340,7 @@
       </c>
       <c r="H64" s="1"/>
       <c r="I64" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J64" s="1" t="s">
         <v>31</v>
@@ -3526,23 +3351,23 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>204</v>
+        <v>161</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>205</v>
+        <v>162</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I65" s="1"/>
       <c r="J65" s="1" t="s">
@@ -3554,23 +3379,23 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>206</v>
+        <v>163</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>207</v>
+        <v>164</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I66" s="1"/>
       <c r="J66" s="1" t="s">
@@ -3582,23 +3407,23 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>208</v>
+        <v>165</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>209</v>
+        <v>166</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I67" s="1"/>
       <c r="J67" s="1" t="s">
@@ -3610,110 +3435,110 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>210</v>
+        <v>167</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>211</v>
+        <v>168</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I68" s="1"/>
       <c r="J68" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="43.5">
+    <row r="69" spans="1:10" ht="45">
       <c r="A69" s="1">
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>212</v>
+        <v>169</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>274</v>
+        <v>231</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J69" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="43.5">
+    <row r="70" spans="1:10" ht="45">
       <c r="A70" s="1">
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>213</v>
+        <v>170</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="58">
+    <row r="71" spans="1:10" ht="60">
       <c r="A71" s="1">
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="E71" s="17" t="s">
-        <v>276</v>
+        <v>233</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>14</v>
@@ -3725,7 +3550,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="87">
+    <row r="72" spans="1:10" ht="105">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -3733,20 +3558,20 @@
         <v>26</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="E72" s="17" t="s">
-        <v>277</v>
+        <v>234</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I72" s="1" t="s">
         <v>30</v>
@@ -3755,7 +3580,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="130.5">
+    <row r="73" spans="1:10" ht="135">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -3763,20 +3588,20 @@
         <v>26</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="E73" s="17" t="s">
-        <v>278</v>
+        <v>235</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I73" s="1" t="s">
         <v>30</v>
@@ -3785,7 +3610,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="116">
+    <row r="74" spans="1:10" ht="135">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -3793,20 +3618,20 @@
         <v>26</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>279</v>
+        <v>236</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>30</v>
@@ -3815,7 +3640,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="43.5">
+    <row r="75" spans="1:10" ht="45">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -3823,19 +3648,17 @@
         <v>26</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>131</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="F75" s="1"/>
       <c r="G75" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>14</v>
@@ -3847,7 +3670,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="43.5">
+    <row r="76" spans="1:10" ht="60">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -3855,13 +3678,13 @@
         <v>26</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="E76" s="17" t="s">
-        <v>281</v>
+        <v>238</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>14</v>
@@ -3870,16 +3693,16 @@
         <v>29</v>
       </c>
       <c r="H76" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I76" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I76" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="J76" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="43.5">
+    <row r="77" spans="1:10" ht="45">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -3887,13 +3710,13 @@
         <v>26</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>282</v>
+        <v>239</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>14</v>
@@ -3902,16 +3725,16 @@
         <v>29</v>
       </c>
       <c r="H77" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I77" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I77" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="J77" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="29">
+    <row r="78" spans="1:10" ht="45">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -3919,13 +3742,13 @@
         <v>26</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>283</v>
+        <v>240</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>14</v>
@@ -3934,16 +3757,16 @@
         <v>29</v>
       </c>
       <c r="H78" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I78" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I78" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="J78" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="29">
+    <row r="79" spans="1:10" ht="45">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -3951,13 +3774,13 @@
         <v>26</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>284</v>
+        <v>241</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>14</v>
@@ -3966,16 +3789,16 @@
         <v>29</v>
       </c>
       <c r="H79" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I79" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I79" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="J79" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="29">
+    <row r="80" spans="1:10" ht="45">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -3983,13 +3806,13 @@
         <v>26</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>285</v>
+        <v>242</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>14</v>
@@ -3998,16 +3821,16 @@
         <v>29</v>
       </c>
       <c r="H80" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I80" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I80" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="J80" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="43.5">
+    <row r="81" spans="1:10" ht="45">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -4015,13 +3838,13 @@
         <v>26</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>286</v>
+        <v>243</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>14</v>
@@ -4030,16 +3853,16 @@
         <v>29</v>
       </c>
       <c r="H81" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I81" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I81" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="J81" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="43.5">
+    <row r="82" spans="1:10" ht="45">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -4047,13 +3870,13 @@
         <v>26</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>287</v>
+        <v>244</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>14</v>
@@ -4062,16 +3885,16 @@
         <v>29</v>
       </c>
       <c r="H82" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I82" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I82" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="J82" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="29">
+    <row r="83" spans="1:10" ht="30">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -4079,13 +3902,13 @@
         <v>26</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>288</v>
+        <v>245</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>14</v>
@@ -4094,16 +3917,16 @@
         <v>29</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="J83" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="29">
+    <row r="84" spans="1:10" ht="30">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -4111,13 +3934,13 @@
         <v>26</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>289</v>
+        <v>246</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>14</v>
@@ -4126,16 +3949,16 @@
         <v>29</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="J84" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="43.5">
+    <row r="85" spans="1:10" ht="45">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -4143,13 +3966,13 @@
         <v>26</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="E85" s="17" t="s">
-        <v>290</v>
+        <v>247</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>14</v>
@@ -4158,16 +3981,16 @@
         <v>29</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="J85" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="29">
+    <row r="86" spans="1:10" ht="30">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -4175,19 +3998,17 @@
         <v>26</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>144</v>
+        <v>121</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>145</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="F86" s="1"/>
       <c r="G86" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>14</v>
@@ -4199,7 +4020,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="72.5">
+    <row r="87" spans="1:10" ht="75">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -4207,19 +4028,17 @@
         <v>26</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="E87" s="17" t="s">
-        <v>292</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>147</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="F87" s="1"/>
       <c r="G87" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>14</v>
@@ -4231,7 +4050,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="43.5">
+    <row r="88" spans="1:10" ht="45">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -4239,19 +4058,17 @@
         <v>26</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>149</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="F88" s="1"/>
       <c r="G88" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>14</v>
@@ -4263,7 +4080,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="43.5">
+    <row r="89" spans="1:10" ht="45">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -4271,19 +4088,17 @@
         <v>26</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>151</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="F89" s="1"/>
       <c r="G89" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>14</v>
@@ -4295,7 +4110,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="29">
+    <row r="90" spans="1:10" ht="30">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -4303,19 +4118,17 @@
         <v>26</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>153</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="F90" s="1"/>
       <c r="G90" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>14</v>
@@ -4327,7 +4140,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="29">
+    <row r="91" spans="1:10" ht="30">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -4335,19 +4148,17 @@
         <v>26</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>296</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>155</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="F91" s="1"/>
       <c r="G91" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>14</v>
@@ -4359,7 +4170,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="58">
+    <row r="92" spans="1:10" ht="60">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -4367,22 +4178,20 @@
         <v>26</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>297</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>254</v>
+      </c>
+      <c r="F92" s="1"/>
       <c r="G92" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I92" s="1" t="s">
         <v>30</v>
@@ -4391,7 +4200,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="29">
+    <row r="93" spans="1:10" ht="30">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -4399,19 +4208,17 @@
         <v>26</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>298</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>158</v>
-      </c>
+        <v>255</v>
+      </c>
+      <c r="F93" s="1"/>
       <c r="G93" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>14</v>
@@ -4423,7 +4230,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="58">
+    <row r="94" spans="1:10" ht="75">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -4431,20 +4238,18 @@
         <v>26</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E94" s="17" t="s">
-        <v>299</v>
-      </c>
-      <c r="F94" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G94" s="1" t="s">
-        <v>203</v>
-      </c>
       <c r="H94" s="1" t="s">
         <v>14</v>
       </c>
@@ -4455,7 +4260,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="130.5">
+    <row r="95" spans="1:10" ht="150">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -4463,19 +4268,17 @@
         <v>26</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>300</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>162</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="F95" s="1"/>
       <c r="G95" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>14</v>
@@ -4492,22 +4295,20 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>163</v>
+        <v>131</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>164</v>
+        <v>132</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>166</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="F96" s="1"/>
       <c r="G96" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>14</v>
@@ -4519,27 +4320,25 @@
         <v>31</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="29">
+    <row r="97" spans="1:10" ht="30">
       <c r="A97" s="1">
         <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>168</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="F97" s="1"/>
       <c r="G97" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>14</v>
@@ -4551,30 +4350,28 @@
         <v>31</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="58">
+    <row r="98" spans="1:10" ht="60">
       <c r="A98" s="1">
         <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>169</v>
+        <v>135</v>
       </c>
       <c r="E98" s="9" t="s">
-        <v>302</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="F98" s="1"/>
       <c r="G98" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I98" s="1"/>
       <c r="J98" s="1" t="s">
@@ -4586,54 +4383,50 @@
         <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="F99" s="1"/>
       <c r="G99" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="J99" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="43.5">
+    <row r="100" spans="1:10" ht="45">
       <c r="A100" s="1">
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="E100" s="17" t="s">
-        <v>303</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>173</v>
-      </c>
+        <v>260</v>
+      </c>
+      <c r="F100" s="1"/>
       <c r="G100" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>14</v>
@@ -4645,27 +4438,25 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="43.5">
+    <row r="101" spans="1:10" ht="45">
       <c r="A101" s="1">
         <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="E101" s="9" t="s">
-        <v>304</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>175</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="F101" s="1"/>
       <c r="G101" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>14</v>
@@ -4677,27 +4468,25 @@
         <v>31</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="29">
+    <row r="102" spans="1:10" ht="30">
       <c r="A102" s="1">
         <v>101</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>176</v>
+        <v>140</v>
       </c>
       <c r="E102" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>177</v>
-      </c>
+        <v>262</v>
+      </c>
+      <c r="F102" s="1"/>
       <c r="G102" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>14</v>
@@ -4709,30 +4498,28 @@
         <v>31</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="29">
+    <row r="103" spans="1:10" ht="30">
       <c r="A103" s="1">
         <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>178</v>
+        <v>141</v>
       </c>
       <c r="E103" s="9" t="s">
-        <v>306</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="F103" s="1"/>
       <c r="G103" s="1" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I103" s="1" t="s">
         <v>14</v>
@@ -4741,30 +4528,28 @@
         <v>31</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="43.5">
+    <row r="104" spans="1:10" ht="45">
       <c r="A104" s="1">
         <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>179</v>
+        <v>142</v>
       </c>
       <c r="E104" s="9" t="s">
-        <v>307</v>
-      </c>
-      <c r="F104" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="F104" s="1"/>
       <c r="G104" s="1" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I104" s="1" t="s">
         <v>14</v>
@@ -4773,57 +4558,53 @@
         <v>31</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="58">
+    <row r="105" spans="1:10" ht="60">
       <c r="A105" s="1">
         <v>105</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>180</v>
+        <v>143</v>
       </c>
       <c r="E105" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="F105" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>265</v>
+      </c>
+      <c r="F105" s="1"/>
       <c r="G105" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I105" s="1"/>
       <c r="J105" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="29">
+    <row r="106" spans="1:10" ht="30">
       <c r="A106" s="1">
         <v>106</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>181</v>
+        <v>144</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>182</v>
+        <v>145</v>
       </c>
       <c r="E106" s="9" t="s">
-        <v>309</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>183</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="F106" s="1"/>
       <c r="G106" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H106" s="1" t="s">
         <v>14</v>
@@ -4835,27 +4616,25 @@
         <v>31</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="43.5">
+    <row r="107" spans="1:10" ht="45">
       <c r="A107" s="1">
         <v>107</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>181</v>
+        <v>144</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>184</v>
+        <v>146</v>
       </c>
       <c r="E107" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>185</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="F107" s="1"/>
       <c r="G107" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H107" s="1" t="s">
         <v>14</v>
@@ -4867,27 +4646,25 @@
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="29">
+    <row r="108" spans="1:10" ht="30">
       <c r="A108" s="1">
         <v>108</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>181</v>
+        <v>144</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>186</v>
+        <v>147</v>
       </c>
       <c r="E108" s="9" t="s">
-        <v>311</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>187</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="F108" s="1"/>
       <c r="G108" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H108" s="1" t="s">
         <v>14</v>
@@ -4899,27 +4676,25 @@
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="43.5">
+    <row r="109" spans="1:10" ht="45">
       <c r="A109" s="1">
         <v>109</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>181</v>
+        <v>144</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>188</v>
+        <v>148</v>
       </c>
       <c r="E109" s="17" t="s">
-        <v>312</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>189</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="F109" s="1"/>
       <c r="G109" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H109" s="1" t="s">
         <v>14</v>
@@ -4931,27 +4706,25 @@
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="43.5">
+    <row r="110" spans="1:10" ht="45">
       <c r="A110" s="1">
         <v>110</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>181</v>
+        <v>144</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>190</v>
+        <v>149</v>
       </c>
       <c r="E110" s="17" t="s">
-        <v>313</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>191</v>
-      </c>
+        <v>270</v>
+      </c>
+      <c r="F110" s="1"/>
       <c r="G110" s="1" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="H110" s="1" t="s">
         <v>14</v>
@@ -4963,30 +4736,28 @@
         <v>31</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="43.5">
+    <row r="111" spans="1:10" ht="45">
       <c r="A111" s="1">
         <v>111</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>181</v>
+        <v>144</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>192</v>
+        <v>150</v>
       </c>
       <c r="E111" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="F111" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="F111" s="1"/>
       <c r="G111" s="1" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I111" s="1" t="s">
         <v>14</v>
@@ -4995,30 +4766,30 @@
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="43.5">
+    <row r="112" spans="1:10" ht="45">
       <c r="A112" s="1">
         <v>112</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>193</v>
+        <v>151</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>194</v>
+        <v>152</v>
       </c>
       <c r="E112" s="9" t="s">
-        <v>315</v>
+        <v>272</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I112" s="1" t="s">
         <v>14</v>
@@ -5027,30 +4798,30 @@
         <v>31</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="43.5">
+    <row r="113" spans="1:10" ht="45">
       <c r="A113" s="1">
         <v>113</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>193</v>
+        <v>151</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>195</v>
+        <v>153</v>
       </c>
       <c r="E113" s="9" t="s">
-        <v>316</v>
+        <v>273</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I113" s="1" t="s">
         <v>14</v>
@@ -5059,21 +4830,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="29">
+    <row r="114" spans="1:10" ht="45">
       <c r="A114" s="1">
         <v>114</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>193</v>
+        <v>151</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>196</v>
+        <v>154</v>
       </c>
       <c r="E114" s="18" t="s">
-        <v>317</v>
+        <v>274</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>14</v>
@@ -5082,7 +4853,7 @@
         <v>41</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I114" s="1" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Removed all required fields from SFDR Excel
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
+++ b/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dataland\datalandClean\dataland-framework-toolbox\inputs\sfdr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92582\Documents\Dataland\Dataland\dataland-framework-toolbox\inputs\sfdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9301C896-2570-46B3-BA20-F045C89CA158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44A4B0B-5FB9-4D03-A0DA-88EDAD5CA268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-10800" windowWidth="38620" windowHeight="21220" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="2" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="274">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>Fiscal Year Deviation</t>
@@ -1392,26 +1389,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}">
   <dimension ref="A1:M114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="F108" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M129" sqref="M129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.265625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="61.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="255.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.73046875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="61.73046875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="255.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.265625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="3"/>
+    <col min="14" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -1466,10 +1463,10 @@
         <v>13</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>14</v>
@@ -1485,9 +1482,6 @@
       </c>
       <c r="J2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1501,28 +1495,25 @@
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="I3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1536,10 +1527,10 @@
         <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>14</v>
@@ -1555,9 +1546,6 @@
       </c>
       <c r="J4" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1571,16 +1559,16 @@
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
@@ -1590,384 +1578,384 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="45">
+    <row r="6" spans="1:13" ht="42.75">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E6" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="75">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="57">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="28.5">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="28.5">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="28.5">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="42.75">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D11" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="42.75">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D12" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="42.75">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="60">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="42.75">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D14" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="42.75">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D15" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="28.5">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="42.75">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D17" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="42.75">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D18" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1975,285 +1963,285 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D19" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="F19" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="75">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="57">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D20" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="90">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="71.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D21" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="28.5">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="42.75">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D23" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="75">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="57">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D24" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="105">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="85.5">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D25" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="75">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="57">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D26" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="75">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="57">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D27" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="90">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="71.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D28" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -2261,27 +2249,27 @@
         <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D29" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -2289,119 +2277,119 @@
         <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D30" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="90">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="71.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E31" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H31" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I31" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="J31" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="90">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="71.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H32" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I32" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="J32" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="42.75">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H33" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I33" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="J33" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2409,95 +2397,95 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="J34" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="42.75">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H35" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I35" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="J35" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="28.5">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2505,20 +2493,20 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>14</v>
@@ -2530,55 +2518,55 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="120">
+    <row r="38" spans="1:10" ht="99.75">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I38" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="J38" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="75">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="57">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="E39" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>14</v>
@@ -2587,28 +2575,28 @@
         <v>14</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="60">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="57">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>14</v>
@@ -2617,28 +2605,28 @@
         <v>14</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="90">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="85.5">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>14</v>
@@ -2647,28 +2635,28 @@
         <v>14</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="135">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="114">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>14</v>
@@ -2677,69 +2665,69 @@
         <v>14</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="75">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="57">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="E43" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G43" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I43" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H43" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="J43" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="180">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="142.5">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="E44" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I44" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H44" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="J44" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2747,20 +2735,20 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="E45" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>14</v>
@@ -2769,7 +2757,7 @@
         <v>14</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2777,20 +2765,20 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D46" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>14</v>
@@ -2799,7 +2787,7 @@
         <v>14</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2807,20 +2795,20 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D47" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>14</v>
@@ -2829,7 +2817,7 @@
         <v>14</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2837,20 +2825,20 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D48" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>14</v>
@@ -2859,7 +2847,7 @@
         <v>14</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2867,20 +2855,20 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D49" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>14</v>
@@ -2889,7 +2877,7 @@
         <v>14</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2897,20 +2885,20 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D50" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>14</v>
@@ -2919,7 +2907,7 @@
         <v>14</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2927,20 +2915,20 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D51" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>14</v>
@@ -2949,7 +2937,7 @@
         <v>14</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2957,20 +2945,20 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D52" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>14</v>
@@ -2979,7 +2967,7 @@
         <v>14</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2987,20 +2975,20 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D53" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>14</v>
@@ -3009,7 +2997,7 @@
         <v>14</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -3017,20 +3005,20 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D54" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>14</v>
@@ -3039,28 +3027,28 @@
         <v>14</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="42.75">
       <c r="A55" s="1">
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D55" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>14</v>
@@ -3069,7 +3057,7 @@
         <v>14</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -3077,20 +3065,20 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D56" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>14</v>
@@ -3099,7 +3087,7 @@
         <v>14</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -3107,20 +3095,20 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D57" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>14</v>
@@ -3129,7 +3117,7 @@
         <v>14</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -3137,20 +3125,20 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D58" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>14</v>
@@ -3159,7 +3147,7 @@
         <v>14</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -3167,20 +3155,20 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D59" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>14</v>
@@ -3189,28 +3177,28 @@
         <v>14</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="60">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="42.75">
       <c r="A60" s="1">
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D60" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>14</v>
@@ -3219,28 +3207,28 @@
         <v>14</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="60">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="57">
       <c r="A61" s="1">
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D61" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>14</v>
@@ -3249,7 +3237,7 @@
         <v>14</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -3257,31 +3245,31 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D62" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E62" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="F62" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -3289,61 +3277,61 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D63" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E63" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="F63" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I63" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="60">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="57">
       <c r="A64" s="1">
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D64" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H64" s="1"/>
       <c r="I64" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -3351,27 +3339,27 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D65" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E65" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I65" s="1"/>
       <c r="J65" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -3379,27 +3367,27 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D66" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E66" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I66" s="1"/>
       <c r="J66" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -3407,27 +3395,27 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D67" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I67" s="1"/>
       <c r="J67" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -3435,110 +3423,110 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D68" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E68" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I68" s="1"/>
       <c r="J68" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="28.5">
       <c r="A69" s="1">
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D69" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="28.5">
       <c r="A70" s="1">
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D70" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="60">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="42.75">
       <c r="A71" s="1">
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D71" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E71" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>14</v>
@@ -3547,118 +3535,118 @@
         <v>14</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="105">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="85.5">
       <c r="A72" s="1">
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C72" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D72" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="E72" s="17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I72" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H72" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I72" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="J72" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="135">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="114">
       <c r="A73" s="1">
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E73" s="17" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I73" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H73" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I73" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="J73" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" ht="135">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="114">
       <c r="A74" s="1">
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I74" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H74" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="J74" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="42.75">
       <c r="A75" s="1">
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>14</v>
@@ -3667,348 +3655,348 @@
         <v>14</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" ht="60">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="42.75">
       <c r="A76" s="1">
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E76" s="17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H76" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I76" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I76" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="J76" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="42.75">
       <c r="A77" s="1">
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H77" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I77" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I77" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="J77" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="28.5">
       <c r="A78" s="1">
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H78" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I78" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I78" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="J78" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="28.5">
       <c r="A79" s="1">
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H79" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I79" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I79" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="J79" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="28.5">
       <c r="A80" s="1">
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H80" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I80" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I80" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="J80" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="42.75">
       <c r="A81" s="1">
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H81" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I81" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I81" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="J81" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="42.75">
       <c r="A82" s="1">
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H82" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I82" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I82" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="J82" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="28.5">
       <c r="A83" s="1">
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D83" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I83" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E83" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H83" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I83" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="J83" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="28.5">
       <c r="A84" s="1">
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="42.75">
       <c r="A85" s="1">
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D85" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E85" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I85" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E85" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G85" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H85" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I85" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="J85" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" ht="30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="28.5">
       <c r="A86" s="1">
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>14</v>
@@ -4017,28 +4005,28 @@
         <v>14</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" ht="75">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="57">
       <c r="A87" s="1">
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E87" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>14</v>
@@ -4047,28 +4035,28 @@
         <v>14</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="42.75">
       <c r="A88" s="1">
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F88" s="1"/>
       <c r="G88" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>14</v>
@@ -4077,28 +4065,28 @@
         <v>14</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="42.75">
       <c r="A89" s="1">
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>14</v>
@@ -4107,28 +4095,28 @@
         <v>14</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" ht="30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="28.5">
       <c r="A90" s="1">
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F90" s="1"/>
       <c r="G90" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>14</v>
@@ -4137,28 +4125,28 @@
         <v>14</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" ht="30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="28.5">
       <c r="A91" s="1">
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>14</v>
@@ -4167,58 +4155,58 @@
         <v>14</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" ht="60">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="57">
       <c r="A92" s="1">
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F92" s="1"/>
       <c r="G92" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I92" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H92" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I92" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="J92" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" ht="30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="28.5">
       <c r="A93" s="1">
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F93" s="1"/>
       <c r="G93" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>14</v>
@@ -4227,28 +4215,28 @@
         <v>14</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" ht="75">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="57">
       <c r="A94" s="1">
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E94" s="17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F94" s="1"/>
       <c r="G94" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>14</v>
@@ -4257,28 +4245,28 @@
         <v>14</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" ht="150">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="114">
       <c r="A95" s="1">
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F95" s="1"/>
       <c r="G95" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>14</v>
@@ -4287,7 +4275,7 @@
         <v>14</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -4295,20 +4283,20 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C96" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="E96" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="F96" s="1"/>
       <c r="G96" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>14</v>
@@ -4317,28 +4305,28 @@
         <v>14</v>
       </c>
       <c r="J96" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" ht="30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="28.5">
       <c r="A97" s="1">
         <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D97" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F97" s="1"/>
       <c r="G97" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>14</v>
@@ -4347,35 +4335,35 @@
         <v>14</v>
       </c>
       <c r="J97" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" ht="60">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" ht="42.75">
       <c r="A98" s="1">
         <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C98" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D98" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E98" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F98" s="1"/>
       <c r="G98" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I98" s="1"/>
       <c r="J98" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -4383,50 +4371,50 @@
         <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C99" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C99" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D99" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F99" s="1"/>
       <c r="G99" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J99" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" ht="42.75">
       <c r="A100" s="1">
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C100" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D100" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E100" s="17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F100" s="1"/>
       <c r="G100" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>14</v>
@@ -4435,28 +4423,28 @@
         <v>14</v>
       </c>
       <c r="J100" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" ht="42.75">
       <c r="A101" s="1">
         <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D101" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E101" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>14</v>
@@ -4465,28 +4453,28 @@
         <v>14</v>
       </c>
       <c r="J101" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" ht="30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" ht="28.5">
       <c r="A102" s="1">
         <v>101</v>
       </c>
       <c r="B102" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D102" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E102" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>14</v>
@@ -4495,116 +4483,116 @@
         <v>14</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" ht="30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" ht="28.5">
       <c r="A103" s="1">
         <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C103" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D103" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E103" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F103" s="1"/>
       <c r="G103" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I103" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" ht="42.75">
       <c r="A104" s="1">
         <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C104" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D104" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E104" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F104" s="1"/>
       <c r="G104" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I104" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" ht="60">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" ht="57">
       <c r="A105" s="1">
         <v>105</v>
       </c>
       <c r="B105" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C105" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D105" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E105" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I105" s="1"/>
       <c r="J105" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" ht="30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" ht="28.5">
       <c r="A106" s="1">
         <v>106</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C106" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D106" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D106" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="E106" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F106" s="1"/>
       <c r="G106" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H106" s="1" t="s">
         <v>14</v>
@@ -4613,28 +4601,28 @@
         <v>14</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" ht="42.75">
       <c r="A107" s="1">
         <v>107</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E107" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F107" s="1"/>
       <c r="G107" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H107" s="1" t="s">
         <v>14</v>
@@ -4643,28 +4631,28 @@
         <v>14</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" ht="30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="28.5">
       <c r="A108" s="1">
         <v>108</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E108" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F108" s="1"/>
       <c r="G108" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H108" s="1" t="s">
         <v>14</v>
@@ -4673,28 +4661,28 @@
         <v>14</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" ht="42.75">
       <c r="A109" s="1">
         <v>109</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E109" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F109" s="1"/>
       <c r="G109" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H109" s="1" t="s">
         <v>14</v>
@@ -4703,28 +4691,28 @@
         <v>14</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" ht="42.75">
       <c r="A110" s="1">
         <v>110</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E110" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F110" s="1"/>
       <c r="G110" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H110" s="1" t="s">
         <v>14</v>
@@ -4733,133 +4721,133 @@
         <v>14</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" ht="42.75">
       <c r="A111" s="1">
         <v>111</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E111" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F111" s="1"/>
       <c r="G111" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I111" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" ht="42.75">
       <c r="A112" s="1">
         <v>112</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C112" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D112" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D112" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="E112" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I112" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="113" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" ht="42.75">
       <c r="A113" s="1">
         <v>113</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E113" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I113" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" ht="28.5">
       <c r="A114" s="1">
         <v>114</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E114" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I114" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Framework Toolbox sfdr change
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
+++ b/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92582\Documents\Dataland\Dataland\dataland-framework-toolbox\inputs\sfdr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92355\Documents\Dataland\Tickets\DALA-5634\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44A4B0B-5FB9-4D03-A0DA-88EDAD5CA268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8BA1951-AD10-4961-ADDF-0A0A328E397A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="2" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="320">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -299,30 +299,18 @@
     <t>Transparency Disclosure Policy</t>
   </si>
   <si>
-    <t>Do you have a transparency policy? If yes, please share the policy with us. According to the OECD Guidelines for Multinational Enterprises, multinational companies should inform the public not only about their financial performance, but also about all of the important aspects of their business activities, such as how they are meeting social and environmental standards and what risks they foresee linked to their business activities.</t>
-  </si>
-  <si>
     <t>Human Rights Due Diligence Policy</t>
   </si>
   <si>
     <t>Policy against Child Labour</t>
   </si>
   <si>
-    <t>Do you have policies in place to abolish all forms of child labour? If yes, please share the policy with us.</t>
-  </si>
-  <si>
     <t>Policy against Forced Labour</t>
   </si>
   <si>
-    <t>Do you have policies in place to abolish all forms of forced labour? If yes, please share the policy with us.</t>
-  </si>
-  <si>
     <t>Policy against Discrimination in the Workplace</t>
   </si>
   <si>
-    <t>Do you have policies in place to eliminate discrimination in the workplace? If yes, please share the policy with us.</t>
-  </si>
-  <si>
     <t>ISO 14001 Certificate</t>
   </si>
   <si>
@@ -332,21 +320,12 @@
     <t>Fair Business Marketing Advertising Policy</t>
   </si>
   <si>
-    <t>Do you have policies and procedures in place to apply fair business, marketing and advertising practices and to guarantee the safety and quality of the goods and services? If yes, please share the relevant documents with us.</t>
-  </si>
-  <si>
     <t>Technologies Expertise Transfer Policy</t>
   </si>
   <si>
-    <t>Do you have policies and procedures in place to permit the transfer and rapid dissemination of technologies and expertise? If yes, please share the relevant documents with us.</t>
-  </si>
-  <si>
     <t>Fair Competition Policy</t>
   </si>
   <si>
-    <t>Do you have policies and procedures in place related to fair competition and anti-competitive cartels? If yes, please share the relevant documents with us.</t>
-  </si>
-  <si>
     <t>Violation Of Tax Rules And Regulation</t>
   </si>
   <si>
@@ -467,9 +446,6 @@
     <t>Securities Not Certified As Green</t>
   </si>
   <si>
-    <t>Do you have securities in investments not certified as green under a future EU legal act setting up an EU Green Bond Standard?</t>
-  </si>
-  <si>
     <t>Workplace Accident Prevention Policy</t>
   </si>
   <si>
@@ -539,12 +515,6 @@
     <t>Scope 1 and 2 and 3 GHG emissions (market-based)</t>
   </si>
   <si>
-    <t>Are you involved in violations of OECD Guidelines for Multinational Enterprises for Taxation: In the field of taxation, multinational enterprises should make their contribution to public finances within the framework of applicable law and regulations, in accordance with the tax rules and regulations of the host countries, and should cooperate with the tax authorities.</t>
-  </si>
-  <si>
-    <t>Do you have policies in place to support/respect human rights and carry out due diligence to ensure that the business activities do not have a negative human rights impact? If yes, please share the relevant documents with us.</t>
-  </si>
-  <si>
     <t>Data Date</t>
   </si>
   <si>
@@ -662,30 +632,6 @@
     <t>Sum of scope 1, 2 and 3 greenhouse gas emissions, using the market-based method to compute scope 2 greenhouse gas emissions (equity share approach preferably used).</t>
   </si>
   <si>
-    <t xml:space="preserve">The sum, at fiscal year-end, of the market capitalisation of ordinary shares, the market capitalisation of preferred shares, the book value of total debt and non-controlling interests, without the deduction of cash or cash equivalents. See also Regulation (EU) 2022/1288, Annex I, top (4). </t>
-  </si>
-  <si>
-    <t>Total revenue for the financial year. i.e., income arising in the course of an entity's ordinary activities, the amounts derived from the sale of products and the provision of services after deducting sales rebates and value added tax and other taxes directly linked to turnover. Overall turnover is equivalent to a firm's total revenues over some period of time.</t>
-  </si>
-  <si>
-    <t>Tonnes of GHG emissions per million units of the enterprise value (in the same currency as total revenue).</t>
-  </si>
-  <si>
-    <t>Tonnes of GHG emissions per million units of revenue (in the same currency as total revenue), preferably calculated using the location-based method and the equity share approach for emissions.</t>
-  </si>
-  <si>
-    <t>Tonnes of scope 1 GHG emissions per million units of revenue (in the same currency as total revenue). Scope 1 carbon emissions are emissions generated from sources that are controlled by the company that issues the underlying assets (equity share approach preferably used for emissions).</t>
-  </si>
-  <si>
-    <t>Tonnes of scope 2 GHG emissions per million units of revenue (in the same currency as total revenue). Scope 2 emissions refer to those generated from the consumption of purchased electricity, steam, or other energy sources produced upstream by external entities or companies. Preferably, these should be calculated using the location-based method and the equity share approach for emissions.</t>
-  </si>
-  <si>
-    <t>Tonnes of scope 3 GHG emissions per million units of revenue (in the same currency as total revenue). Scope 3 emissions encompass all indirect upstream and downstream emissions not covered by Scope 2. Preferably, the equity share approach should be used for calculating these emissions.</t>
-  </si>
-  <si>
-    <t>Tonnes of scope 4 GHG emissions per million units of revenue (in the same currency as total revenue). As per the GHG Protocol, Scope 4 refers to emissions avoided when a product is used as a substitute for other goods or services, providing the same functions with a lower carbon footprint.</t>
-  </si>
-  <si>
     <t>(Part of) revenues derived from exploration, mining, extraction, production, processing, storage, refining or distribution, including transportation, storage and trade, of fossil fuels. (Fossil fuels mean non-renewable carbon-based energy sources such as solid fuels, natural gas and oil.) See also Regulation (EU) 2022/1288, Annex I, top (5).</t>
   </si>
   <si>
@@ -809,18 +755,9 @@
     <t>Amount of water recycled and reused by the company. See Regulation (EU) 2022/1288, Annex I, table 2, indicator nr. 6.2 .</t>
   </si>
   <si>
-    <t>Amount in cubic meters of fresh water used per million units of revenue (in the same currency as the total revenue). See Regulation (EU) 2022/1288, Annex I, table 2, indicator nr. 6.1 .</t>
-  </si>
-  <si>
     <t>Existence of policies and procedures for water management. See Regulation (EU) 2022/1288, Annex I, table 2, indicator nr. 7.</t>
   </si>
   <si>
-    <t>Sites (partly) located in "areas of high water stress", i.e. in regions where the percentage of total water withdrawn is high (40-80%) or extremely high (greater than 80%), without a water management policy. See Regulation (EU) 2022/1288, Annex I, top (13) and table 2, indicator nr. 8.</t>
-  </si>
-  <si>
-    <t>Involvement in manufacture of pesticides and other agrochemical products. See Regulation (EU) 2022/1288, Annex I, table 2, indicator nr. 9 and Regulation (EC) No 1893/2006, Annex I, Division 20.2.</t>
-  </si>
-  <si>
     <t>Involvement in activities, which cause land degradation, desertification or soil sealing. See Regulation (EU) 2022/1288, Annex I, table 2, indicator nr. 10.</t>
   </si>
   <si>
@@ -875,12 +812,6 @@
     <t>Existence of a policy against trafficking in human beings. See Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 11.</t>
   </si>
   <si>
-    <t>Number of reported incidents of child labor within own operations or supply chain. Linked to Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 12.</t>
-  </si>
-  <si>
-    <t>Number of reported incidents of forced or compulsory labor within own operations or supply chain. Linked to Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 13.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Number of cases of severe human rights issues and incidents connected to the company. See Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 14. </t>
   </si>
   <si>
@@ -891,13 +822,220 @@
   </si>
   <si>
     <t xml:space="preserve">Amount of fines for violations of anti-corruption and anti-bribery laws. See Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 17. </t>
+  </si>
+  <si>
+    <t>Existence of a transparency policy. According to the OECD Guidelines for Multinational Enterprises, multinational companies should inform the public not only about their financial performance, but also about all of the important aspects of their business activities, such as how they are meeting social and environmental standards and what risks they foresee linked to their business activities.</t>
+  </si>
+  <si>
+    <t>Existence of policies in place to support/respect human rights and carry out due diligence to ensure that the business activities do not have a negative human rights impact.</t>
+  </si>
+  <si>
+    <t>Existence of policies in place to abolish all forms of child labour.</t>
+  </si>
+  <si>
+    <t>Existence of policies in place to abolish all forms of forced labour.</t>
+  </si>
+  <si>
+    <t>Existence of policies in place to eliminate discrimination in the workplace.</t>
+  </si>
+  <si>
+    <t>Existence of policies and procedures in place to apply fair business, marketing and advertising practices and to guarantee the safety and quality of the goods and services.</t>
+  </si>
+  <si>
+    <t>Existence of policies and procedures in place to permit the transfer and rapid dissemination of technologies and expertise.</t>
+  </si>
+  <si>
+    <t>Existence of policies and procedures in place related to fair competition and anti-competitive cartels.</t>
+  </si>
+  <si>
+    <t>Involvement in a violation of OECD Guidelines for Multinational Enterprises for Taxation: In the field of taxation, multinational enterprises should make their contribution to public finances within the framework of applicable law and regulations, in accordance with the tax rules and regulations of the host countries, and should cooperate with the tax authorities.</t>
+  </si>
+  <si>
+    <t>Does the company have policies and procedures for water management? (See Regulation (EU) 2022/1288, Annex I, table 2, indicator nr. 7.) If yes, please share the relevant documents with us.</t>
+  </si>
+  <si>
+    <t>Does the company have sites or operations that are located, either partially or entirely, in or near primary forests and other wooded areas where their activities have a negative impact on these environments? Refer to Regulation (EU) 2022/1288, Annex I, table 1, indicator number 7 for more details.</t>
+  </si>
+  <si>
+    <t>Does the company have sites or operations that are partially or fully located in or near protected areas, where their activities adversely impact these regions? For further details, please refer to Regulation (EU) 2022/1288, Annex I, table 1, indicator number 7.</t>
+  </si>
+  <si>
+    <t>Does the company have sites or operations located in or near areas designated for the protection of species, including flora and fauna, where their activities lead to the deterioration of natural habitats and disturb the species for which these areas have been designated? For more information, please refer to Regulation (EU) 2022/1288, Annex I, table 1, indicator number 7, and Annex I, item 18(a).</t>
+  </si>
+  <si>
+    <t>Does the company have sites or operations that are partially or fully situated in areas of highly biodiverse grassland, which may be categorized as either: (i) natural grassland, meaning areas that would remain grassland without human intervention and preserve natural species composition and ecological characteristics; or (ii) non-natural grassland, meaning areas that would no longer be grassland without human intervention but are species-rich and not degraded, unless it is demonstrated that harvesting the raw material is essential to maintain its grassland status?</t>
+  </si>
+  <si>
+    <t>Does the company have an environmental policy? If yes, please share the policy with us.</t>
+  </si>
+  <si>
+    <t>Does the company have a transparency policy? If yes, please share the policy with us. According to the OECD Guidelines for Multinational Enterprises, multinational companies should inform the public not only about their financial performance, but also about all of the important aspects of their business activities, such as how they are meeting social and environmental standards and what risks they foresee linked to their business activities.</t>
+  </si>
+  <si>
+    <t>Does the company have policies in place to support/respect human rights and carry out due diligence to ensure that the business activities do not have a negative human rights impact? If yes, please share the relevant documents with us.</t>
+  </si>
+  <si>
+    <t>Does the company have policies in place to abolish all forms of child labour? If yes, please share the policy with us.</t>
+  </si>
+  <si>
+    <t>Does the company have policies in place to abolish all forms of forced labour? If yes, please share the policy with us.</t>
+  </si>
+  <si>
+    <t>Does the company have policies in place to eliminate discrimination in the workplace? If yes, please share the policy with us.</t>
+  </si>
+  <si>
+    <t>Does the company have a policy on anti-corruption and anti-bribery consistent with the United Nations Convention against Corruption? (See Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 15.) If yes, please share the policy with us.</t>
+  </si>
+  <si>
+    <t>Does the company have policies and procedures in place to apply fair business, marketing and advertising practices and to guarantee the safety and quality of the goods and services? If yes, please share the relevant documents with us.</t>
+  </si>
+  <si>
+    <t>Does the company have policies and procedures in place to permit the transfer and rapid dissemination of technologies and expertise? If yes, please share the relevant documents with us.</t>
+  </si>
+  <si>
+    <t>Does the company have policies and procedures in place related to fair competition and anti-competitive cartels? If yes, please share the relevant documents with us.</t>
+  </si>
+  <si>
+    <t>Does the company have a policy to monitor compliance with the UNGC principles or OECD Guidelines for Multinational Enterprises? (See Regulation (EU) 2022/1288, Annex I, top (22) and table 1, indicator nr. 11.) If yes, please share the relevant documents with us.</t>
+  </si>
+  <si>
+    <t>Does the company have grievance/complaints handling mechanisms to address violations of the UNGC principles or OECD Guidelines for Multinational Enterprises? (See Regulation (EU) 2022/1288, Annex I, top (22) and table 1, indicator nr. 11.) If yes, please share the policy with us.</t>
+  </si>
+  <si>
+    <t>Does the company have any policies or procedures for carbon emission reduction aimed at aligning with the Paris Agreement? (See Regulation (EU) 2022/1288, Annex I, table 2, indicator nr. 4.) If yes, please share the relevant documents with us.</t>
+  </si>
+  <si>
+    <t>Does the company have securities in investments not certified as green under a future EU legal act setting up an EU Green Bond Standard?</t>
+  </si>
+  <si>
+    <t>Sites or operations that are located, either partially or entirely, in "areas of high water stress", i.e. in regions where the percentage of total water withdrawn is high (40-80%) or extremely high (greater than 80%), without a water management policy. See Regulation (EU) 2022/1288, Annex I, top (13) and table 2, indicator nr. 8.</t>
+  </si>
+  <si>
+    <t>Involvements in manufacture of pesticides and other agrochemical products. See Regulation (EU) 2022/1288, Annex I, table 2, indicator nr. 9 and Regulation (EC) No 1893/2006, Annex I, Division 20.2.</t>
+  </si>
+  <si>
+    <t>Is the company involved in manufacture of pesticides and other agrochemical products? See Regulation (EU) 2022/1288, Annex I, table 2, indicator nr. 9 and Regulation (EC) No 1893/2006, Annex I, Division 20.2.</t>
+  </si>
+  <si>
+    <t>Is the company involved in activities, which cause land degradation, desertification or soil sealing? See Regulation (EU) 2022/1288, Annex I, table 2, indicator nr. 10.</t>
+  </si>
+  <si>
+    <t>Does the company have sustainable land or agriculture practices or policies? (See Regulation (EU) 2022/1288, Annex I, table 2, indicator nr. 11.) If yes, please share the relevant documents with us.</t>
+  </si>
+  <si>
+    <t>Does the company have sustainable oceans or seas practices or policies? (See Regulation (EU) 2022/1288, Annex I, table 2, indicator nr. 12.) If yes, please share the relevant documents with us.</t>
+  </si>
+  <si>
+    <t>Does the company have operations, which affect threatened species? See Regulation (EU) 2022/1288, Annex I, table 2, indicator nr. 14.1 .</t>
+  </si>
+  <si>
+    <t>Does the company have a biodiversity protection policy that encompasses operational sites owned, leased, managed in, or adjacent to a protected area or an area of high biodiversity value outside protected areas? (See Regulation (EU) 2022/1288, Annex I, table 2, indicator nr. 14.2.) If yes, please share the policy with us.</t>
+  </si>
+  <si>
+    <t>Does the company have a policy to address deforestation? If yes, please share the policy with us. "Deforestation" means the human-induced conversion of forested land to non-forested land, which can be permanent, when this change is definitive, or temporary when this change is part of a cycle that includes natural or assisted regeneration, according to the Intergovernmental Science-Policy Platform on Biodiversity and Ecosystem Services (IPBES) as referred to in paragraph 100 of Decision No 1386/2013/EU of the European Parliament and of the Council. See Regulation (EU) 2022/1288, Annex I, table 2, indicator nr. 15.</t>
+  </si>
+  <si>
+    <t>Possession of securities in investments that are not certified as green under a future EU legal act setting up an EU Green Bond Standard.</t>
+  </si>
+  <si>
+    <t>Does the company have a workplace accident prevention policy? (See Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 1.) If yes, please share the policy with us.</t>
+  </si>
+  <si>
+    <t>Does the company have a supplier code of conduct addressing unsafe working conditions, precarious work, child labor, and forced labor? (See Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 4.) If yes, please share the document with us.</t>
+  </si>
+  <si>
+    <t>Does the company have a grievance/complaints handling mechanism related to employee matters? See Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 5.</t>
+  </si>
+  <si>
+    <t>Does the company have a policy on the protection of whistleblowers? (See Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 6.) If yes, please share the policy with us.</t>
+  </si>
+  <si>
+    <t>Does the company have a human rights policy? (See Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 9.) If yes, please share the policy with us.</t>
+  </si>
+  <si>
+    <t>Reported incidents of child labor within own operations or supply chain. Linked to Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 12.</t>
+  </si>
+  <si>
+    <t>Reported incidents of forced or compulsory labor within own operations or supply chain. Linked to Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 13.</t>
+  </si>
+  <si>
+    <t>Does the company have due diligence processes to identify, prevent, mitigate and address adverse human rights impacts? See Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 10.</t>
+  </si>
+  <si>
+    <t>Does the company have reported incidents of child labor within own operations or supply chain? Linked to Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 12.</t>
+  </si>
+  <si>
+    <t>Does the company have reported incidents of forced or compulsory labor within own operations or supply chain? Linked to Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 13.</t>
+  </si>
+  <si>
+    <t>Does the company have a policy against trafficking in human beings? (See Regulation (EU) 2022/1288, Annex I, table 3, indicator nr. 11.)  If yes, please share the policy with us.</t>
+  </si>
+  <si>
+    <t>Does the company abide by the ILO Core Labour Standards?</t>
+  </si>
+  <si>
+    <t>Has the company been involved in Human Rights related legal proceedings?</t>
+  </si>
+  <si>
+    <t>Has the company been involved in corruption-related legal proceedings?</t>
+  </si>
+  <si>
+    <t>Is the company ISO 14001 certified (Environmental Management)? If yes, please share the certificate with us.</t>
+  </si>
+  <si>
+    <t>Please select any sector(s) applicable activities (NACE Codes A-H, L).</t>
+  </si>
+  <si>
+    <t>Is the company involved in a violation of OECD Guidelines for Multinational Enterprises for Taxation? In the field of taxation, multinational enterprises should make their contribution to public finances within the framework of applicable law and regulations, in accordance with the tax rules and regulations of the host countries, and should cooperate with the tax authorities.</t>
+  </si>
+  <si>
+    <t>Is the company involved in the manufacture or selling of controversial weapons such as anti-personnel mines, cluster munitions, chemical weapons and biological weapons? See Regulation (EU) 2022/1288, Annex I, table 1, indicator nr. 14.</t>
+  </si>
+  <si>
+    <t>Does the company have sites or operations that are located, either partially or entirely, in "areas of high water stress", i.e. in regions where the percentage of total water withdrawn is high (40-80%) or extremely high (greater than 80%), without a water management policy? See Regulation (EU) 2022/1288, Annex I, top (13) and table 2, indicator nr. 8.</t>
+  </si>
+  <si>
+    <t>Does the company derive any revenues from exploration, mining, extraction, production, processing, storage, refining or distribution, including transportation, storage and trade, of fossil fuels? (Fossil fuels mean non-renewable carbon-based energy sources such as solid fuels, natural gas and oil.) See also Regulation (EU) 2022/1288, Annex I, top (5).</t>
+  </si>
+  <si>
+    <t>Tonnes of scope 1 GHG emissions per million EUR revenue. Scope 1 carbon emissions are emissions generated from sources that are controlled by the company that issues the underlying assets (equity share approach preferably used for emissions).</t>
+  </si>
+  <si>
+    <t>Tonnes of scope 2 GHG emissions per million EUR revenue. Scope 2 emissions refer to those generated from the consumption of purchased electricity, steam, or other energy sources produced upstream by external entities or companies. Preferably, these should be calculated using the location-based method and the equity share approach for emissions.</t>
+  </si>
+  <si>
+    <t>Tonnes of scope 3 GHG emissions per million EUR revenue. Scope 3 emissions encompass all indirect upstream and downstream emissions not covered by Scope 2. Preferably, the equity share approach should be used for calculating these emissions.</t>
+  </si>
+  <si>
+    <t>Tonnes of scope 4 GHG emissions per million EUR revenue. As per the GHG Protocol, Scope 4 refers to emissions avoided when a product is used as a substitute for other goods or services, providing the same functions with a lower carbon footprint.</t>
+  </si>
+  <si>
+    <t>Total revenue in EUR for the financial year. i.e., income arising in the course of an entity's ordinary activities, the amounts derived from the sale of products and the provision of services after deducting sales rebates and value added tax and other taxes directly linked to turnover. Overall turnover is equivalent to a firm's total revenues over some period of time.</t>
+  </si>
+  <si>
+    <t>Tonnes / €M Enterprise Value</t>
+  </si>
+  <si>
+    <t>Tonnes of GHG emissions per million EUR enterprise value.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The enterprise value in EUR, i.e. the sum, at fiscal year-end, of the market capitalisation of ordinary shares, the market capitalisation of preferred shares, the book value of total debt and non-controlling interests, without the deduction of cash or cash equivalents. See also Regulation (EU) 2022/1288, Annex I, top (4). </t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>Tonnes of GHG emissions per million EUR revenue, preferably calculated using the location-based method and the equity share approach for emissions.</t>
+  </si>
+  <si>
+    <t>Amount in cubic meters of fresh water used per million EUR revenue. See Regulation (EU) 2022/1288, Annex I, table 2, indicator nr. 6.1.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -939,13 +1077,32 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -1024,14 +1181,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
@@ -1048,22 +1202,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1072,6 +1214,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1389,66 +1571,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}">
   <dimension ref="A1:M114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F108" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M129" sqref="M129"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E112" sqref="E112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.73046875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.73046875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="61.73046875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="255.73046875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.73046875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.1328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.73046875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.7265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="61.7265625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="54.453125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="2.6328125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="24.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1328125" style="3"/>
+    <col min="14" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1462,16 +1644,16 @@
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="D2" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1497,10 +1679,10 @@
       <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -1529,10 +1711,10 @@
       <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="F4" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -1561,10 +1743,10 @@
       <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="14" t="s">
         <v>23</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -1578,7 +1760,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="42.75">
+    <row r="6" spans="1:13" ht="43.5">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1591,10 +1773,10 @@
       <c r="D6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="E6" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="F6" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -1608,7 +1790,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="57">
+    <row r="7" spans="1:13" ht="72.5">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1621,10 +1803,10 @@
       <c r="D7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="F7" s="1"/>
+      <c r="E7" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="F7" s="14"/>
       <c r="G7" s="1" t="s">
         <v>28</v>
       </c>
@@ -1636,7 +1818,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="28.5">
+    <row r="8" spans="1:13" ht="29">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1649,10 +1831,10 @@
       <c r="D8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="E8" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -1666,7 +1848,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="28.5">
+    <row r="9" spans="1:13" ht="29">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1679,10 +1861,10 @@
       <c r="D9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="E9" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="F9" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -1696,7 +1878,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="28.5">
+    <row r="10" spans="1:13" ht="29">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1709,10 +1891,10 @@
       <c r="D10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="E10" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="F10" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -1726,7 +1908,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="42.75">
+    <row r="11" spans="1:13" ht="43.5">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1736,13 +1918,13 @@
       <c r="C11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="E11" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="F11" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -1756,7 +1938,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="42.75">
+    <row r="12" spans="1:13" ht="43.5">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1766,13 +1948,13 @@
       <c r="C12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="E12" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="F12" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -1786,7 +1968,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="42.75">
+    <row r="13" spans="1:13" ht="43.5">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1799,10 +1981,10 @@
       <c r="D13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="E13" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="F13" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -1816,7 +1998,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="42.75">
+    <row r="14" spans="1:13" ht="43.5">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1827,12 +2009,12 @@
         <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="F14" s="1"/>
+        <v>160</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="F14" s="14"/>
       <c r="G14" s="1" t="s">
         <v>28</v>
       </c>
@@ -1844,7 +2026,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="42.75">
+    <row r="15" spans="1:13" ht="43.5">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1855,12 +2037,12 @@
         <v>26</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="F15" s="1"/>
+        <v>161</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="F15" s="14"/>
       <c r="G15" s="1" t="s">
         <v>28</v>
       </c>
@@ -1872,7 +2054,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="28.5">
+    <row r="16" spans="1:13" ht="29">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1885,10 +2067,10 @@
       <c r="D16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="E16" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F16" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -1902,7 +2084,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="42.75">
+    <row r="17" spans="1:10" ht="43.5">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1912,13 +2094,13 @@
       <c r="C17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="F17" s="1"/>
+      <c r="D17" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="F17" s="14"/>
       <c r="G17" s="1" t="s">
         <v>28</v>
       </c>
@@ -1930,7 +2112,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="42.75">
+    <row r="18" spans="1:10" ht="43.5">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1940,13 +2122,13 @@
       <c r="C18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="F18" s="1"/>
+      <c r="D18" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="F18" s="14"/>
       <c r="G18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1958,7 +2140,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" ht="43.5">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1969,12 +2151,12 @@
         <v>26</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="F19" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="F19" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -1988,7 +2170,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="57">
+    <row r="20" spans="1:10" ht="72.5">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2001,22 +2183,22 @@
       <c r="D20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1" t="s">
-        <v>40</v>
+      <c r="E20" s="21" t="s">
+        <v>316</v>
+      </c>
+      <c r="F20" s="14"/>
+      <c r="G20" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="H20" s="1"/>
-      <c r="I20" s="1" t="s">
-        <v>14</v>
+      <c r="I20" s="18" t="s">
+        <v>317</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="71.25">
+    <row r="21" spans="1:10" ht="87">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2029,22 +2211,22 @@
       <c r="D21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1" t="s">
-        <v>40</v>
+      <c r="E21" s="17" t="s">
+        <v>313</v>
+      </c>
+      <c r="F21" s="14"/>
+      <c r="G21" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="H21" s="1"/>
-      <c r="I21" s="1" t="s">
-        <v>14</v>
+      <c r="I21" s="18" t="s">
+        <v>317</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="28.5">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2057,24 +2239,24 @@
       <c r="D22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="F22" s="1" t="s">
+      <c r="E22" s="21" t="s">
+        <v>315</v>
+      </c>
+      <c r="F22" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>28</v>
       </c>
       <c r="H22" s="1"/>
-      <c r="I22" s="1" t="s">
-        <v>43</v>
+      <c r="I22" s="23" t="s">
+        <v>314</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="42.75">
+    <row r="23" spans="1:10" ht="43.5">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2087,10 +2269,10 @@
       <c r="D23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="F23" s="1" t="s">
+      <c r="E23" s="21" t="s">
+        <v>318</v>
+      </c>
+      <c r="F23" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -2104,7 +2286,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="57">
+    <row r="24" spans="1:10" ht="58">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2115,12 +2297,12 @@
         <v>26</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="F24" s="1"/>
+        <v>162</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>309</v>
+      </c>
+      <c r="F24" s="14"/>
       <c r="G24" s="1" t="s">
         <v>28</v>
       </c>
@@ -2132,7 +2314,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="85.5">
+    <row r="25" spans="1:10" ht="87">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2143,12 +2325,12 @@
         <v>26</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="F25" s="1"/>
+        <v>163</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>310</v>
+      </c>
+      <c r="F25" s="14"/>
       <c r="G25" s="1" t="s">
         <v>28</v>
       </c>
@@ -2160,7 +2342,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="57">
+    <row r="26" spans="1:10" ht="58">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2171,12 +2353,12 @@
         <v>26</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>203</v>
-      </c>
-      <c r="F26" s="1"/>
+        <v>164</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="F26" s="14"/>
       <c r="G26" s="1" t="s">
         <v>28</v>
       </c>
@@ -2188,7 +2370,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="57">
+    <row r="27" spans="1:10" ht="58">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2199,12 +2381,12 @@
         <v>26</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>204</v>
-      </c>
-      <c r="F27" s="1"/>
+        <v>165</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>312</v>
+      </c>
+      <c r="F27" s="14"/>
       <c r="G27" s="1" t="s">
         <v>28</v>
       </c>
@@ -2216,7 +2398,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="71.25">
+    <row r="28" spans="1:10" ht="159.5">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2229,12 +2411,14 @@
       <c r="D28" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="F28" s="1"/>
+      <c r="E28" s="22" t="s">
+        <v>308</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>187</v>
+      </c>
       <c r="G28" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>14</v>
@@ -2248,27 +2432,27 @@
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="7" t="s">
+      <c r="D29" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="F29" s="14"/>
+      <c r="G29" s="6" t="s">
         <v>28</v>
       </c>
       <c r="H29" s="1"/>
-      <c r="I29" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="J29" s="7" t="s">
+      <c r="I29" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="J29" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2276,31 +2460,31 @@
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="7" t="s">
+      <c r="D30" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="F30" s="14"/>
+      <c r="G30" s="6" t="s">
         <v>28</v>
       </c>
       <c r="H30" s="1"/>
-      <c r="I30" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="J30" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="71.25">
+      <c r="I30" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="72.5">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2313,10 +2497,10 @@
       <c r="D31" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="F31" s="1"/>
+      <c r="E31" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="F31" s="14"/>
       <c r="G31" s="1" t="s">
         <v>28</v>
       </c>
@@ -2330,7 +2514,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="71.25">
+    <row r="32" spans="1:10" ht="72.5">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2343,10 +2527,10 @@
       <c r="D32" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="F32" s="1"/>
+      <c r="E32" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="F32" s="14"/>
       <c r="G32" s="1" t="s">
         <v>28</v>
       </c>
@@ -2360,7 +2544,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="42.75">
+    <row r="33" spans="1:10" ht="43.5">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2373,10 +2557,10 @@
       <c r="D33" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="F33" s="1" t="s">
+      <c r="E33" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="F33" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G33" s="1" t="s">
@@ -2392,7 +2576,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" ht="29">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2405,10 +2589,10 @@
       <c r="D34" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F34" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G34" s="1" t="s">
@@ -2424,7 +2608,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="42.75">
+    <row r="35" spans="1:10" ht="43.5">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2437,10 +2621,10 @@
       <c r="D35" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E35" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="F35" s="1" t="s">
+      <c r="E35" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="F35" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G35" s="1" t="s">
@@ -2456,7 +2640,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="28.5">
+    <row r="36" spans="1:10" ht="29">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2469,10 +2653,10 @@
       <c r="D36" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E36" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="F36" s="1" t="s">
+      <c r="E36" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="F36" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G36" s="1" t="s">
@@ -2498,13 +2682,15 @@
       <c r="C37" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E37" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="F37" s="1"/>
+      <c r="E37" s="23" t="s">
+        <v>304</v>
+      </c>
+      <c r="F37" s="24" t="s">
+        <v>195</v>
+      </c>
       <c r="G37" s="1" t="s">
         <v>58</v>
       </c>
@@ -2518,7 +2704,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="99.75">
+    <row r="38" spans="1:10" ht="101.5">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2531,10 +2717,10 @@
       <c r="D38" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E38" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="F38" s="1"/>
+      <c r="E38" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="F38" s="14"/>
       <c r="G38" s="1" t="s">
         <v>28</v>
       </c>
@@ -2548,7 +2734,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="57">
+    <row r="39" spans="1:10" ht="81" customHeight="1">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2561,12 +2747,14 @@
       <c r="D39" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E39" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="F39" s="1"/>
+      <c r="E39" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="F39" s="25" t="s">
+        <v>197</v>
+      </c>
       <c r="G39" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>14</v>
@@ -2578,7 +2766,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="57">
+    <row r="40" spans="1:10" ht="58">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2591,12 +2779,14 @@
       <c r="D40" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E40" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="F40" s="1"/>
+      <c r="E40" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="F40" s="25" t="s">
+        <v>198</v>
+      </c>
       <c r="G40" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>14</v>
@@ -2608,7 +2798,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="85.5">
+    <row r="41" spans="1:10" ht="101.5">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2621,12 +2811,14 @@
       <c r="D41" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E41" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="F41" s="1"/>
+      <c r="E41" s="25" t="s">
+        <v>263</v>
+      </c>
+      <c r="F41" s="26" t="s">
+        <v>199</v>
+      </c>
       <c r="G41" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>14</v>
@@ -2638,7 +2830,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="114">
+    <row r="42" spans="1:10" ht="130.5">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2651,12 +2843,14 @@
       <c r="D42" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E42" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="F42" s="1"/>
+      <c r="E42" s="25" t="s">
+        <v>264</v>
+      </c>
+      <c r="F42" s="25" t="s">
+        <v>200</v>
+      </c>
       <c r="G42" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>14</v>
@@ -2668,7 +2862,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="57">
+    <row r="43" spans="1:10" ht="72.5">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2681,10 +2875,10 @@
       <c r="D43" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E43" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="F43" s="1" t="s">
+      <c r="E43" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="F43" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G43" s="1" t="s">
@@ -2700,7 +2894,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="142.5">
+    <row r="44" spans="1:10" ht="159.5">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2713,10 +2907,10 @@
       <c r="D44" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E44" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="F44" s="1"/>
+      <c r="E44" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="F44" s="14"/>
       <c r="G44" s="1" t="s">
         <v>28</v>
       </c>
@@ -2730,7 +2924,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" ht="29">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2743,12 +2937,14 @@
       <c r="D45" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E45" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="F45" s="1"/>
+      <c r="E45" s="27" t="s">
+        <v>301</v>
+      </c>
+      <c r="F45" s="24" t="s">
+        <v>203</v>
+      </c>
       <c r="G45" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>14</v>
@@ -2773,12 +2969,14 @@
       <c r="D46" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E46" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="F46" s="1"/>
+      <c r="E46" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="F46" s="24" t="s">
+        <v>204</v>
+      </c>
       <c r="G46" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>14</v>
@@ -2790,7 +2988,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" ht="29">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2803,12 +3001,14 @@
       <c r="D47" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E47" s="16" t="s">
-        <v>223</v>
-      </c>
-      <c r="F47" s="1"/>
+      <c r="E47" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="F47" s="24" t="s">
+        <v>205</v>
+      </c>
       <c r="G47" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>14</v>
@@ -2820,7 +3020,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" ht="29">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2833,12 +3033,14 @@
       <c r="D48" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E48" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="F48" s="1"/>
+      <c r="E48" s="27" t="s">
+        <v>302</v>
+      </c>
+      <c r="F48" s="24" t="s">
+        <v>206</v>
+      </c>
       <c r="G48" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>14</v>
@@ -2850,7 +3052,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" ht="101.5">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2863,12 +3065,14 @@
       <c r="D49" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F49" s="1"/>
+      <c r="E49" s="26" t="s">
+        <v>266</v>
+      </c>
+      <c r="F49" s="27" t="s">
+        <v>251</v>
+      </c>
       <c r="G49" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>14</v>
@@ -2880,7 +3084,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" ht="58">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2891,14 +3095,16 @@
         <v>70</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F50" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="E50" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="F50" s="27" t="s">
+        <v>252</v>
+      </c>
       <c r="G50" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>14</v>
@@ -2910,7 +3116,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" ht="29">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2921,14 +3127,16 @@
         <v>70</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F51" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="E51" s="26" t="s">
+        <v>268</v>
+      </c>
+      <c r="F51" s="27" t="s">
+        <v>253</v>
+      </c>
       <c r="G51" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>14</v>
@@ -2940,7 +3148,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" ht="29">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2951,14 +3159,16 @@
         <v>70</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F52" s="1"/>
+        <v>78</v>
+      </c>
+      <c r="E52" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="F52" s="26" t="s">
+        <v>254</v>
+      </c>
       <c r="G52" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>14</v>
@@ -2970,7 +3180,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" ht="29">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -2981,14 +3191,16 @@
         <v>70</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F53" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="E53" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="F53" s="26" t="s">
+        <v>255</v>
+      </c>
       <c r="G53" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>14</v>
@@ -3000,7 +3212,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" ht="29">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3011,14 +3223,16 @@
         <v>70</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E54" s="16" t="s">
-        <v>225</v>
-      </c>
-      <c r="F54" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="E54" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="F54" s="24" t="s">
+        <v>207</v>
+      </c>
       <c r="G54" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>14</v>
@@ -3030,7 +3244,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="42.75">
+    <row r="55" spans="1:10" ht="58">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3041,14 +3255,16 @@
         <v>70</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="F55" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="E55" s="28" t="s">
+        <v>271</v>
+      </c>
+      <c r="F55" s="28" t="s">
+        <v>208</v>
+      </c>
       <c r="G55" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>14</v>
@@ -3060,7 +3276,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" ht="58">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3071,14 +3287,16 @@
         <v>70</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F56" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="E56" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="F56" s="26" t="s">
+        <v>256</v>
+      </c>
       <c r="G56" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>14</v>
@@ -3090,7 +3308,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" ht="43.5">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3101,14 +3319,16 @@
         <v>70</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F57" s="1"/>
+        <v>83</v>
+      </c>
+      <c r="E57" s="26" t="s">
+        <v>273</v>
+      </c>
+      <c r="F57" s="26" t="s">
+        <v>257</v>
+      </c>
       <c r="G57" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>14</v>
@@ -3120,7 +3340,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" ht="43.5">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3131,14 +3351,16 @@
         <v>70</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F58" s="1"/>
+        <v>84</v>
+      </c>
+      <c r="E58" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="F58" s="26" t="s">
+        <v>258</v>
+      </c>
       <c r="G58" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>14</v>
@@ -3150,7 +3372,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" ht="101.5">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3161,14 +3383,16 @@
         <v>70</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E59" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="F59" s="1"/>
+        <v>85</v>
+      </c>
+      <c r="E59" s="27" t="s">
+        <v>305</v>
+      </c>
+      <c r="F59" s="27" t="s">
+        <v>259</v>
+      </c>
       <c r="G59" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>14</v>
@@ -3180,7 +3404,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="42.75">
+    <row r="60" spans="1:10" ht="58">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -3191,14 +3415,16 @@
         <v>70</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="F60" s="1"/>
+        <v>86</v>
+      </c>
+      <c r="E60" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="F60" s="28" t="s">
+        <v>209</v>
+      </c>
       <c r="G60" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>14</v>
@@ -3210,7 +3436,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="57">
+    <row r="61" spans="1:10" ht="58">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -3221,14 +3447,16 @@
         <v>70</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="F61" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="E61" s="28" t="s">
+        <v>276</v>
+      </c>
+      <c r="F61" s="28" t="s">
+        <v>210</v>
+      </c>
       <c r="G61" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>14</v>
@@ -3251,12 +3479,12 @@
         <v>70</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F62" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E62" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="F62" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G62" s="1" t="s">
@@ -3283,12 +3511,12 @@
         <v>70</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F63" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F63" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G63" s="1" t="s">
@@ -3304,7 +3532,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="57">
+    <row r="64" spans="1:10" ht="58">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -3315,12 +3543,12 @@
         <v>70</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="F64" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="F64" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G64" s="1" t="s">
@@ -3334,7 +3562,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" ht="29">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -3345,14 +3573,14 @@
         <v>70</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F65" s="1"/>
+        <v>150</v>
+      </c>
+      <c r="E65" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="F65" s="14"/>
       <c r="G65" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>48</v>
@@ -3373,14 +3601,14 @@
         <v>70</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="F66" s="1"/>
+        <v>152</v>
+      </c>
+      <c r="E66" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="F66" s="14"/>
       <c r="G66" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>48</v>
@@ -3390,7 +3618,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" ht="29">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -3401,14 +3629,14 @@
         <v>70</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="F67" s="1"/>
+        <v>154</v>
+      </c>
+      <c r="E67" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="F67" s="14"/>
       <c r="G67" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>48</v>
@@ -3429,14 +3657,14 @@
         <v>70</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F68" s="1"/>
+        <v>156</v>
+      </c>
+      <c r="E68" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="F68" s="14"/>
       <c r="G68" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>48</v>
@@ -3446,7 +3674,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="28.5">
+    <row r="69" spans="1:10" ht="43.5">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -3457,17 +3685,17 @@
         <v>70</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="E69" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="F69" s="1"/>
+        <v>158</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="F69" s="14"/>
       <c r="G69" s="1" t="s">
         <v>28</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="I69" s="1" t="s">
         <v>54</v>
@@ -3476,7 +3704,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="28.5">
+    <row r="70" spans="1:10" ht="43.5">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -3487,17 +3715,17 @@
         <v>70</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E70" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="F70" s="1"/>
+        <v>159</v>
+      </c>
+      <c r="E70" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="F70" s="14"/>
       <c r="G70" s="1" t="s">
         <v>28</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="I70" s="1" t="s">
         <v>54</v>
@@ -3506,7 +3734,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="42.75">
+    <row r="71" spans="1:10" ht="58">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -3517,16 +3745,16 @@
         <v>70</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E71" s="17" t="s">
-        <v>232</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>14</v>
+        <v>95</v>
+      </c>
+      <c r="E71" s="25" t="s">
+        <v>306</v>
+      </c>
+      <c r="F71" s="25" t="s">
+        <v>214</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>14</v>
@@ -3538,7 +3766,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="85.5">
+    <row r="72" spans="1:10" ht="87">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -3546,15 +3774,15 @@
         <v>25</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E72" s="17" t="s">
-        <v>233</v>
-      </c>
-      <c r="F72" s="1"/>
+        <v>97</v>
+      </c>
+      <c r="E72" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="F72" s="14"/>
       <c r="G72" s="1" t="s">
         <v>28</v>
       </c>
@@ -3568,7 +3796,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="114">
+    <row r="73" spans="1:10" ht="130.5">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -3576,15 +3804,15 @@
         <v>25</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E73" s="17" t="s">
-        <v>234</v>
-      </c>
-      <c r="F73" s="1"/>
+        <v>98</v>
+      </c>
+      <c r="E73" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="F73" s="14"/>
       <c r="G73" s="1" t="s">
         <v>28</v>
       </c>
@@ -3598,7 +3826,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="114">
+    <row r="74" spans="1:10" ht="116">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -3606,15 +3834,15 @@
         <v>25</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E74" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="F74" s="1"/>
+        <v>99</v>
+      </c>
+      <c r="E74" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="F74" s="14"/>
       <c r="G74" s="1" t="s">
         <v>28</v>
       </c>
@@ -3628,7 +3856,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="42.75">
+    <row r="75" spans="1:10" ht="58">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -3636,17 +3864,19 @@
         <v>25</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E75" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="F75" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="E75" s="28" t="s">
+        <v>277</v>
+      </c>
+      <c r="F75" s="28" t="s">
+        <v>218</v>
+      </c>
       <c r="G75" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>14</v>
@@ -3658,7 +3888,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="42.75">
+    <row r="76" spans="1:10" ht="43.5">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -3669,12 +3899,12 @@
         <v>46</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E76" s="17" t="s">
-        <v>237</v>
-      </c>
-      <c r="F76" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E76" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="F76" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G76" s="1" t="s">
@@ -3690,7 +3920,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="42.75">
+    <row r="77" spans="1:10" ht="43.5">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -3701,12 +3931,12 @@
         <v>46</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E77" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="F77" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E77" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="F77" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G77" s="1" t="s">
@@ -3722,7 +3952,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="28.5">
+    <row r="78" spans="1:10" ht="29">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -3733,12 +3963,12 @@
         <v>46</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E78" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="F78" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E78" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="F78" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G78" s="1" t="s">
@@ -3754,7 +3984,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="28.5">
+    <row r="79" spans="1:10" ht="29">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -3765,12 +3995,12 @@
         <v>46</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E79" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="F79" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E79" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="F79" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G79" s="1" t="s">
@@ -3786,7 +4016,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="28.5">
+    <row r="80" spans="1:10" ht="29">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -3797,12 +4027,12 @@
         <v>46</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E80" s="9" t="s">
-        <v>241</v>
-      </c>
-      <c r="F80" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E80" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="F80" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G80" s="1" t="s">
@@ -3818,7 +4048,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="42.75">
+    <row r="81" spans="1:10" ht="43.5">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -3829,12 +4059,12 @@
         <v>46</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E81" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="F81" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E81" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="F81" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G81" s="1" t="s">
@@ -3850,7 +4080,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="42.75">
+    <row r="82" spans="1:10" ht="43.5">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -3861,12 +4091,12 @@
         <v>46</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="F82" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E82" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="F82" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G82" s="1" t="s">
@@ -3882,7 +4112,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="28.5">
+    <row r="83" spans="1:10" ht="29">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -3893,12 +4123,12 @@
         <v>65</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E83" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="F83" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E83" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="F83" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G83" s="1" t="s">
@@ -3908,13 +4138,13 @@
         <v>48</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="J83" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="28.5">
+    <row r="84" spans="1:10" ht="29">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -3925,12 +4155,12 @@
         <v>65</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E84" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="F84" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E84" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="F84" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G84" s="1" t="s">
@@ -3940,13 +4170,13 @@
         <v>48</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="J84" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="42.75">
+    <row r="85" spans="1:10" ht="29">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -3957,12 +4187,12 @@
         <v>65</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E85" s="17" t="s">
-        <v>246</v>
-      </c>
-      <c r="F85" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E85" s="19" t="s">
+        <v>319</v>
+      </c>
+      <c r="F85" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G85" s="1" t="s">
@@ -3971,14 +4201,14 @@
       <c r="H85" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I85" s="1" t="s">
-        <v>119</v>
+      <c r="I85" s="29" t="s">
+        <v>112</v>
       </c>
       <c r="J85" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="28.5">
+    <row r="86" spans="1:10" ht="43.5">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -3989,14 +4219,16 @@
         <v>65</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E86" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="F86" s="1"/>
+        <v>113</v>
+      </c>
+      <c r="E86" s="28" t="s">
+        <v>260</v>
+      </c>
+      <c r="F86" s="28" t="s">
+        <v>228</v>
+      </c>
       <c r="G86" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>14</v>
@@ -4008,7 +4240,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="57">
+    <row r="87" spans="1:10" ht="87">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -4019,14 +4251,16 @@
         <v>65</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E87" s="17" t="s">
-        <v>248</v>
-      </c>
-      <c r="F87" s="1"/>
+        <v>114</v>
+      </c>
+      <c r="E87" s="25" t="s">
+        <v>307</v>
+      </c>
+      <c r="F87" s="25" t="s">
+        <v>279</v>
+      </c>
       <c r="G87" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>14</v>
@@ -4038,7 +4272,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="42.75">
+    <row r="88" spans="1:10" ht="58">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -4049,14 +4283,16 @@
         <v>60</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E88" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="F88" s="1"/>
+        <v>115</v>
+      </c>
+      <c r="E88" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="F88" s="28" t="s">
+        <v>280</v>
+      </c>
       <c r="G88" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>14</v>
@@ -4068,7 +4304,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="42.75">
+    <row r="89" spans="1:10" ht="43.5">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -4079,14 +4315,16 @@
         <v>60</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E89" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="F89" s="1"/>
+        <v>116</v>
+      </c>
+      <c r="E89" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="F89" s="28" t="s">
+        <v>229</v>
+      </c>
       <c r="G89" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>14</v>
@@ -4098,7 +4336,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="28.5">
+    <row r="90" spans="1:10" ht="43.5">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -4109,14 +4347,16 @@
         <v>60</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E90" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="F90" s="1"/>
+        <v>117</v>
+      </c>
+      <c r="E90" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="F90" s="28" t="s">
+        <v>230</v>
+      </c>
       <c r="G90" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>14</v>
@@ -4128,7 +4368,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="28.5">
+    <row r="91" spans="1:10" ht="43.5">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -4139,14 +4379,16 @@
         <v>60</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="F91" s="1"/>
+        <v>118</v>
+      </c>
+      <c r="E91" s="28" t="s">
+        <v>284</v>
+      </c>
+      <c r="F91" s="28" t="s">
+        <v>231</v>
+      </c>
       <c r="G91" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>14</v>
@@ -4158,7 +4400,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="57">
+    <row r="92" spans="1:10" ht="58">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -4169,12 +4411,12 @@
         <v>67</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E92" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="F92" s="1"/>
+        <v>119</v>
+      </c>
+      <c r="E92" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="F92" s="14"/>
       <c r="G92" s="1" t="s">
         <v>28</v>
       </c>
@@ -4188,7 +4430,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="28.5">
+    <row r="93" spans="1:10" ht="29">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -4199,14 +4441,16 @@
         <v>60</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E93" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="F93" s="1"/>
+        <v>120</v>
+      </c>
+      <c r="E93" s="28" t="s">
+        <v>285</v>
+      </c>
+      <c r="F93" s="28" t="s">
+        <v>233</v>
+      </c>
       <c r="G93" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>14</v>
@@ -4218,7 +4462,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="57">
+    <row r="94" spans="1:10" ht="72.5">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -4229,14 +4473,16 @@
         <v>60</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E94" s="17" t="s">
-        <v>255</v>
-      </c>
-      <c r="F94" s="1"/>
+        <v>121</v>
+      </c>
+      <c r="E94" s="25" t="s">
+        <v>286</v>
+      </c>
+      <c r="F94" s="25" t="s">
+        <v>234</v>
+      </c>
       <c r="G94" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>14</v>
@@ -4248,7 +4494,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="114">
+    <row r="95" spans="1:10" ht="145">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -4259,14 +4505,16 @@
         <v>60</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E95" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="F95" s="1"/>
+        <v>122</v>
+      </c>
+      <c r="E95" s="28" t="s">
+        <v>287</v>
+      </c>
+      <c r="F95" s="28" t="s">
+        <v>235</v>
+      </c>
       <c r="G95" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>14</v>
@@ -4278,7 +4526,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" ht="43.5">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -4286,17 +4534,19 @@
         <v>69</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F96" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="E96" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="F96" s="27" t="s">
+        <v>288</v>
+      </c>
       <c r="G96" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>14</v>
@@ -4308,7 +4558,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="28.5">
+    <row r="97" spans="1:10" ht="43.5">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -4319,14 +4569,16 @@
         <v>70</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E97" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="F97" s="1"/>
+        <v>125</v>
+      </c>
+      <c r="E97" s="28" t="s">
+        <v>289</v>
+      </c>
+      <c r="F97" s="28" t="s">
+        <v>236</v>
+      </c>
       <c r="G97" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>14</v>
@@ -4338,7 +4590,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="42.75">
+    <row r="98" spans="1:10" ht="58">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -4349,12 +4601,12 @@
         <v>70</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E98" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="F98" s="1"/>
+        <v>126</v>
+      </c>
+      <c r="E98" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="F98" s="14"/>
       <c r="G98" s="1" t="s">
         <v>28</v>
       </c>
@@ -4366,7 +4618,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" ht="29">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -4377,12 +4629,12 @@
         <v>70</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="F99" s="1"/>
+        <v>127</v>
+      </c>
+      <c r="E99" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="F99" s="14"/>
       <c r="G99" s="1" t="s">
         <v>28</v>
       </c>
@@ -4390,13 +4642,13 @@
         <v>48</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="J99" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="42.75">
+    <row r="100" spans="1:10" ht="58">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -4407,14 +4659,16 @@
         <v>70</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E100" s="17" t="s">
-        <v>259</v>
-      </c>
-      <c r="F100" s="1"/>
+        <v>129</v>
+      </c>
+      <c r="E100" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="F100" s="25" t="s">
+        <v>238</v>
+      </c>
       <c r="G100" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>14</v>
@@ -4426,7 +4680,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="42.75">
+    <row r="101" spans="1:10" ht="43.5">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -4437,14 +4691,16 @@
         <v>70</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E101" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="F101" s="1"/>
+        <v>130</v>
+      </c>
+      <c r="E101" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="F101" s="28" t="s">
+        <v>239</v>
+      </c>
       <c r="G101" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>14</v>
@@ -4456,7 +4712,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="28.5">
+    <row r="102" spans="1:10" ht="43.5">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -4467,14 +4723,16 @@
         <v>70</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E102" s="9" t="s">
-        <v>261</v>
-      </c>
-      <c r="F102" s="1"/>
+        <v>131</v>
+      </c>
+      <c r="E102" s="28" t="s">
+        <v>292</v>
+      </c>
+      <c r="F102" s="28" t="s">
+        <v>240</v>
+      </c>
       <c r="G102" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>14</v>
@@ -4486,7 +4744,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="28.5">
+    <row r="103" spans="1:10" ht="29">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -4497,14 +4755,14 @@
         <v>70</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E103" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="F103" s="1"/>
+        <v>132</v>
+      </c>
+      <c r="E103" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="F103" s="14"/>
       <c r="G103" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>48</v>
@@ -4516,7 +4774,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="42.75">
+    <row r="104" spans="1:10" ht="43.5">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -4527,14 +4785,14 @@
         <v>70</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E104" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="F104" s="1"/>
+        <v>133</v>
+      </c>
+      <c r="E104" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="F104" s="14"/>
       <c r="G104" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="H104" s="1" t="s">
         <v>48</v>
@@ -4546,9 +4804,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="57">
+    <row r="105" spans="1:10" ht="58">
       <c r="A105" s="1">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>69</v>
@@ -4557,12 +4815,12 @@
         <v>70</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E105" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="F105" s="1"/>
+        <v>134</v>
+      </c>
+      <c r="E105" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="F105" s="14"/>
       <c r="G105" s="1" t="s">
         <v>28</v>
       </c>
@@ -4574,25 +4832,27 @@
         <v>30</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="28.5">
+    <row r="106" spans="1:10" ht="43.5">
       <c r="A106" s="1">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E106" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="F106" s="1"/>
+        <v>136</v>
+      </c>
+      <c r="E106" s="28" t="s">
+        <v>293</v>
+      </c>
+      <c r="F106" s="28" t="s">
+        <v>244</v>
+      </c>
       <c r="G106" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H106" s="1" t="s">
         <v>14</v>
@@ -4604,25 +4864,27 @@
         <v>30</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="42.75">
+    <row r="107" spans="1:10" ht="43.5">
       <c r="A107" s="1">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E107" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="F107" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="E107" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="F107" s="28" t="s">
+        <v>245</v>
+      </c>
       <c r="G107" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H107" s="1" t="s">
         <v>14</v>
@@ -4634,25 +4896,27 @@
         <v>30</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="28.5">
+    <row r="108" spans="1:10" ht="43.5">
       <c r="A108" s="1">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E108" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="F108" s="1"/>
+        <v>138</v>
+      </c>
+      <c r="E108" s="28" t="s">
+        <v>299</v>
+      </c>
+      <c r="F108" s="28" t="s">
+        <v>246</v>
+      </c>
       <c r="G108" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H108" s="1" t="s">
         <v>14</v>
@@ -4664,25 +4928,27 @@
         <v>30</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="42.75">
+    <row r="109" spans="1:10" ht="43.5">
       <c r="A109" s="1">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E109" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="F109" s="1"/>
+        <v>139</v>
+      </c>
+      <c r="E109" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="F109" s="25" t="s">
+        <v>294</v>
+      </c>
       <c r="G109" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H109" s="1" t="s">
         <v>14</v>
@@ -4694,25 +4960,27 @@
         <v>30</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="42.75">
+    <row r="110" spans="1:10" ht="43.5">
       <c r="A110" s="1">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E110" s="17" t="s">
-        <v>269</v>
-      </c>
-      <c r="F110" s="1"/>
+        <v>140</v>
+      </c>
+      <c r="E110" s="25" t="s">
+        <v>298</v>
+      </c>
+      <c r="F110" s="25" t="s">
+        <v>295</v>
+      </c>
       <c r="G110" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H110" s="1" t="s">
         <v>14</v>
@@ -4724,25 +4992,25 @@
         <v>30</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="42.75">
+    <row r="111" spans="1:10" ht="43.5">
       <c r="A111" s="1">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E111" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="F111" s="1"/>
+        <v>141</v>
+      </c>
+      <c r="E111" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="F111" s="14"/>
       <c r="G111" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="H111" s="1" t="s">
         <v>48</v>
@@ -4754,27 +5022,27 @@
         <v>30</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="42.75">
+    <row r="112" spans="1:10" ht="43.5">
       <c r="A112" s="1">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E112" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="F112" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E112" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="F112" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="H112" s="1" t="s">
         <v>48</v>
@@ -4786,27 +5054,27 @@
         <v>30</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="42.75">
+    <row r="113" spans="1:10" ht="43.5">
       <c r="A113" s="1">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E113" s="9" t="s">
-        <v>272</v>
-      </c>
-      <c r="F113" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E113" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="F113" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="H113" s="1" t="s">
         <v>48</v>
@@ -4818,23 +5086,23 @@
         <v>30</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="28.5">
+    <row r="114" spans="1:10" ht="29">
       <c r="A114" s="1">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E114" s="18" t="s">
-        <v>273</v>
-      </c>
-      <c r="F114" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E114" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="F114" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G114" s="1" t="s">

</xml_diff>

<commit_message>
DALA-6204: PCAF Implementation (#1414)
Co-authored-by: Dennis Groh <173401487+dennis-dfine@users.noreply.github.com>
Co-authored-by: SimonHofmann12 <192322604+SimonHofmann12@users.noreply.github.com>
Co-authored-by: Fabian-dfine <Fabian-dfine@users.noreply.github.com>
Co-authored-by: KoenMoors-dfine <215665213+KoenMoors-dfine@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
+++ b/dataland-framework-toolbox/inputs/sfdr/sfdr.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93542\Dataland\dataland-framework-toolbox\inputs\sfdr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\dataland-repos\Dataland\dataland-framework-toolbox\inputs\sfdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE63FC7A-3394-4083-9A6D-85A70E689404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4BC214-88E7-401E-B17C-413AF5CEC83D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
+    <workbookView xWindow="-86" yWindow="0" windowWidth="16629" windowHeight="17880" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="2" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="436">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -593,18 +593,9 @@
     <t>The date the fiscal year ends.</t>
   </si>
   <si>
-    <t>Scope 1 greenhouse gas emissions, namely emissions generated from sources that are controlled by the company that issues the underlying assets (equity share approach preferably used).</t>
-  </si>
-  <si>
     <t>Scope 2 greenhouse gas emissions, namely emissions from the consumption of purchased electricity, steam, or other sources of energy generated upstream from the company that issues the underlying assets (preferably using the location-based method and equity share approach).</t>
   </si>
   <si>
-    <t>Scope 2 greenhouse gas emissions computed using the location-based method (equity share approach preferably used).</t>
-  </si>
-  <si>
-    <t>Scope 2 greenhouse gas emissions computed using the market-based method (equity share approach preferably used).</t>
-  </si>
-  <si>
     <t>Sum of scope 1 and 2 greenhouse gas emissions (computed preferably using the location-based method and equity share approach).</t>
   </si>
   <si>
@@ -1371,6 +1362,21 @@
   </si>
   <si>
     <t>TOTAL_AMOUNT_OF_REPORTED_FINES_OF_BRIBERY_AND_CORRUPTION</t>
+  </si>
+  <si>
+    <t>Greenhouse gas emissions</t>
+  </si>
+  <si>
+    <t>Scope 1 greenhouse gas emissions in tonnes, namely emissions generated from sources that are controlled by the company that issues the underlying assets (equity share approach preferably used).</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Scope 2 greenhouse gas emissions in tonnes from the consumption of purchased electricity, steam, or other sources of energy computed using the location-based method (equity share approach preferably used).</t>
+  </si>
+  <si>
+    <t>Scope 2 greenhouse gas emissions in tonnes from the consumption of purchased electricity, steam, or other sources of energy computed using the market-based method (equity share approach preferably used).</t>
   </si>
 </sst>
 </file>
@@ -1791,16 +1797,16 @@
   <dimension ref="A1:N114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="58.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="64.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="255.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.69140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.3828125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.53515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="255.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1817,7 +1823,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
@@ -1861,7 +1867,7 @@
         <v>148</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="F2" t="s">
         <v>172</v>
@@ -1899,7 +1905,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>17</v>
@@ -1937,7 +1943,7 @@
         <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F4" t="s">
         <v>173</v>
@@ -1975,7 +1981,7 @@
         <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>22</v>
@@ -2005,24 +2011,26 @@
         <v>25</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>26</v>
+        <v>431</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="F6" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>14</v>
+        <v>433</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="4"/>
+      <c r="I6" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="J6" s="4" t="s">
         <v>29</v>
       </c>
@@ -2044,10 +2052,10 @@
         <v>31</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="F7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
@@ -2069,29 +2077,40 @@
         <v>25</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>26</v>
+        <v>431</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>32</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="F8" t="s">
-        <v>176</v>
+        <v>434</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>14</v>
+        <v>433</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="4"/>
+      <c r="I8" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="J8" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>30</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="6" customFormat="1">
@@ -2102,29 +2121,40 @@
         <v>25</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>26</v>
+        <v>431</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>33</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F9" t="s">
-        <v>177</v>
+        <v>435</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>14</v>
+        <v>433</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="4"/>
+      <c r="I9" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="J9" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>30</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="6" customFormat="1">
@@ -2141,10 +2171,10 @@
         <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="F10" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>14</v>
@@ -2174,10 +2204,10 @@
         <v>35</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F11" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>14</v>
@@ -2207,10 +2237,10 @@
         <v>36</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F12" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>14</v>
@@ -2234,24 +2264,26 @@
         <v>25</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>26</v>
+        <v>431</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="F13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>14</v>
+        <v>433</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I13" s="4"/>
+      <c r="I13" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="J13" s="4" t="s">
         <v>29</v>
       </c>
@@ -2273,10 +2305,10 @@
         <v>160</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="F14" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4" t="s">
@@ -2304,10 +2336,10 @@
         <v>161</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="F15" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4" t="s">
@@ -2335,10 +2367,10 @@
         <v>38</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="F16" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>14</v>
@@ -2368,10 +2400,10 @@
         <v>146</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="F17" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4" t="s">
@@ -2399,10 +2431,10 @@
         <v>147</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="F18" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4" t="s">
@@ -2430,7 +2462,7 @@
         <v>169</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>170</v>
@@ -2463,10 +2495,10 @@
         <v>39</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F20" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4" t="s">
@@ -2474,7 +2506,7 @@
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>30</v>
@@ -2494,10 +2526,10 @@
         <v>41</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F21" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4" t="s">
@@ -2505,7 +2537,7 @@
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>30</v>
@@ -2525,10 +2557,10 @@
         <v>42</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="F22" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>14</v>
@@ -2538,7 +2570,7 @@
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="K22" s="4" t="s">
         <v>30</v>
@@ -2558,10 +2590,10 @@
         <v>44</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="F23" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>14</v>
@@ -2591,10 +2623,10 @@
         <v>162</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="F24" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="4" t="s">
@@ -2622,10 +2654,10 @@
         <v>163</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="F25" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="4" t="s">
@@ -2653,10 +2685,10 @@
         <v>164</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="F26" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4" t="s">
@@ -2684,10 +2716,10 @@
         <v>165</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="F27" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4" t="s">
@@ -2715,13 +2747,13 @@
         <v>45</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F28" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G28" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>149</v>
@@ -2748,10 +2780,10 @@
         <v>166</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F29" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="5" t="s">
@@ -2779,10 +2811,10 @@
         <v>168</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="F30" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="5" t="s">
@@ -2810,10 +2842,10 @@
         <v>47</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="F31" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="4" t="s">
@@ -2843,10 +2875,10 @@
         <v>50</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F32" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="4" t="s">
@@ -2876,10 +2908,10 @@
         <v>51</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="F33" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>14</v>
@@ -2911,7 +2943,7 @@
         <v>52</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>53</v>
@@ -2946,10 +2978,10 @@
         <v>55</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="F35" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>14</v>
@@ -2981,10 +3013,10 @@
         <v>56</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F36" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>14</v>
@@ -3016,13 +3048,13 @@
         <v>57</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G37" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H37" s="4" t="s">
         <v>58</v>
@@ -3051,10 +3083,10 @@
         <v>59</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F38" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="4" t="s">
@@ -3084,10 +3116,10 @@
         <v>101</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="F39" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>14</v>
@@ -3119,10 +3151,10 @@
         <v>102</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F40" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>14</v>
@@ -3154,10 +3186,10 @@
         <v>103</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F41" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>14</v>
@@ -3189,10 +3221,10 @@
         <v>104</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="F42" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>14</v>
@@ -3224,10 +3256,10 @@
         <v>105</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F43" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>14</v>
@@ -3259,10 +3291,10 @@
         <v>106</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="F44" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>14</v>
@@ -3294,10 +3326,10 @@
         <v>107</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F45" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>14</v>
@@ -3329,13 +3361,13 @@
         <v>61</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F46" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G46" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H46" s="4" t="s">
         <v>149</v>
@@ -3364,13 +3396,13 @@
         <v>62</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="F47" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="G47" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>149</v>
@@ -3399,13 +3431,13 @@
         <v>63</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="F48" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H48" s="4" t="s">
         <v>149</v>
@@ -3434,13 +3466,13 @@
         <v>64</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="F49" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G49" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H49" s="4" t="s">
         <v>149</v>
@@ -3469,13 +3501,13 @@
         <v>115</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="F50" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="G50" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H50" s="4" t="s">
         <v>149</v>
@@ -3504,13 +3536,13 @@
         <v>116</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="F51" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="G51" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>149</v>
@@ -3539,13 +3571,13 @@
         <v>117</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="F52" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="G52" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H52" s="4" t="s">
         <v>149</v>
@@ -3574,13 +3606,13 @@
         <v>118</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F53" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="G53" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>149</v>
@@ -3609,13 +3641,13 @@
         <v>120</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="F54" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G54" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>149</v>
@@ -3644,13 +3676,13 @@
         <v>121</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="F55" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G55" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H55" s="4" t="s">
         <v>149</v>
@@ -3679,13 +3711,13 @@
         <v>122</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="F56" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="G56" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="H56" s="4" t="s">
         <v>149</v>
@@ -3714,10 +3746,10 @@
         <v>66</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="F57" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>14</v>
@@ -3749,10 +3781,10 @@
         <v>108</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="F58" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>14</v>
@@ -3784,10 +3816,10 @@
         <v>110</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F59" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>14</v>
@@ -3819,10 +3851,10 @@
         <v>111</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="F60" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>14</v>
@@ -3854,13 +3886,13 @@
         <v>113</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F61" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="G61" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H61" s="4" t="s">
         <v>149</v>
@@ -3889,13 +3921,13 @@
         <v>114</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="F62" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G62" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="H62" s="4" t="s">
         <v>149</v>
@@ -3924,10 +3956,10 @@
         <v>68</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="F63" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G63" s="4"/>
       <c r="H63" s="4" t="s">
@@ -3957,10 +3989,10 @@
         <v>119</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="F64" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="4" t="s">
@@ -3990,10 +4022,10 @@
         <v>97</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="F65" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G65" s="4"/>
       <c r="H65" s="4" t="s">
@@ -4023,10 +4055,10 @@
         <v>98</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="F66" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G66" s="4"/>
       <c r="H66" s="4" t="s">
@@ -4056,10 +4088,10 @@
         <v>99</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="F67" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G67" s="4"/>
       <c r="H67" s="4" t="s">
@@ -4089,13 +4121,13 @@
         <v>100</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="F68" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G68" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H68" s="4" t="s">
         <v>149</v>
@@ -4124,13 +4156,13 @@
         <v>71</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="G69" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H69" s="4" t="s">
         <v>149</v>
@@ -4159,13 +4191,13 @@
         <v>72</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G70" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H70" s="4" t="s">
         <v>149</v>
@@ -4194,13 +4226,13 @@
         <v>73</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G71" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H71" s="4" t="s">
         <v>149</v>
@@ -4229,13 +4261,13 @@
         <v>74</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="G72" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H72" s="4" t="s">
         <v>149</v>
@@ -4264,13 +4296,13 @@
         <v>75</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H73" s="4" t="s">
         <v>149</v>
@@ -4299,13 +4331,13 @@
         <v>76</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="H74" s="4" t="s">
         <v>149</v>
@@ -4334,13 +4366,13 @@
         <v>77</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="H75" s="4" t="s">
         <v>149</v>
@@ -4369,13 +4401,13 @@
         <v>78</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H76" s="4" t="s">
         <v>149</v>
@@ -4404,13 +4436,13 @@
         <v>79</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H77" s="4" t="s">
         <v>149</v>
@@ -4439,13 +4471,13 @@
         <v>80</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G78" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H78" s="4" t="s">
         <v>149</v>
@@ -4474,13 +4506,13 @@
         <v>81</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F79" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G79" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H79" s="4" t="s">
         <v>149</v>
@@ -4509,13 +4541,13 @@
         <v>82</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="H80" s="4" t="s">
         <v>149</v>
@@ -4544,13 +4576,13 @@
         <v>83</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="H81" s="4" t="s">
         <v>149</v>
@@ -4579,13 +4611,13 @@
         <v>84</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="H82" s="4" t="s">
         <v>149</v>
@@ -4614,13 +4646,13 @@
         <v>85</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="H83" s="4" t="s">
         <v>149</v>
@@ -4649,13 +4681,13 @@
         <v>86</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="F84" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="G84" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H84" s="4" t="s">
         <v>149</v>
@@ -4684,13 +4716,13 @@
         <v>87</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F85" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G85" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H85" s="4" t="s">
         <v>149</v>
@@ -4719,7 +4751,7 @@
         <v>88</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="F86" s="4" t="s">
         <v>89</v>
@@ -4754,7 +4786,7 @@
         <v>90</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="F87" s="4" t="s">
         <v>91</v>
@@ -4789,10 +4821,10 @@
         <v>92</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="F88" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G88" s="4" t="s">
         <v>14</v>
@@ -4822,7 +4854,7 @@
         <v>150</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="F89" s="4" t="s">
         <v>151</v>
@@ -4853,7 +4885,7 @@
         <v>152</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="F90" s="4" t="s">
         <v>153</v>
@@ -4884,7 +4916,7 @@
         <v>154</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="F91" s="4" t="s">
         <v>155</v>
@@ -4915,7 +4947,7 @@
         <v>156</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="F92" s="4" t="s">
         <v>157</v>
@@ -4946,10 +4978,10 @@
         <v>158</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="F93" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G93" s="4"/>
       <c r="H93" s="4" t="s">
@@ -4979,10 +5011,10 @@
         <v>159</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="F94" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G94" s="4"/>
       <c r="H94" s="4" t="s">
@@ -5012,13 +5044,13 @@
         <v>95</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="F95" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G95" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H95" s="4" t="s">
         <v>149</v>
@@ -5047,13 +5079,13 @@
         <v>125</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="F96" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="G96" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H96" s="4" t="s">
         <v>149</v>
@@ -5082,10 +5114,10 @@
         <v>126</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="F97" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G97" s="4"/>
       <c r="H97" s="4" t="s">
@@ -5113,7 +5145,7 @@
         <v>127</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="F98" s="4" t="s">
         <v>171</v>
@@ -5146,13 +5178,13 @@
         <v>129</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="F99" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="G99" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H99" s="4" t="s">
         <v>149</v>
@@ -5181,13 +5213,13 @@
         <v>130</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="F100" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="G100" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="H100" s="4" t="s">
         <v>149</v>
@@ -5216,13 +5248,13 @@
         <v>131</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="F101" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G101" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="H101" s="4" t="s">
         <v>149</v>
@@ -5251,10 +5283,10 @@
         <v>132</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="F102" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G102" s="4"/>
       <c r="H102" s="4" t="s">
@@ -5284,10 +5316,10 @@
         <v>133</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="F103" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G103" s="4"/>
       <c r="H103" s="4" t="s">
@@ -5317,10 +5349,10 @@
         <v>134</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="F104" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G104" s="4"/>
       <c r="H104" s="4" t="s">
@@ -5348,13 +5380,13 @@
         <v>124</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G105" s="5" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="H105" s="4" t="s">
         <v>149</v>
@@ -5383,13 +5415,13 @@
         <v>136</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="F106" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="G106" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H106" s="4" t="s">
         <v>149</v>
@@ -5418,13 +5450,13 @@
         <v>137</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="F107" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="G107" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H107" s="4" t="s">
         <v>149</v>
@@ -5453,13 +5485,13 @@
         <v>138</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="F108" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="G108" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="H108" s="4" t="s">
         <v>149</v>
@@ -5488,13 +5520,13 @@
         <v>139</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="F109" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G109" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="H109" s="4" t="s">
         <v>149</v>
@@ -5523,13 +5555,13 @@
         <v>140</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="F110" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G110" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="H110" s="4" t="s">
         <v>149</v>
@@ -5558,10 +5590,10 @@
         <v>141</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="F111" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="G111" s="4"/>
       <c r="H111" s="4" t="s">
@@ -5591,10 +5623,10 @@
         <v>143</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="F112" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="G112" s="4" t="s">
         <v>14</v>
@@ -5626,10 +5658,10 @@
         <v>144</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="F113" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G113" s="4" t="s">
         <v>14</v>
@@ -5661,10 +5693,10 @@
         <v>145</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="F114" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G114" s="4" t="s">
         <v>14</v>

</xml_diff>